<commit_message>
update individuals so that questions appear in add step/add 'title' to propertyList for gwas_stats question
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/www/genomics/project_home/NiagadsSite/Model/lib/wdk/ontology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/www/genomics/project_home/GenomicsDBWebsite/Model/lib/wdk/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1DD762-7AB9-9D45-8FA9-57BC469C1E6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE0138A-19BE-6B4F-8853-DEA418F2BB65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="760" windowWidth="44840" windowHeight="23660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="476">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1484,6 +1486,15 @@
   </si>
   <si>
     <t>is_annotated</t>
+  </si>
+  <si>
+    <t>VariantQuestions.gwas_stats</t>
+  </si>
+  <si>
+    <t>VariantQuestions.vupload</t>
+  </si>
+  <si>
+    <t>VariantQuestions.vid</t>
   </si>
 </sst>
 </file>
@@ -1825,10 +1836,10 @@
   <dimension ref="A1:N173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M69" sqref="M69"/>
+      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3243,7 +3254,7 @@
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="str">
         <f>CONCATENATE(D60,".",F60)</f>
-        <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.Identifier</v>
+        <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vid</v>
       </c>
       <c r="B60" t="s">
         <v>31</v>
@@ -3258,7 +3269,7 @@
         <v>21</v>
       </c>
       <c r="F60" t="s">
-        <v>424</v>
+        <v>475</v>
       </c>
       <c r="L60" t="s">
         <v>22</v>
@@ -3270,7 +3281,7 @@
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="str">
         <f>CONCATENATE(D61,".",F61)</f>
-        <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.Upload</v>
+        <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vupload</v>
       </c>
       <c r="B61" t="s">
         <v>31</v>
@@ -3285,7 +3296,7 @@
         <v>21</v>
       </c>
       <c r="F61" t="s">
-        <v>425</v>
+        <v>474</v>
       </c>
       <c r="L61" t="s">
         <v>22</v>
@@ -3297,13 +3308,13 @@
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="str">
         <f>CONCATENATE(D62,".",F62)</f>
-        <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.GWAS</v>
+        <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.gwas_stats</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>301</v>
       </c>
       <c r="C62" t="s">
-        <v>32</v>
+        <v>299</v>
       </c>
       <c r="D62" t="s">
         <v>230</v>
@@ -3312,7 +3323,7 @@
         <v>21</v>
       </c>
       <c r="F62" t="s">
-        <v>426</v>
+        <v>473</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -3382,7 +3393,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="str">
-        <f t="shared" ref="A68:A69" si="3">CONCATENATE(D68,".",F68)</f>
+        <f t="shared" ref="A68" si="3">CONCATENATE(D68,".",F68)</f>
         <v>VariantRecordClasses.VariantRecordClass.metaseq_id</v>
       </c>
       <c r="B68" t="s">

</xml_diff>

<commit_message>
update to gene record to move link outs into own section/breaks gene header
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/www/genomics/project_home/GenomicsDBWebsite/Model/lib/wdk/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE0138A-19BE-6B4F-8853-DEA418F2BB65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EE1E87-C598-874E-81B8-C68954990AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="760" windowWidth="44840" windowHeight="23660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">entity_data_mapping!$A$1:$A$104</definedName>
-    <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$136</definedName>
+    <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$140</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="480">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1495,6 +1495,18 @@
   </si>
   <si>
     <t>VariantQuestions.vid</t>
+  </si>
+  <si>
+    <t>sequence_link_outs</t>
+  </si>
+  <si>
+    <t>protein_link_outs</t>
+  </si>
+  <si>
+    <t>clinical_link_outs</t>
+  </si>
+  <si>
+    <t>Data identity and mapping</t>
   </si>
 </sst>
 </file>
@@ -1833,13 +1845,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N173"/>
+  <dimension ref="A1:N177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
+      <selection pane="bottomRight" activeCell="L66" sqref="L66:M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2114,7 +2126,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
-        <f t="shared" ref="A19:A56" si="0">CONCATENATE(D19,".",F19)</f>
+        <f t="shared" ref="A19:A54" si="0">CONCATENATE(D19,".",F19)</f>
         <v>GeneRecordClasses.GeneRecordClass.chromosome</v>
       </c>
       <c r="B19" t="s">
@@ -2784,13 +2796,13 @@
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.third_party_data_links</v>
+        <v>GeneRecordClasses.GeneRecordClass.cytogenetic_location</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D40" t="s">
         <v>64</v>
@@ -2799,46 +2811,25 @@
         <v>24</v>
       </c>
       <c r="F40" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="J40" t="s">
         <v>66</v>
       </c>
+      <c r="L40" t="s">
+        <v>27</v>
+      </c>
       <c r="M40" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.record_link_outs</v>
-      </c>
-      <c r="B41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" t="s">
-        <v>64</v>
-      </c>
-      <c r="E41" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" t="s">
-        <v>260</v>
-      </c>
-      <c r="J41" t="s">
-        <v>66</v>
-      </c>
-      <c r="M41" t="s">
-        <v>70</v>
+      <c r="N40" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.cytogenetic_location</v>
+        <v>GeneRecordClasses.GeneRecordClass.full_jbrowse_link</v>
       </c>
       <c r="B42" t="s">
         <v>34</v>
@@ -2853,31 +2844,52 @@
         <v>24</v>
       </c>
       <c r="F42" t="s">
-        <v>262</v>
+        <v>305</v>
       </c>
       <c r="J42" t="s">
         <v>66</v>
       </c>
-      <c r="L42" t="s">
-        <v>27</v>
-      </c>
       <c r="M42" t="s">
         <v>70</v>
       </c>
-      <c r="N42" t="s">
-        <v>26</v>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="str">
+        <f t="shared" ref="A43" si="1">CONCATENATE(D43,".",F43)</f>
+        <v>GeneRecordClasses.GeneRecordClass.jbrowse_source_url</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" t="s">
+        <v>304</v>
+      </c>
+      <c r="J43" t="s">
+        <v>66</v>
+      </c>
+      <c r="M43" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.full_jbrowse_link</v>
+        <v>GeneRecordClasses.GeneRecordClass.dynspan_link</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D44" t="s">
         <v>64</v>
@@ -2886,7 +2898,7 @@
         <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>305</v>
+        <v>261</v>
       </c>
       <c r="J44" t="s">
         <v>66</v>
@@ -2897,8 +2909,8 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="str">
-        <f t="shared" ref="A45" si="1">CONCATENATE(D45,".",F45)</f>
-        <v>GeneRecordClasses.GeneRecordClass.jbrowse_source_url</v>
+        <f t="shared" si="0"/>
+        <v>GeneRecordClasses.GeneRecordClass.span</v>
       </c>
       <c r="B45" t="s">
         <v>34</v>
@@ -2913,85 +2925,97 @@
         <v>24</v>
       </c>
       <c r="F45" t="s">
-        <v>304</v>
+        <v>218</v>
       </c>
       <c r="J45" t="s">
         <v>66</v>
       </c>
+      <c r="L45" t="s">
+        <v>27</v>
+      </c>
       <c r="M45" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.dynspan_link</v>
-      </c>
-      <c r="B46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E46" t="s">
-        <v>24</v>
-      </c>
-      <c r="F46" t="s">
-        <v>261</v>
-      </c>
-      <c r="J46" t="s">
-        <v>66</v>
-      </c>
-      <c r="M46" t="s">
-        <v>70</v>
+      <c r="N45" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.span</v>
+        <v>GeneRecordClasses.GeneRecordClass.transcripts</v>
       </c>
       <c r="B47" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D47" t="s">
         <v>64</v>
       </c>
       <c r="E47" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F47" t="s">
-        <v>218</v>
+        <v>205</v>
+      </c>
+      <c r="I47" t="s">
+        <v>208</v>
       </c>
       <c r="J47" t="s">
         <v>66</v>
       </c>
-      <c r="L47" t="s">
-        <v>27</v>
-      </c>
       <c r="M47" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="N47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneRecordClasses.GeneRecordClass.ad_skat_adsp</v>
+      </c>
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" t="s">
+        <v>209</v>
+      </c>
+      <c r="I48" t="s">
+        <v>207</v>
+      </c>
+      <c r="J48" t="s">
+        <v>66</v>
+      </c>
+      <c r="M48" t="s">
+        <v>25</v>
+      </c>
+      <c r="N48" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.transcripts</v>
+        <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_gwas</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>301</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>299</v>
       </c>
       <c r="D49" t="s">
         <v>64</v>
@@ -3000,13 +3024,13 @@
         <v>28</v>
       </c>
       <c r="F49" t="s">
-        <v>205</v>
-      </c>
-      <c r="I49" t="s">
-        <v>208</v>
+        <v>290</v>
       </c>
       <c r="J49" t="s">
         <v>66</v>
+      </c>
+      <c r="K49">
+        <v>3</v>
       </c>
       <c r="M49" t="s">
         <v>25</v>
@@ -3018,13 +3042,13 @@
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.ad_skat_adsp</v>
+        <v>GeneRecordClasses.GeneRecordClass.other_variants_from_gwas</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>301</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>299</v>
       </c>
       <c r="D50" t="s">
         <v>64</v>
@@ -3033,14 +3057,14 @@
         <v>28</v>
       </c>
       <c r="F50" t="s">
-        <v>209</v>
-      </c>
-      <c r="I50" t="s">
-        <v>207</v>
+        <v>291</v>
       </c>
       <c r="J50" t="s">
         <v>66</v>
       </c>
+      <c r="K50">
+        <v>2</v>
+      </c>
       <c r="M50" t="s">
         <v>25</v>
       </c>
@@ -3050,14 +3074,14 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_gwas</v>
+        <f>CONCATENATE(D51,".",F51)</f>
+        <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_catalog</v>
       </c>
       <c r="B51" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C51" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D51" t="s">
         <v>64</v>
@@ -3066,13 +3090,13 @@
         <v>28</v>
       </c>
       <c r="F51" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="J51" t="s">
         <v>66</v>
       </c>
       <c r="K51">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M51" t="s">
         <v>25</v>
@@ -3084,13 +3108,13 @@
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.other_variants_from_gwas</v>
+        <v>GeneRecordClasses.GeneRecordClass.other_variants_from_catalog</v>
       </c>
       <c r="B52" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C52" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D52" t="s">
         <v>64</v>
@@ -3099,13 +3123,13 @@
         <v>28</v>
       </c>
       <c r="F52" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="J52" t="s">
         <v>66</v>
       </c>
       <c r="K52">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M52" t="s">
         <v>25</v>
@@ -3116,14 +3140,14 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="str">
-        <f>CONCATENATE(D53,".",F53)</f>
-        <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_catalog</v>
+        <f t="shared" si="0"/>
+        <v>GeneRecordClasses.GeneRecordClass.go_terms</v>
       </c>
       <c r="B53" t="s">
-        <v>302</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>300</v>
+        <v>45</v>
       </c>
       <c r="D53" t="s">
         <v>64</v>
@@ -3132,13 +3156,13 @@
         <v>28</v>
       </c>
       <c r="F53" t="s">
-        <v>292</v>
+        <v>206</v>
+      </c>
+      <c r="I53" t="s">
+        <v>212</v>
       </c>
       <c r="J53" t="s">
         <v>66</v>
-      </c>
-      <c r="K53">
-        <v>1</v>
       </c>
       <c r="M53" t="s">
         <v>25</v>
@@ -3150,13 +3174,13 @@
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.other_variants_from_catalog</v>
+        <v>GeneRecordClasses.GeneRecordClass.pathways</v>
       </c>
       <c r="B54" t="s">
-        <v>302</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>300</v>
+        <v>133</v>
       </c>
       <c r="D54" t="s">
         <v>64</v>
@@ -3165,14 +3189,14 @@
         <v>28</v>
       </c>
       <c r="F54" t="s">
-        <v>293</v>
+        <v>210</v>
+      </c>
+      <c r="I54" t="s">
+        <v>211</v>
       </c>
       <c r="J54" t="s">
         <v>66</v>
       </c>
-      <c r="K54">
-        <v>4</v>
-      </c>
       <c r="M54" t="s">
         <v>25</v>
       </c>
@@ -3182,14 +3206,14 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.go_terms</v>
+        <f t="shared" ref="A55:A58" si="2">CONCATENATE(D55,".",F55)</f>
+        <v>GeneRecordClasses.GeneRecordClass.record_link_outs</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>45</v>
+        <v>479</v>
       </c>
       <c r="D55" t="s">
         <v>64</v>
@@ -3198,14 +3222,14 @@
         <v>28</v>
       </c>
       <c r="F55" t="s">
-        <v>206</v>
-      </c>
-      <c r="I55" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
       <c r="J55" t="s">
         <v>66</v>
       </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
       <c r="M55" t="s">
         <v>25</v>
       </c>
@@ -3215,14 +3239,14 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>GeneRecordClasses.GeneRecordClass.pathways</v>
+        <f t="shared" si="2"/>
+        <v>GeneRecordClasses.GeneRecordClass.sequence_link_outs</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>133</v>
+        <v>479</v>
       </c>
       <c r="D56" t="s">
         <v>64</v>
@@ -3231,14 +3255,14 @@
         <v>28</v>
       </c>
       <c r="F56" t="s">
-        <v>210</v>
-      </c>
-      <c r="I56" t="s">
-        <v>211</v>
+        <v>476</v>
       </c>
       <c r="J56" t="s">
         <v>66</v>
       </c>
+      <c r="K56">
+        <v>4</v>
+      </c>
       <c r="M56" t="s">
         <v>25</v>
       </c>
@@ -3246,209 +3270,167 @@
         <v>26</v>
       </c>
     </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>GeneRecordClasses.GeneRecordClass.protein_link_outs</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" t="s">
+        <v>479</v>
+      </c>
+      <c r="D57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" t="s">
+        <v>477</v>
+      </c>
+      <c r="J57" t="s">
+        <v>66</v>
+      </c>
+      <c r="K57">
+        <v>3</v>
+      </c>
+      <c r="M57" t="s">
+        <v>25</v>
+      </c>
+      <c r="N57" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>GeneRecordClasses.GeneRecordClass.clinical_link_outs</v>
+      </c>
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" t="s">
+        <v>479</v>
+      </c>
+      <c r="D58" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58" t="s">
+        <v>478</v>
+      </c>
+      <c r="J58" t="s">
+        <v>66</v>
+      </c>
+      <c r="K58">
+        <v>2</v>
+      </c>
+      <c r="M58" t="s">
+        <v>25</v>
+      </c>
+      <c r="N58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="str">
-        <f>CONCATENATE(D60,".",F60)</f>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="str">
+        <f>CONCATENATE(D64,".",F64)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vid</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B64" t="s">
         <v>31</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C64" t="s">
         <v>32</v>
       </c>
-      <c r="D60" t="s">
-        <v>230</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="D64" t="s">
+        <v>230</v>
+      </c>
+      <c r="E64" t="s">
         <v>21</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F64" t="s">
         <v>475</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L64" t="s">
         <v>22</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M64" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="str">
-        <f>CONCATENATE(D61,".",F61)</f>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="str">
+        <f>CONCATENATE(D65,".",F65)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vupload</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B65" t="s">
         <v>31</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C65" t="s">
         <v>32</v>
       </c>
-      <c r="D61" t="s">
-        <v>230</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="D65" t="s">
+        <v>230</v>
+      </c>
+      <c r="E65" t="s">
         <v>21</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F65" t="s">
         <v>474</v>
       </c>
-      <c r="L61" t="s">
+      <c r="L65" t="s">
         <v>22</v>
       </c>
-      <c r="M61" t="s">
+      <c r="M65" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="str">
-        <f>CONCATENATE(D62,".",F62)</f>
-        <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.gwas_stats</v>
-      </c>
-      <c r="B62" t="s">
-        <v>301</v>
-      </c>
-      <c r="C62" t="s">
-        <v>299</v>
-      </c>
-      <c r="D62" t="s">
-        <v>230</v>
-      </c>
-      <c r="E62" t="s">
-        <v>21</v>
-      </c>
-      <c r="F62" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="str">
         <f>CONCATENATE(D66,".",F66)</f>
-        <v>VariantRecordClasses.VariantRecordClass.variant_source</v>
+        <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.gwas_stats</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>301</v>
       </c>
       <c r="C66" t="s">
-        <v>32</v>
+        <v>299</v>
       </c>
       <c r="D66" t="s">
         <v>230</v>
       </c>
       <c r="E66" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F66" t="s">
-        <v>231</v>
+        <v>473</v>
       </c>
       <c r="L66" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M66" t="s">
-        <v>70</v>
-      </c>
-      <c r="N66" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="str">
-        <f t="shared" ref="A67:A123" si="2">CONCATENATE(D67,".",F67)</f>
-        <v>VariantRecordClasses.VariantRecordClass.ref_snp_id</v>
-      </c>
-      <c r="B67" t="s">
-        <v>31</v>
-      </c>
-      <c r="C67" t="s">
-        <v>32</v>
-      </c>
-      <c r="D67" t="s">
-        <v>230</v>
-      </c>
-      <c r="E67" t="s">
-        <v>24</v>
-      </c>
-      <c r="F67" t="s">
-        <v>232</v>
-      </c>
-      <c r="L67" t="s">
-        <v>27</v>
-      </c>
-      <c r="M67" t="s">
-        <v>70</v>
-      </c>
-      <c r="N67" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="str">
-        <f t="shared" ref="A68" si="3">CONCATENATE(D68,".",F68)</f>
-        <v>VariantRecordClasses.VariantRecordClass.metaseq_id</v>
-      </c>
-      <c r="B68" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68" t="s">
-        <v>32</v>
-      </c>
-      <c r="D68" t="s">
-        <v>230</v>
-      </c>
-      <c r="E68" t="s">
-        <v>24</v>
-      </c>
-      <c r="F68" t="s">
-        <v>272</v>
-      </c>
-      <c r="L68" t="s">
-        <v>27</v>
-      </c>
-      <c r="M68" t="s">
-        <v>70</v>
-      </c>
-      <c r="N68" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="str">
-        <f t="shared" ref="A69" si="4">CONCATENATE(D69,".",F69)</f>
-        <v>VariantRecordClasses.VariantRecordClass.is_annotated</v>
-      </c>
-      <c r="B69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C69" t="s">
-        <v>32</v>
-      </c>
-      <c r="D69" t="s">
-        <v>230</v>
-      </c>
-      <c r="E69" t="s">
-        <v>24</v>
-      </c>
-      <c r="F69" t="s">
-        <v>472</v>
-      </c>
-      <c r="M69" t="s">
-        <v>70</v>
+      <c r="A68" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="str">
-        <f t="shared" ref="A70" si="5">CONCATENATE(D70,".",F70)</f>
-        <v>VariantRecordClasses.VariantRecordClass.adsp_id</v>
+        <f>CONCATENATE(D70,".",F70)</f>
+        <v>VariantRecordClasses.VariantRecordClass.variant_source</v>
       </c>
       <c r="B70" t="s">
         <v>31</v>
@@ -3463,7 +3445,7 @@
         <v>24</v>
       </c>
       <c r="F70" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
       <c r="L70" t="s">
         <v>27</v>
@@ -3477,14 +3459,14 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.ref_allele</v>
+        <f t="shared" ref="A71:A127" si="3">CONCATENATE(D71,".",F71)</f>
+        <v>VariantRecordClasses.VariantRecordClass.ref_snp_id</v>
       </c>
       <c r="B71" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C71" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D71" t="s">
         <v>230</v>
@@ -3493,7 +3475,7 @@
         <v>24</v>
       </c>
       <c r="F71" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L71" t="s">
         <v>27</v>
@@ -3507,14 +3489,14 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.alt_allele</v>
+        <f t="shared" ref="A72" si="4">CONCATENATE(D72,".",F72)</f>
+        <v>VariantRecordClasses.VariantRecordClass.metaseq_id</v>
       </c>
       <c r="B72" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C72" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D72" t="s">
         <v>230</v>
@@ -3523,7 +3505,7 @@
         <v>24</v>
       </c>
       <c r="F72" t="s">
-        <v>234</v>
+        <v>272</v>
       </c>
       <c r="L72" t="s">
         <v>27</v>
@@ -3537,14 +3519,14 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.chromosome</v>
+        <f t="shared" ref="A73" si="5">CONCATENATE(D73,".",F73)</f>
+        <v>VariantRecordClasses.VariantRecordClass.is_annotated</v>
       </c>
       <c r="B73" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C73" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D73" t="s">
         <v>230</v>
@@ -3553,28 +3535,22 @@
         <v>24</v>
       </c>
       <c r="F73" t="s">
-        <v>79</v>
-      </c>
-      <c r="L73" t="s">
-        <v>27</v>
+        <v>472</v>
       </c>
       <c r="M73" t="s">
         <v>70</v>
       </c>
-      <c r="N73" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.position</v>
+        <f t="shared" ref="A74" si="6">CONCATENATE(D74,".",F74)</f>
+        <v>VariantRecordClasses.VariantRecordClass.adsp_id</v>
       </c>
       <c r="B74" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C74" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D74" t="s">
         <v>230</v>
@@ -3583,7 +3559,7 @@
         <v>24</v>
       </c>
       <c r="F74" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="L74" t="s">
         <v>27</v>
@@ -3597,14 +3573,14 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.location</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.ref_allele</v>
       </c>
       <c r="B75" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C75" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D75" t="s">
         <v>230</v>
@@ -3613,7 +3589,7 @@
         <v>24</v>
       </c>
       <c r="F75" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L75" t="s">
         <v>27</v>
@@ -3627,14 +3603,14 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.full_jbrowse_link</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.alt_allele</v>
       </c>
       <c r="B76" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C76" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D76" t="s">
         <v>230</v>
@@ -3643,16 +3619,22 @@
         <v>24</v>
       </c>
       <c r="F76" t="s">
-        <v>305</v>
+        <v>234</v>
+      </c>
+      <c r="L76" t="s">
+        <v>27</v>
       </c>
       <c r="M76" t="s">
         <v>70</v>
       </c>
+      <c r="N76" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.jbrowse_source_url</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.chromosome</v>
       </c>
       <c r="B77" t="s">
         <v>34</v>
@@ -3667,22 +3649,28 @@
         <v>24</v>
       </c>
       <c r="F77" t="s">
-        <v>304</v>
+        <v>79</v>
+      </c>
+      <c r="L77" t="s">
+        <v>27</v>
       </c>
       <c r="M77" t="s">
         <v>70</v>
       </c>
+      <c r="N77" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="str">
-        <f>CONCATENATE(D78,".",F78)</f>
-        <v>VariantRecordClasses.VariantRecordClass.display_allele</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.position</v>
       </c>
       <c r="B78" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C78" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D78" t="s">
         <v>230</v>
@@ -3691,7 +3679,7 @@
         <v>24</v>
       </c>
       <c r="F78" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="L78" t="s">
         <v>27</v>
@@ -3705,14 +3693,14 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="str">
-        <f>CONCATENATE(D79,".",F79)</f>
-        <v>VariantRecordClasses.VariantRecordClass.sequence_allele</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.location</v>
       </c>
       <c r="B79" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C79" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D79" t="s">
         <v>230</v>
@@ -3721,7 +3709,7 @@
         <v>24</v>
       </c>
       <c r="F79" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="L79" t="s">
         <v>27</v>
@@ -3735,8 +3723,8 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.upstream_sequence</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.full_jbrowse_link</v>
       </c>
       <c r="B80" t="s">
         <v>34</v>
@@ -3751,7 +3739,7 @@
         <v>24</v>
       </c>
       <c r="F80" t="s">
-        <v>237</v>
+        <v>305</v>
       </c>
       <c r="M80" t="s">
         <v>70</v>
@@ -3759,8 +3747,8 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.downstream_sequence</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.jbrowse_source_url</v>
       </c>
       <c r="B81" t="s">
         <v>34</v>
@@ -3775,7 +3763,7 @@
         <v>24</v>
       </c>
       <c r="F81" t="s">
-        <v>238</v>
+        <v>304</v>
       </c>
       <c r="M81" t="s">
         <v>70</v>
@@ -3783,14 +3771,14 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.is_adsp_variant</v>
+        <f>CONCATENATE(D82,".",F82)</f>
+        <v>VariantRecordClasses.VariantRecordClass.display_allele</v>
       </c>
       <c r="B82" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C82" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D82" t="s">
         <v>230</v>
@@ -3799,7 +3787,7 @@
         <v>24</v>
       </c>
       <c r="F82" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="L82" t="s">
         <v>27</v>
@@ -3813,14 +3801,14 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.is_adsp_wes</v>
+        <f>CONCATENATE(D83,".",F83)</f>
+        <v>VariantRecordClasses.VariantRecordClass.sequence_allele</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C83" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D83" t="s">
         <v>230</v>
@@ -3829,7 +3817,7 @@
         <v>24</v>
       </c>
       <c r="F83" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="L83" t="s">
         <v>27</v>
@@ -3843,14 +3831,14 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.is_adsp_wgs</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.upstream_sequence</v>
       </c>
       <c r="B84" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C84" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D84" t="s">
         <v>230</v>
@@ -3859,28 +3847,22 @@
         <v>24</v>
       </c>
       <c r="F84" t="s">
-        <v>241</v>
-      </c>
-      <c r="L84" t="s">
-        <v>27</v>
+        <v>237</v>
       </c>
       <c r="M84" t="s">
         <v>70</v>
       </c>
-      <c r="N84" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.is_multi_allelic</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.downstream_sequence</v>
       </c>
       <c r="B85" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C85" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D85" t="s">
         <v>230</v>
@@ -3889,28 +3871,22 @@
         <v>24</v>
       </c>
       <c r="F85" t="s">
-        <v>264</v>
-      </c>
-      <c r="L85" t="s">
-        <v>27</v>
+        <v>238</v>
       </c>
       <c r="M85" t="s">
         <v>70</v>
       </c>
-      <c r="N85" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.is_reversed</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.is_adsp_variant</v>
       </c>
       <c r="B86" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D86" t="s">
         <v>230</v>
@@ -3919,7 +3895,10 @@
         <v>24</v>
       </c>
       <c r="F86" t="s">
-        <v>216</v>
+        <v>239</v>
+      </c>
+      <c r="L86" t="s">
+        <v>27</v>
       </c>
       <c r="M86" t="s">
         <v>70</v>
@@ -3930,14 +3909,14 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.variant_class</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.is_adsp_wes</v>
       </c>
       <c r="B87" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C87" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D87" t="s">
         <v>230</v>
@@ -3946,10 +3925,10 @@
         <v>24</v>
       </c>
       <c r="F87" t="s">
-        <v>242</v>
-      </c>
-      <c r="H87" t="s">
-        <v>0</v>
+        <v>240</v>
+      </c>
+      <c r="L87" t="s">
+        <v>27</v>
       </c>
       <c r="M87" t="s">
         <v>70</v>
@@ -3960,14 +3939,14 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.variant_class_abbrev</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.is_adsp_wgs</v>
       </c>
       <c r="B88" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C88" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D88" t="s">
         <v>230</v>
@@ -3976,7 +3955,7 @@
         <v>24</v>
       </c>
       <c r="F88" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L88" t="s">
         <v>27</v>
@@ -3990,14 +3969,14 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.sequence</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.is_multi_allelic</v>
       </c>
       <c r="B89" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C89" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D89" t="s">
         <v>230</v>
@@ -4006,25 +3985,28 @@
         <v>24</v>
       </c>
       <c r="F89" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="L89" t="s">
         <v>27</v>
       </c>
+      <c r="M89" t="s">
+        <v>70</v>
+      </c>
       <c r="N89" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.has_merge_history</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.is_reversed</v>
       </c>
       <c r="B90" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C90" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D90" t="s">
         <v>230</v>
@@ -4033,22 +4015,25 @@
         <v>24</v>
       </c>
       <c r="F90" t="s">
-        <v>271</v>
+        <v>216</v>
       </c>
       <c r="M90" t="s">
         <v>70</v>
       </c>
+      <c r="N90" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.current_rsid</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.variant_class</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C91" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D91" t="s">
         <v>230</v>
@@ -4057,22 +4042,28 @@
         <v>24</v>
       </c>
       <c r="F91" t="s">
-        <v>245</v>
+        <v>242</v>
+      </c>
+      <c r="H91" t="s">
+        <v>0</v>
       </c>
       <c r="M91" t="s">
         <v>70</v>
       </c>
+      <c r="N91" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.current_primary_key</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.variant_class_abbrev</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C92" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D92" t="s">
         <v>230</v>
@@ -4081,22 +4072,28 @@
         <v>24</v>
       </c>
       <c r="F92" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="L92" t="s">
+        <v>27</v>
       </c>
       <c r="M92" t="s">
         <v>70</v>
       </c>
+      <c r="N92" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.sequence</v>
       </c>
       <c r="B93" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D93" t="s">
         <v>230</v>
@@ -4105,10 +4102,10 @@
         <v>24</v>
       </c>
       <c r="F93" t="s">
-        <v>267</v>
-      </c>
-      <c r="M93" t="s">
-        <v>70</v>
+        <v>244</v>
+      </c>
+      <c r="L93" t="s">
+        <v>27</v>
       </c>
       <c r="N93" t="s">
         <v>26</v>
@@ -4116,14 +4113,14 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.has_merge_history</v>
       </c>
       <c r="B94" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D94" t="s">
         <v>230</v>
@@ -4132,25 +4129,22 @@
         <v>24</v>
       </c>
       <c r="F94" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="M94" t="s">
         <v>70</v>
       </c>
-      <c r="N94" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="str">
-        <f t="shared" ref="A95:A96" si="6">CONCATENATE(D95,".",F95)</f>
-        <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status_display</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.current_rsid</v>
       </c>
       <c r="B95" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C95" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D95" t="s">
         <v>230</v>
@@ -4159,10 +4153,7 @@
         <v>24</v>
       </c>
       <c r="F95" t="s">
-        <v>269</v>
-      </c>
-      <c r="L95" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="M95" t="s">
         <v>70</v>
@@ -4170,14 +4161,14 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status_display</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.current_primary_key</v>
       </c>
       <c r="B96" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C96" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D96" t="s">
         <v>230</v>
@@ -4186,10 +4177,7 @@
         <v>24</v>
       </c>
       <c r="F96" t="s">
-        <v>270</v>
-      </c>
-      <c r="L96" t="s">
-        <v>27</v>
+        <v>246</v>
       </c>
       <c r="M96" t="s">
         <v>70</v>
@@ -4197,14 +4185,14 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.colocated_gene_link</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status</v>
       </c>
       <c r="B97" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C97" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D97" t="s">
         <v>230</v>
@@ -4213,25 +4201,25 @@
         <v>24</v>
       </c>
       <c r="F97" t="s">
-        <v>247</v>
-      </c>
-      <c r="L97" t="s">
-        <v>27</v>
+        <v>267</v>
       </c>
       <c r="M97" t="s">
         <v>70</v>
       </c>
+      <c r="N97" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.colocated_gene</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status</v>
       </c>
       <c r="B98" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C98" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D98" t="s">
         <v>230</v>
@@ -4240,7 +4228,7 @@
         <v>24</v>
       </c>
       <c r="F98" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="M98" t="s">
         <v>70</v>
@@ -4251,14 +4239,14 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.num_colocated_genes</v>
+        <f t="shared" ref="A99:A100" si="7">CONCATENATE(D99,".",F99)</f>
+        <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status_display</v>
       </c>
       <c r="B99" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C99" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D99" t="s">
         <v>230</v>
@@ -4267,7 +4255,7 @@
         <v>24</v>
       </c>
       <c r="F99" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="L99" t="s">
         <v>27</v>
@@ -4275,20 +4263,17 @@
       <c r="M99" t="s">
         <v>70</v>
       </c>
-      <c r="N99" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.colocated_transcripts</v>
+        <f t="shared" si="7"/>
+        <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status_display</v>
       </c>
       <c r="B100" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C100" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D100" t="s">
         <v>230</v>
@@ -4297,7 +4282,10 @@
         <v>24</v>
       </c>
       <c r="F100" t="s">
-        <v>250</v>
+        <v>270</v>
+      </c>
+      <c r="L100" t="s">
+        <v>27</v>
       </c>
       <c r="M100" t="s">
         <v>70</v>
@@ -4305,14 +4293,14 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.cadd_raw_score</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.colocated_gene_link</v>
       </c>
       <c r="B101" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C101" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D101" t="s">
         <v>230</v>
@@ -4321,28 +4309,25 @@
         <v>24</v>
       </c>
       <c r="F101" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="L101" t="s">
         <v>27</v>
       </c>
       <c r="M101" t="s">
-        <v>25</v>
-      </c>
-      <c r="N101" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.cadd_phred_score</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.colocated_gene</v>
       </c>
       <c r="B102" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C102" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D102" t="s">
         <v>230</v>
@@ -4351,13 +4336,10 @@
         <v>24</v>
       </c>
       <c r="F102" t="s">
-        <v>252</v>
-      </c>
-      <c r="L102" t="s">
-        <v>27</v>
+        <v>248</v>
       </c>
       <c r="M102" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="N102" t="s">
         <v>26</v>
@@ -4365,14 +4347,14 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="str">
-        <f t="shared" ref="A103" si="7">CONCATENATE(D103,".",F103)</f>
-        <v>VariantRecordClasses.VariantRecordClass.num_colocated_variants</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.num_colocated_genes</v>
       </c>
       <c r="B103" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C103" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D103" t="s">
         <v>230</v>
@@ -4381,22 +4363,28 @@
         <v>24</v>
       </c>
       <c r="F103" t="s">
-        <v>203</v>
+        <v>249</v>
+      </c>
+      <c r="L103" t="s">
+        <v>27</v>
       </c>
       <c r="M103" t="s">
         <v>70</v>
       </c>
+      <c r="N103" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="str">
-        <f t="shared" ref="A104:A115" si="8">CONCATENATE(D104,".",F104)</f>
-        <v>VariantRecordClasses.VariantRecordClass.colocated_variants</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.colocated_transcripts</v>
       </c>
       <c r="B104" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C104" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D104" t="s">
         <v>230</v>
@@ -4405,7 +4393,7 @@
         <v>24</v>
       </c>
       <c r="F104" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="M104" t="s">
         <v>70</v>
@@ -4413,14 +4401,14 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.num_alternative_variants</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.cadd_raw_score</v>
       </c>
       <c r="B105" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C105" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D105" t="s">
         <v>230</v>
@@ -4429,22 +4417,28 @@
         <v>24</v>
       </c>
       <c r="F105" t="s">
-        <v>254</v>
+        <v>251</v>
+      </c>
+      <c r="L105" t="s">
+        <v>27</v>
       </c>
       <c r="M105" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="N105" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.alternative_variants</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.cadd_phred_score</v>
       </c>
       <c r="B106" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C106" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D106" t="s">
         <v>230</v>
@@ -4453,22 +4447,28 @@
         <v>24</v>
       </c>
       <c r="F106" t="s">
-        <v>255</v>
+        <v>252</v>
+      </c>
+      <c r="L106" t="s">
+        <v>27</v>
       </c>
       <c r="M106" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="N106" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.most_severe_consequence</v>
+        <f t="shared" ref="A107" si="8">CONCATENATE(D107,".",F107)</f>
+        <v>VariantRecordClasses.VariantRecordClass.num_colocated_variants</v>
       </c>
       <c r="B107" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C107" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D107" t="s">
         <v>230</v>
@@ -4477,28 +4477,22 @@
         <v>24</v>
       </c>
       <c r="F107" t="s">
-        <v>273</v>
-      </c>
-      <c r="L107" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
       <c r="M107" t="s">
         <v>70</v>
       </c>
-      <c r="N107" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.msc_impact</v>
+        <f t="shared" ref="A108:A119" si="9">CONCATENATE(D108,".",F108)</f>
+        <v>VariantRecordClasses.VariantRecordClass.colocated_variants</v>
       </c>
       <c r="B108" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C108" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D108" t="s">
         <v>230</v>
@@ -4507,28 +4501,22 @@
         <v>24</v>
       </c>
       <c r="F108" t="s">
-        <v>274</v>
-      </c>
-      <c r="L108" t="s">
-        <v>27</v>
+        <v>253</v>
       </c>
       <c r="M108" t="s">
         <v>70</v>
       </c>
-      <c r="N108" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene_link</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.num_alternative_variants</v>
       </c>
       <c r="B109" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C109" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D109" t="s">
         <v>230</v>
@@ -4537,10 +4525,7 @@
         <v>24</v>
       </c>
       <c r="F109" t="s">
-        <v>275</v>
-      </c>
-      <c r="L109" t="s">
-        <v>27</v>
+        <v>254</v>
       </c>
       <c r="M109" t="s">
         <v>70</v>
@@ -4548,14 +4533,14 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.alternative_variants</v>
       </c>
       <c r="B110" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C110" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D110" t="s">
         <v>230</v>
@@ -4564,19 +4549,16 @@
         <v>24</v>
       </c>
       <c r="F110" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="M110" t="s">
         <v>70</v>
       </c>
-      <c r="N110" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.msc_impacted_symbol</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.most_severe_consequence</v>
       </c>
       <c r="B111" t="s">
         <v>44</v>
@@ -4591,7 +4573,10 @@
         <v>24</v>
       </c>
       <c r="F111" t="s">
-        <v>277</v>
+        <v>273</v>
+      </c>
+      <c r="L111" t="s">
+        <v>27</v>
       </c>
       <c r="M111" t="s">
         <v>70</v>
@@ -4602,8 +4587,8 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.msc_impacted_transcript</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.msc_impact</v>
       </c>
       <c r="B112" t="s">
         <v>44</v>
@@ -4618,7 +4603,7 @@
         <v>24</v>
       </c>
       <c r="F112" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="L112" t="s">
         <v>27</v>
@@ -4632,8 +4617,8 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.msc_amino_acid_change</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene_link</v>
       </c>
       <c r="B113" t="s">
         <v>44</v>
@@ -4648,7 +4633,7 @@
         <v>24</v>
       </c>
       <c r="F113" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="L113" t="s">
         <v>27</v>
@@ -4656,14 +4641,11 @@
       <c r="M113" t="s">
         <v>70</v>
       </c>
-      <c r="N113" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.msc_codon_change</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene</v>
       </c>
       <c r="B114" t="s">
         <v>44</v>
@@ -4678,10 +4660,7 @@
         <v>24</v>
       </c>
       <c r="F114" t="s">
-        <v>280</v>
-      </c>
-      <c r="L114" t="s">
-        <v>27</v>
+        <v>276</v>
       </c>
       <c r="M114" t="s">
         <v>70</v>
@@ -4692,8 +4671,8 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>VariantRecordClasses.VariantRecordClass.msc_is_coding</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.msc_impacted_symbol</v>
       </c>
       <c r="B115" t="s">
         <v>44</v>
@@ -4708,10 +4687,7 @@
         <v>24</v>
       </c>
       <c r="F115" t="s">
-        <v>281</v>
-      </c>
-      <c r="L115" t="s">
-        <v>27</v>
+        <v>277</v>
       </c>
       <c r="M115" t="s">
         <v>70</v>
@@ -4722,8 +4698,8 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="str">
-        <f t="shared" ref="A116:A117" si="9">CONCATENATE(D116,".",F116)</f>
-        <v>VariantRecordClasses.VariantRecordClass.num_impacted_transcripts</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.msc_impacted_transcript</v>
       </c>
       <c r="B116" t="s">
         <v>44</v>
@@ -4738,16 +4714,22 @@
         <v>24</v>
       </c>
       <c r="F116" t="s">
-        <v>282</v>
+        <v>278</v>
+      </c>
+      <c r="L116" t="s">
+        <v>27</v>
       </c>
       <c r="M116" t="s">
         <v>70</v>
+      </c>
+      <c r="N116" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>VariantRecordClasses.VariantRecordClass.num_impacted_genes</v>
+        <v>VariantRecordClasses.VariantRecordClass.msc_amino_acid_change</v>
       </c>
       <c r="B117" t="s">
         <v>44</v>
@@ -4762,16 +4744,22 @@
         <v>24</v>
       </c>
       <c r="F117" t="s">
-        <v>283</v>
+        <v>279</v>
+      </c>
+      <c r="L117" t="s">
+        <v>27</v>
       </c>
       <c r="M117" t="s">
         <v>70</v>
       </c>
+      <c r="N117" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="str">
-        <f t="shared" ref="A118" si="10">CONCATENATE(D118,".",F118)</f>
-        <v>VariantRecordClasses.VariantRecordClass.transcript_consequence_summary</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.msc_codon_change</v>
       </c>
       <c r="B118" t="s">
         <v>44</v>
@@ -4786,49 +4774,58 @@
         <v>24</v>
       </c>
       <c r="F118" t="s">
-        <v>284</v>
+        <v>280</v>
+      </c>
+      <c r="L118" t="s">
+        <v>27</v>
       </c>
       <c r="M118" t="s">
         <v>70</v>
       </c>
+      <c r="N118" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="str">
-        <f t="shared" ref="A119" si="11">CONCATENATE(D119,".",F119)</f>
-        <v>VariantRecordClasses.VariantRecordClass.locuszoom_gwas_datasets</v>
+        <f t="shared" si="9"/>
+        <v>VariantRecordClasses.VariantRecordClass.msc_is_coding</v>
       </c>
       <c r="B119" t="s">
-        <v>301</v>
+        <v>44</v>
       </c>
       <c r="C119" t="s">
-        <v>299</v>
+        <v>45</v>
       </c>
       <c r="D119" t="s">
         <v>230</v>
       </c>
       <c r="E119" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F119" t="s">
-        <v>288</v>
-      </c>
-      <c r="K119">
-        <v>1</v>
+        <v>281</v>
+      </c>
+      <c r="L119" t="s">
+        <v>27</v>
       </c>
       <c r="M119" t="s">
-        <v>25</v>
+        <v>70</v>
+      </c>
+      <c r="N119" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="str">
-        <f>CONCATENATE(D120,".",F120)</f>
-        <v>VariantRecordClasses.VariantRecordClass.display_metaseq_id</v>
+        <f t="shared" ref="A120:A121" si="10">CONCATENATE(D120,".",F120)</f>
+        <v>VariantRecordClasses.VariantRecordClass.num_impacted_transcripts</v>
       </c>
       <c r="B120" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C120" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D120" t="s">
         <v>230</v>
@@ -4837,52 +4834,70 @@
         <v>24</v>
       </c>
       <c r="F120" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="M120" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>VariantRecordClasses.VariantRecordClass.num_impacted_genes</v>
+      </c>
+      <c r="B121" t="s">
+        <v>44</v>
+      </c>
+      <c r="C121" t="s">
+        <v>45</v>
+      </c>
+      <c r="D121" t="s">
+        <v>230</v>
+      </c>
+      <c r="E121" t="s">
+        <v>24</v>
+      </c>
+      <c r="F121" t="s">
+        <v>283</v>
+      </c>
+      <c r="M121" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="str">
-        <f t="shared" ref="A122" si="12">CONCATENATE(D122,".",F122)</f>
-        <v>VariantRecordClasses.VariantRecordClass.allele_frequencies</v>
+        <f t="shared" ref="A122" si="11">CONCATENATE(D122,".",F122)</f>
+        <v>VariantRecordClasses.VariantRecordClass.transcript_consequence_summary</v>
       </c>
       <c r="B122" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C122" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D122" t="s">
         <v>230</v>
       </c>
       <c r="E122" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F122" t="s">
-        <v>294</v>
-      </c>
-      <c r="K122">
-        <v>1</v>
+        <v>284</v>
       </c>
       <c r="M122" t="s">
-        <v>25</v>
-      </c>
-      <c r="N122" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>VariantRecordClasses.VariantRecordClass.transcript_consequences</v>
+        <f t="shared" ref="A123" si="12">CONCATENATE(D123,".",F123)</f>
+        <v>VariantRecordClasses.VariantRecordClass.locuszoom_gwas_datasets</v>
       </c>
       <c r="B123" t="s">
-        <v>44</v>
+        <v>301</v>
       </c>
       <c r="C123" t="s">
-        <v>45</v>
+        <v>299</v>
       </c>
       <c r="D123" t="s">
         <v>230</v>
@@ -4891,7 +4906,7 @@
         <v>28</v>
       </c>
       <c r="F123" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="K123">
         <v>1</v>
@@ -4899,80 +4914,41 @@
       <c r="M123" t="s">
         <v>25</v>
       </c>
-      <c r="N123" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="str">
-        <f t="shared" ref="A124:A129" si="13">CONCATENATE(D124,".",F124)</f>
-        <v>VariantRecordClasses.VariantRecordClass.intergenic_consequences</v>
+        <f>CONCATENATE(D124,".",F124)</f>
+        <v>VariantRecordClasses.VariantRecordClass.display_metaseq_id</v>
       </c>
       <c r="B124" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C124" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D124" t="s">
         <v>230</v>
       </c>
       <c r="E124" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F124" t="s">
-        <v>286</v>
-      </c>
-      <c r="K124">
-        <v>3</v>
+        <v>289</v>
       </c>
       <c r="M124" t="s">
-        <v>25</v>
-      </c>
-      <c r="N124" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="str">
-        <f t="shared" ref="A125" si="14">CONCATENATE(D125,".",F125)</f>
-        <v>VariantRecordClasses.VariantRecordClass.regulatory_consequences</v>
-      </c>
-      <c r="B125" t="s">
-        <v>44</v>
-      </c>
-      <c r="C125" t="s">
-        <v>45</v>
-      </c>
-      <c r="D125" t="s">
-        <v>230</v>
-      </c>
-      <c r="E125" t="s">
-        <v>28</v>
-      </c>
-      <c r="F125" t="s">
-        <v>287</v>
-      </c>
-      <c r="K125">
-        <v>2</v>
-      </c>
-      <c r="M125" t="s">
-        <v>25</v>
-      </c>
-      <c r="N125" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_gwas</v>
+        <f t="shared" ref="A126" si="13">CONCATENATE(D126,".",F126)</f>
+        <v>VariantRecordClasses.VariantRecordClass.allele_frequencies</v>
       </c>
       <c r="B126" t="s">
-        <v>301</v>
+        <v>57</v>
       </c>
       <c r="C126" t="s">
-        <v>299</v>
+        <v>69</v>
       </c>
       <c r="D126" t="s">
         <v>230</v>
@@ -4981,10 +4957,10 @@
         <v>28</v>
       </c>
       <c r="F126" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M126" t="s">
         <v>25</v>
@@ -4995,14 +4971,14 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>VariantRecordClasses.VariantRecordClass.other_associations_from_gwas</v>
+        <f t="shared" si="3"/>
+        <v>VariantRecordClasses.VariantRecordClass.transcript_consequences</v>
       </c>
       <c r="B127" t="s">
-        <v>301</v>
+        <v>44</v>
       </c>
       <c r="C127" t="s">
-        <v>299</v>
+        <v>45</v>
       </c>
       <c r="D127" t="s">
         <v>230</v>
@@ -5011,10 +4987,10 @@
         <v>28</v>
       </c>
       <c r="F127" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="K127">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M127" t="s">
         <v>25</v>
@@ -5025,14 +5001,14 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_catalog</v>
+        <f t="shared" ref="A128:A133" si="14">CONCATENATE(D128,".",F128)</f>
+        <v>VariantRecordClasses.VariantRecordClass.intergenic_consequences</v>
       </c>
       <c r="B128" t="s">
-        <v>302</v>
+        <v>44</v>
       </c>
       <c r="C128" t="s">
-        <v>300</v>
+        <v>45</v>
       </c>
       <c r="D128" t="s">
         <v>230</v>
@@ -5041,10 +5017,10 @@
         <v>28</v>
       </c>
       <c r="F128" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="K128">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M128" t="s">
         <v>25</v>
@@ -5055,14 +5031,14 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>VariantRecordClasses.VariantRecordClass.other_associations_from_catalog</v>
+        <f t="shared" ref="A129" si="15">CONCATENATE(D129,".",F129)</f>
+        <v>VariantRecordClasses.VariantRecordClass.regulatory_consequences</v>
       </c>
       <c r="B129" t="s">
-        <v>302</v>
+        <v>44</v>
       </c>
       <c r="C129" t="s">
-        <v>300</v>
+        <v>45</v>
       </c>
       <c r="D129" t="s">
         <v>230</v>
@@ -5071,10 +5047,10 @@
         <v>28</v>
       </c>
       <c r="F129" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="K129">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M129" t="s">
         <v>25</v>
@@ -5085,14 +5061,14 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="str">
-        <f t="shared" ref="A130" si="15">CONCATENATE(D130,".",F130)</f>
-        <v>VariantRecordClasses.VariantRecordClass.linkage</v>
+        <f t="shared" si="14"/>
+        <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_gwas</v>
       </c>
       <c r="B130" t="s">
-        <v>57</v>
+        <v>301</v>
       </c>
       <c r="C130" t="s">
-        <v>69</v>
+        <v>299</v>
       </c>
       <c r="D130" t="s">
         <v>230</v>
@@ -5101,7 +5077,7 @@
         <v>28</v>
       </c>
       <c r="F130" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="K130">
         <v>2</v>
@@ -5113,15 +5089,100 @@
         <v>26</v>
       </c>
     </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>VariantRecordClasses.VariantRecordClass.other_associations_from_gwas</v>
+      </c>
+      <c r="B131" t="s">
+        <v>301</v>
+      </c>
+      <c r="C131" t="s">
+        <v>299</v>
+      </c>
+      <c r="D131" t="s">
+        <v>230</v>
+      </c>
+      <c r="E131" t="s">
+        <v>28</v>
+      </c>
+      <c r="F131" t="s">
+        <v>296</v>
+      </c>
+      <c r="K131">
+        <v>3</v>
+      </c>
+      <c r="M131" t="s">
+        <v>25</v>
+      </c>
+      <c r="N131" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A132" s="2" t="s">
-        <v>448</v>
+      <c r="A132" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_catalog</v>
+      </c>
+      <c r="B132" t="s">
+        <v>302</v>
+      </c>
+      <c r="C132" t="s">
+        <v>300</v>
+      </c>
+      <c r="D132" t="s">
+        <v>230</v>
+      </c>
+      <c r="E132" t="s">
+        <v>28</v>
+      </c>
+      <c r="F132" t="s">
+        <v>297</v>
+      </c>
+      <c r="K132">
+        <v>5</v>
+      </c>
+      <c r="M132" t="s">
+        <v>25</v>
+      </c>
+      <c r="N132" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>VariantRecordClasses.VariantRecordClass.other_associations_from_catalog</v>
+      </c>
+      <c r="B133" t="s">
+        <v>302</v>
+      </c>
+      <c r="C133" t="s">
+        <v>300</v>
+      </c>
+      <c r="D133" t="s">
+        <v>230</v>
+      </c>
+      <c r="E133" t="s">
+        <v>28</v>
+      </c>
+      <c r="F133" t="s">
+        <v>298</v>
+      </c>
+      <c r="K133">
+        <v>4</v>
+      </c>
+      <c r="M133" t="s">
+        <v>25</v>
+      </c>
+      <c r="N133" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="str">
-        <f>CONCATENATE(D134,".",F134)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.ResourceQuestions.GWAS</v>
+        <f t="shared" ref="A134" si="16">CONCATENATE(D134,".",F134)</f>
+        <v>VariantRecordClasses.VariantRecordClass.linkage</v>
       </c>
       <c r="B134" t="s">
         <v>57</v>
@@ -5130,163 +5191,66 @@
         <v>69</v>
       </c>
       <c r="D134" t="s">
-        <v>427</v>
+        <v>230</v>
       </c>
       <c r="E134" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F134" t="s">
-        <v>449</v>
-      </c>
-      <c r="L134" t="s">
-        <v>22</v>
+        <v>303</v>
+      </c>
+      <c r="K134">
+        <v>2</v>
       </c>
       <c r="M134" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="135" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>25</v>
+      </c>
+      <c r="N134" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="str">
-        <f t="shared" ref="A138" si="16">CONCATENATE(D138,".",F138)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.name</v>
+        <f>CONCATENATE(D138,".",F138)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.ResourceQuestions.GWAS</v>
       </c>
       <c r="B138" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C138" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D138" t="s">
         <v>427</v>
       </c>
       <c r="E138" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F138" t="s">
-        <v>3</v>
-      </c>
-      <c r="K138">
-        <v>1</v>
+        <v>449</v>
       </c>
       <c r="L138" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M138" t="s">
-        <v>25</v>
-      </c>
-      <c r="N138" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A139" s="2" t="str">
-        <f t="shared" ref="A139" si="17">CONCATENATE(D139,".",F139)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.description</v>
-      </c>
-      <c r="B139" t="s">
-        <v>31</v>
-      </c>
-      <c r="C139" t="s">
-        <v>32</v>
-      </c>
-      <c r="D139" t="s">
-        <v>427</v>
-      </c>
-      <c r="E139" t="s">
-        <v>24</v>
-      </c>
-      <c r="F139" t="s">
-        <v>6</v>
-      </c>
-      <c r="K139">
-        <v>4</v>
-      </c>
-      <c r="L139" t="s">
-        <v>27</v>
-      </c>
-      <c r="M139" t="s">
-        <v>25</v>
-      </c>
-      <c r="N139" t="s">
-        <v>26</v>
-      </c>
-    </row>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A140" s="2" t="str">
-        <f t="shared" ref="A140" si="18">CONCATENATE(D140,".",F140)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.attribution</v>
-      </c>
-      <c r="B140" t="s">
-        <v>31</v>
-      </c>
-      <c r="C140" t="s">
-        <v>32</v>
-      </c>
-      <c r="D140" t="s">
-        <v>427</v>
-      </c>
-      <c r="E140" t="s">
-        <v>24</v>
-      </c>
-      <c r="F140" t="s">
-        <v>431</v>
-      </c>
-      <c r="K140">
-        <v>3</v>
-      </c>
-      <c r="L140" t="s">
-        <v>27</v>
-      </c>
-      <c r="M140" t="s">
-        <v>25</v>
-      </c>
-      <c r="N140" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A141" s="2" t="str">
-        <f t="shared" ref="A141" si="19">CONCATENATE(D141,".",F141)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.version</v>
-      </c>
-      <c r="B141" t="s">
-        <v>31</v>
-      </c>
-      <c r="C141" t="s">
-        <v>32</v>
-      </c>
-      <c r="D141" t="s">
-        <v>427</v>
-      </c>
-      <c r="E141" t="s">
-        <v>24</v>
-      </c>
-      <c r="F141" t="s">
-        <v>432</v>
-      </c>
-      <c r="K141">
-        <v>5</v>
-      </c>
-      <c r="L141" t="s">
-        <v>27</v>
-      </c>
-      <c r="M141" t="s">
-        <v>25</v>
-      </c>
-      <c r="N141" t="s">
-        <v>26</v>
+      <c r="A140" s="2" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="str">
-        <f t="shared" ref="A142" si="20">CONCATENATE(D142,".",F142)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.category</v>
+        <f t="shared" ref="A142" si="17">CONCATENATE(D142,".",F142)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.name</v>
       </c>
       <c r="B142" t="s">
         <v>31</v>
@@ -5301,10 +5265,10 @@
         <v>24</v>
       </c>
       <c r="F142" t="s">
-        <v>433</v>
+        <v>3</v>
       </c>
       <c r="K142">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L142" t="s">
         <v>27</v>
@@ -5318,8 +5282,8 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="str">
-        <f t="shared" ref="A143:A144" si="21">CONCATENATE(D143,".",F143)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.caveats</v>
+        <f t="shared" ref="A143" si="18">CONCATENATE(D143,".",F143)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.description</v>
       </c>
       <c r="B143" t="s">
         <v>31</v>
@@ -5334,19 +5298,25 @@
         <v>24</v>
       </c>
       <c r="F143" t="s">
-        <v>434</v>
+        <v>6</v>
       </c>
       <c r="K143">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="L143" t="s">
+        <v>27</v>
       </c>
       <c r="M143" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="N143" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="str">
-        <f t="shared" si="21"/>
-        <v>DatasetRecordClasses.ResourceRecordClass.is_adsp</v>
+        <f t="shared" ref="A144" si="19">CONCATENATE(D144,".",F144)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.attribution</v>
       </c>
       <c r="B144" t="s">
         <v>31</v>
@@ -5361,7 +5331,10 @@
         <v>24</v>
       </c>
       <c r="F144" t="s">
-        <v>435</v>
+        <v>431</v>
+      </c>
+      <c r="K144">
+        <v>3</v>
       </c>
       <c r="L144" t="s">
         <v>27</v>
@@ -5375,8 +5348,8 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="str">
-        <f t="shared" ref="A145" si="22">CONCATENATE(D145,".",F145)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.accession_link</v>
+        <f t="shared" ref="A145" si="20">CONCATENATE(D145,".",F145)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.version</v>
       </c>
       <c r="B145" t="s">
         <v>31</v>
@@ -5391,7 +5364,10 @@
         <v>24</v>
       </c>
       <c r="F145" t="s">
-        <v>430</v>
+        <v>432</v>
+      </c>
+      <c r="K145">
+        <v>5</v>
       </c>
       <c r="L145" t="s">
         <v>27</v>
@@ -5405,8 +5381,8 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="str">
-        <f t="shared" ref="A146" si="23">CONCATENATE(D146,".",F146)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.datasets</v>
+        <f t="shared" ref="A146" si="21">CONCATENATE(D146,".",F146)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.category</v>
       </c>
       <c r="B146" t="s">
         <v>31</v>
@@ -5418,13 +5394,16 @@
         <v>427</v>
       </c>
       <c r="E146" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F146" t="s">
-        <v>306</v>
+        <v>433</v>
       </c>
       <c r="K146">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="L146" t="s">
+        <v>27</v>
       </c>
       <c r="M146" t="s">
         <v>25</v>
@@ -5433,15 +5412,97 @@
         <v>26</v>
       </c>
     </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="str">
+        <f t="shared" ref="A147:A148" si="22">CONCATENATE(D147,".",F147)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.caveats</v>
+      </c>
+      <c r="B147" t="s">
+        <v>31</v>
+      </c>
+      <c r="C147" t="s">
+        <v>32</v>
+      </c>
+      <c r="D147" t="s">
+        <v>427</v>
+      </c>
+      <c r="E147" t="s">
+        <v>24</v>
+      </c>
+      <c r="F147" t="s">
+        <v>434</v>
+      </c>
+      <c r="K147">
+        <v>2</v>
+      </c>
+      <c r="M147" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A148" s="2" t="s">
-        <v>450</v>
+      <c r="A148" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>DatasetRecordClasses.ResourceRecordClass.is_adsp</v>
+      </c>
+      <c r="B148" t="s">
+        <v>31</v>
+      </c>
+      <c r="C148" t="s">
+        <v>32</v>
+      </c>
+      <c r="D148" t="s">
+        <v>427</v>
+      </c>
+      <c r="E148" t="s">
+        <v>24</v>
+      </c>
+      <c r="F148" t="s">
+        <v>435</v>
+      </c>
+      <c r="L148" t="s">
+        <v>27</v>
+      </c>
+      <c r="M148" t="s">
+        <v>25</v>
+      </c>
+      <c r="N148" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="str">
+        <f t="shared" ref="A149" si="23">CONCATENATE(D149,".",F149)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.accession_link</v>
+      </c>
+      <c r="B149" t="s">
+        <v>31</v>
+      </c>
+      <c r="C149" t="s">
+        <v>32</v>
+      </c>
+      <c r="D149" t="s">
+        <v>427</v>
+      </c>
+      <c r="E149" t="s">
+        <v>24</v>
+      </c>
+      <c r="F149" t="s">
+        <v>430</v>
+      </c>
+      <c r="L149" t="s">
+        <v>27</v>
+      </c>
+      <c r="M149" t="s">
+        <v>25</v>
+      </c>
+      <c r="N149" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="str">
-        <f t="shared" ref="A150:A153" si="24">CONCATENATE(D150,".",F150)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
+        <f t="shared" ref="A150" si="24">CONCATENATE(D150,".",F150)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.datasets</v>
       </c>
       <c r="B150" t="s">
         <v>31</v>
@@ -5450,118 +5511,33 @@
         <v>32</v>
       </c>
       <c r="D150" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
       <c r="E150" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F150" t="s">
-        <v>3</v>
-      </c>
-      <c r="L150" t="s">
-        <v>27</v>
+        <v>306</v>
+      </c>
+      <c r="K150">
+        <v>2</v>
       </c>
       <c r="M150" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="N150" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A151" s="2" t="str">
-        <f t="shared" si="24"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
-      </c>
-      <c r="B151" t="s">
-        <v>31</v>
-      </c>
-      <c r="C151" t="s">
-        <v>32</v>
-      </c>
-      <c r="D151" t="s">
-        <v>451</v>
-      </c>
-      <c r="E151" t="s">
-        <v>24</v>
-      </c>
-      <c r="F151" t="s">
-        <v>6</v>
-      </c>
-      <c r="L151" t="s">
-        <v>27</v>
-      </c>
-      <c r="M151" t="s">
-        <v>70</v>
-      </c>
-      <c r="N151" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A152" s="2" t="str">
-        <f t="shared" si="24"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
-      </c>
-      <c r="B152" t="s">
-        <v>31</v>
-      </c>
-      <c r="C152" t="s">
-        <v>32</v>
-      </c>
-      <c r="D152" t="s">
-        <v>451</v>
-      </c>
-      <c r="E152" t="s">
-        <v>24</v>
-      </c>
-      <c r="F152" t="s">
-        <v>433</v>
-      </c>
-      <c r="L152" t="s">
-        <v>27</v>
-      </c>
-      <c r="M152" t="s">
-        <v>70</v>
-      </c>
-      <c r="N152" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A153" s="2" t="str">
-        <f t="shared" si="24"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
-      </c>
-      <c r="B153" t="s">
-        <v>31</v>
-      </c>
-      <c r="C153" t="s">
-        <v>32</v>
-      </c>
-      <c r="D153" t="s">
-        <v>451</v>
-      </c>
-      <c r="E153" t="s">
-        <v>24</v>
-      </c>
-      <c r="F153" t="s">
-        <v>435</v>
-      </c>
-      <c r="L153" t="s">
-        <v>27</v>
-      </c>
-      <c r="M153" t="s">
-        <v>70</v>
-      </c>
-      <c r="N153" t="s">
-        <v>26</v>
+      <c r="A152" s="2" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="str">
-        <f t="shared" ref="A154" si="25">CONCATENATE(D154,".",F154)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
+        <f t="shared" ref="A154:A157" si="25">CONCATENATE(D154,".",F154)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
       </c>
       <c r="B154" t="s">
         <v>31</v>
@@ -5576,7 +5552,7 @@
         <v>24</v>
       </c>
       <c r="F154" t="s">
-        <v>430</v>
+        <v>3</v>
       </c>
       <c r="L154" t="s">
         <v>27</v>
@@ -5590,8 +5566,8 @@
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="str">
-        <f t="shared" ref="A155:A160" si="26">CONCATENATE(D155,".",F155)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
       </c>
       <c r="B155" t="s">
         <v>31</v>
@@ -5606,7 +5582,7 @@
         <v>24</v>
       </c>
       <c r="F155" t="s">
-        <v>452</v>
+        <v>6</v>
       </c>
       <c r="L155" t="s">
         <v>27</v>
@@ -5614,125 +5590,137 @@
       <c r="M155" t="s">
         <v>70</v>
       </c>
+      <c r="N155" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
+      </c>
+      <c r="B156" t="s">
+        <v>31</v>
+      </c>
+      <c r="C156" t="s">
+        <v>32</v>
+      </c>
+      <c r="D156" t="s">
+        <v>451</v>
+      </c>
+      <c r="E156" t="s">
+        <v>24</v>
+      </c>
+      <c r="F156" t="s">
+        <v>433</v>
+      </c>
+      <c r="L156" t="s">
+        <v>27</v>
+      </c>
+      <c r="M156" t="s">
+        <v>70</v>
+      </c>
+      <c r="N156" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="str">
-        <f>CONCATENATE(D157,".",F157)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
       </c>
       <c r="B157" t="s">
-        <v>457</v>
+        <v>31</v>
       </c>
       <c r="C157" t="s">
-        <v>156</v>
+        <v>32</v>
       </c>
       <c r="D157" t="s">
         <v>451</v>
       </c>
       <c r="E157" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F157" t="s">
-        <v>453</v>
-      </c>
-      <c r="K157">
-        <v>1</v>
+        <v>435</v>
+      </c>
+      <c r="L157" t="s">
+        <v>27</v>
       </c>
       <c r="M157" t="s">
-        <v>25</v>
+        <v>70</v>
+      </c>
+      <c r="N157" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="str">
-        <f t="shared" si="26"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
+        <f t="shared" ref="A158" si="26">CONCATENATE(D158,".",F158)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
       </c>
       <c r="B158" t="s">
-        <v>457</v>
+        <v>31</v>
       </c>
       <c r="C158" t="s">
-        <v>156</v>
+        <v>32</v>
       </c>
       <c r="D158" t="s">
         <v>451</v>
       </c>
       <c r="E158" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F158" t="s">
-        <v>456</v>
-      </c>
-      <c r="K158">
-        <v>2</v>
+        <v>430</v>
+      </c>
+      <c r="L158" t="s">
+        <v>27</v>
       </c>
       <c r="M158" t="s">
-        <v>25</v>
+        <v>70</v>
+      </c>
+      <c r="N158" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="str">
-        <f>CONCATENATE(D159,".",F159)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
+        <f t="shared" ref="A159:A164" si="27">CONCATENATE(D159,".",F159)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
       </c>
       <c r="B159" t="s">
-        <v>457</v>
+        <v>31</v>
       </c>
       <c r="C159" t="s">
-        <v>156</v>
+        <v>32</v>
       </c>
       <c r="D159" t="s">
         <v>451</v>
       </c>
       <c r="E159" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F159" t="s">
-        <v>455</v>
-      </c>
-      <c r="K159">
-        <v>3</v>
+        <v>452</v>
+      </c>
+      <c r="L159" t="s">
+        <v>27</v>
       </c>
       <c r="M159" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A160" s="2" t="str">
-        <f t="shared" si="26"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
-      </c>
-      <c r="B160" t="s">
-        <v>458</v>
-      </c>
-      <c r="C160" t="s">
-        <v>459</v>
-      </c>
-      <c r="D160" t="s">
-        <v>451</v>
-      </c>
-      <c r="E160" t="s">
-        <v>28</v>
-      </c>
-      <c r="F160" t="s">
-        <v>454</v>
-      </c>
-      <c r="K160">
-        <v>1</v>
-      </c>
-      <c r="M160" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="str">
-        <f t="shared" ref="A161:A162" si="27">CONCATENATE(D161,".",F161)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
+        <f>CONCATENATE(D161,".",F161)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
       </c>
       <c r="B161" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C161" t="s">
-        <v>459</v>
+        <v>156</v>
       </c>
       <c r="D161" t="s">
         <v>451</v>
@@ -5741,10 +5729,10 @@
         <v>28</v>
       </c>
       <c r="F161" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="K161">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M161" t="s">
         <v>25</v>
@@ -5753,13 +5741,13 @@
     <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="str">
         <f t="shared" si="27"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
       </c>
       <c r="B162" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C162" t="s">
-        <v>459</v>
+        <v>156</v>
       </c>
       <c r="D162" t="s">
         <v>451</v>
@@ -5768,10 +5756,10 @@
         <v>28</v>
       </c>
       <c r="F162" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="K162">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M162" t="s">
         <v>25</v>
@@ -5779,14 +5767,14 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="str">
-        <f t="shared" ref="A163" si="28">CONCATENATE(D163,".",F163)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
+        <f>CONCATENATE(D163,".",F163)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
       </c>
       <c r="B163" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C163" t="s">
-        <v>459</v>
+        <v>156</v>
       </c>
       <c r="D163" t="s">
         <v>451</v>
@@ -5795,10 +5783,10 @@
         <v>28</v>
       </c>
       <c r="F163" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="K163">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M163" t="s">
         <v>25</v>
@@ -5806,14 +5794,14 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="str">
-        <f t="shared" ref="A164:A165" si="29">CONCATENATE(D164,".",F164)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+        <f t="shared" si="27"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
       </c>
       <c r="B164" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C164" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D164" t="s">
         <v>451</v>
@@ -5822,10 +5810,10 @@
         <v>28</v>
       </c>
       <c r="F164" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="K164">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M164" t="s">
         <v>25</v>
@@ -5833,14 +5821,14 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="str">
-        <f t="shared" si="29"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
+        <f t="shared" ref="A165:A166" si="28">CONCATENATE(D165,".",F165)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
       </c>
       <c r="B165" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C165" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D165" t="s">
         <v>451</v>
@@ -5849,10 +5837,10 @@
         <v>28</v>
       </c>
       <c r="F165" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K165">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M165" t="s">
         <v>25</v>
@@ -5860,14 +5848,14 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="str">
-        <f>CONCATENATE(D166,".",F166)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
+        <f t="shared" si="28"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
       </c>
       <c r="B166" t="s">
-        <v>57</v>
+        <v>458</v>
       </c>
       <c r="C166" t="s">
-        <v>69</v>
+        <v>459</v>
       </c>
       <c r="D166" t="s">
         <v>451</v>
@@ -5876,7 +5864,10 @@
         <v>28</v>
       </c>
       <c r="F166" t="s">
-        <v>465</v>
+        <v>463</v>
+      </c>
+      <c r="K166">
+        <v>4</v>
       </c>
       <c r="M166" t="s">
         <v>25</v>
@@ -5884,14 +5875,14 @@
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="str">
-        <f>CONCATENATE(D167,".",F167)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+        <f t="shared" ref="A167" si="29">CONCATENATE(D167,".",F167)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
       </c>
       <c r="B167" t="s">
-        <v>31</v>
+        <v>458</v>
       </c>
       <c r="C167" t="s">
-        <v>32</v>
+        <v>459</v>
       </c>
       <c r="D167" t="s">
         <v>451</v>
@@ -5900,76 +5891,97 @@
         <v>28</v>
       </c>
       <c r="F167" t="s">
-        <v>468</v>
+        <v>464</v>
+      </c>
+      <c r="K167">
+        <v>2</v>
       </c>
       <c r="M167" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="str">
+        <f t="shared" ref="A168:A169" si="30">CONCATENATE(D168,".",F168)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+      </c>
+      <c r="B168" t="s">
+        <v>460</v>
+      </c>
+      <c r="C168" t="s">
+        <v>461</v>
+      </c>
+      <c r="D168" t="s">
+        <v>451</v>
+      </c>
+      <c r="E168" t="s">
+        <v>28</v>
+      </c>
+      <c r="F168" t="s">
+        <v>466</v>
+      </c>
+      <c r="K168">
+        <v>2</v>
+      </c>
+      <c r="M168" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="str">
-        <f>CONCATENATE(D169,".",F169)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
+        <f t="shared" si="30"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
       </c>
       <c r="B169" t="s">
-        <v>31</v>
+        <v>460</v>
       </c>
       <c r="C169" t="s">
-        <v>32</v>
+        <v>461</v>
       </c>
       <c r="D169" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="E169" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F169" t="s">
-        <v>3</v>
-      </c>
-      <c r="L169" t="s">
-        <v>471</v>
+        <v>467</v>
+      </c>
+      <c r="K169">
+        <v>1</v>
       </c>
       <c r="M169" t="s">
-        <v>70</v>
-      </c>
-      <c r="N169" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="str">
-        <f t="shared" ref="A170:A173" si="30">CONCATENATE(D170,".",F170)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
+        <f>CONCATENATE(D170,".",F170)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
       </c>
       <c r="B170" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C170" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D170" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="E170" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F170" t="s">
-        <v>6</v>
-      </c>
-      <c r="L170" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="M170" t="s">
-        <v>70</v>
-      </c>
-      <c r="N170" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
+        <f>CONCATENATE(D171,".",F171)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
       </c>
       <c r="B171" t="s">
         <v>31</v>
@@ -5978,58 +5990,22 @@
         <v>32</v>
       </c>
       <c r="D171" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="E171" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F171" t="s">
-        <v>470</v>
-      </c>
-      <c r="L171" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="M171" t="s">
-        <v>70</v>
-      </c>
-      <c r="N171" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A172" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
-      </c>
-      <c r="B172" t="s">
-        <v>31</v>
-      </c>
-      <c r="C172" t="s">
-        <v>32</v>
-      </c>
-      <c r="D172" t="s">
-        <v>469</v>
-      </c>
-      <c r="E172" t="s">
-        <v>24</v>
-      </c>
-      <c r="F172" t="s">
-        <v>435</v>
-      </c>
-      <c r="L172" t="s">
-        <v>471</v>
-      </c>
-      <c r="M172" t="s">
-        <v>70</v>
-      </c>
-      <c r="N172" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+        <f>CONCATENATE(D173,".",F173)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
       </c>
       <c r="B173" t="s">
         <v>31</v>
@@ -6041,15 +6017,135 @@
         <v>469</v>
       </c>
       <c r="E173" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F173" t="s">
-        <v>306</v>
+        <v>3</v>
       </c>
       <c r="L173" t="s">
         <v>471</v>
       </c>
       <c r="M173" t="s">
+        <v>70</v>
+      </c>
+      <c r="N173" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="str">
+        <f t="shared" ref="A174:A177" si="31">CONCATENATE(D174,".",F174)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
+      </c>
+      <c r="B174" t="s">
+        <v>31</v>
+      </c>
+      <c r="C174" t="s">
+        <v>32</v>
+      </c>
+      <c r="D174" t="s">
+        <v>469</v>
+      </c>
+      <c r="E174" t="s">
+        <v>24</v>
+      </c>
+      <c r="F174" t="s">
+        <v>6</v>
+      </c>
+      <c r="L174" t="s">
+        <v>471</v>
+      </c>
+      <c r="M174" t="s">
+        <v>70</v>
+      </c>
+      <c r="N174" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
+      </c>
+      <c r="B175" t="s">
+        <v>31</v>
+      </c>
+      <c r="C175" t="s">
+        <v>32</v>
+      </c>
+      <c r="D175" t="s">
+        <v>469</v>
+      </c>
+      <c r="E175" t="s">
+        <v>24</v>
+      </c>
+      <c r="F175" t="s">
+        <v>470</v>
+      </c>
+      <c r="L175" t="s">
+        <v>471</v>
+      </c>
+      <c r="M175" t="s">
+        <v>70</v>
+      </c>
+      <c r="N175" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+      </c>
+      <c r="B176" t="s">
+        <v>31</v>
+      </c>
+      <c r="C176" t="s">
+        <v>32</v>
+      </c>
+      <c r="D176" t="s">
+        <v>469</v>
+      </c>
+      <c r="E176" t="s">
+        <v>24</v>
+      </c>
+      <c r="F176" t="s">
+        <v>435</v>
+      </c>
+      <c r="L176" t="s">
+        <v>471</v>
+      </c>
+      <c r="M176" t="s">
+        <v>70</v>
+      </c>
+      <c r="N176" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+      </c>
+      <c r="B177" t="s">
+        <v>31</v>
+      </c>
+      <c r="C177" t="s">
+        <v>32</v>
+      </c>
+      <c r="D177" t="s">
+        <v>469</v>
+      </c>
+      <c r="E177" t="s">
+        <v>28</v>
+      </c>
+      <c r="F177" t="s">
+        <v>306</v>
+      </c>
+      <c r="L177" t="s">
+        <v>471</v>
+      </c>
+      <c r="M177" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added gws_variants_summary_highchart attribute to the gene record; refers #16
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/www/genomics/project_home/GenomicsDBWebsite/Model/lib/wdk/ontology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenem\niagads_genomicsdb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED37EB86-8F91-7F43-AD46-ACA9F0FF26A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13465915-4183-4060-8E2F-80836E292D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="760" windowWidth="44840" windowHeight="23660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="6" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="481">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1507,6 +1507,9 @@
   </si>
   <si>
     <t>transcript_link_outs</t>
+  </si>
+  <si>
+    <t>gws_variants_summary_highchart</t>
   </si>
 </sst>
 </file>
@@ -1848,29 +1851,29 @@
   <dimension ref="A1:N176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A47" sqref="A47:XFD47"/>
+      <selection pane="bottomRight" activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="82.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="38.83203125" customWidth="1"/>
-    <col min="7" max="7" width="68.6640625" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
-    <col min="9" max="9" width="80.6640625" customWidth="1"/>
-    <col min="10" max="10" width="32.83203125" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" customWidth="1"/>
+    <col min="6" max="6" width="38.875" customWidth="1"/>
+    <col min="7" max="7" width="68.625" customWidth="1"/>
+    <col min="8" max="8" width="33.625" customWidth="1"/>
+    <col min="9" max="9" width="80.625" customWidth="1"/>
+    <col min="10" max="10" width="32.875" customWidth="1"/>
+    <col min="11" max="11" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -1943,12 +1946,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1962,7 +1965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1976,12 +1979,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
         <f>CONCATENATE(D11,".",F11)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.GeneTextSearch</v>
@@ -2008,7 +2011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
         <f>CONCATENATE(D12,".",F12)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.Identifier</v>
@@ -2035,7 +2038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
         <f>CONCATENATE(D13,".",F13)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.Upload</v>
@@ -2062,7 +2065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f>CONCATENATE(D14,".",F14)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneRisk</v>
@@ -2089,12 +2092,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f>CONCATENATE(D18,".",F18)</f>
         <v>GeneRecordClasses.GeneRecordClass.source_id</v>
@@ -2124,7 +2127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f t="shared" ref="A19:A53" si="0">CONCATENATE(D19,".",F19)</f>
         <v>GeneRecordClasses.GeneRecordClass.chromosome</v>
@@ -2157,7 +2160,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_name</v>
@@ -2190,7 +2193,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_type</v>
@@ -2223,7 +2226,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.strand</v>
@@ -2253,7 +2256,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.location_start</v>
@@ -2286,7 +2289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.location_end</v>
@@ -2319,7 +2322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_symbol</v>
@@ -2352,7 +2355,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.synonyms</v>
@@ -2385,7 +2388,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.jbrowse_span</v>
@@ -2412,7 +2415,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.has_ad_evidence</v>
@@ -2442,7 +2445,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_evidence_flag</v>
@@ -2472,7 +2475,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.num_colocated_variants</v>
@@ -2505,7 +2508,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.num_unique_colocated_variants</v>
@@ -2538,7 +2541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.is_reversed</v>
@@ -2562,7 +2565,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.hgnc_id</v>
@@ -2595,7 +2598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.omim_id</v>
@@ -2628,7 +2631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ucsc_id</v>
@@ -2661,7 +2664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.vega_id</v>
@@ -2694,7 +2697,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.entrez_id</v>
@@ -2727,7 +2730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ensembl_id</v>
@@ -2760,7 +2763,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.uniprot_id</v>
@@ -2793,7 +2796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.cytogenetic_location</v>
@@ -2826,7 +2829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.full_jbrowse_link</v>
@@ -2853,7 +2856,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="str">
         <f t="shared" ref="A43" si="1">CONCATENATE(D43,".",F43)</f>
         <v>GeneRecordClasses.GeneRecordClass.jbrowse_source_url</v>
@@ -2880,7 +2883,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.dynspan_link</v>
@@ -2907,7 +2910,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.span</v>
@@ -2940,7 +2943,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_skat_adsp</v>
@@ -2973,7 +2976,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_gwas</v>
@@ -3006,7 +3009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.other_variants_from_gwas</v>
@@ -3039,7 +3042,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="str">
         <f>CONCATENATE(D50,".",F50)</f>
         <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_catalog</v>
@@ -3072,7 +3075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.other_variants_from_catalog</v>
@@ -3105,7 +3108,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.go_terms</v>
@@ -3138,7 +3141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.pathways</v>
@@ -3171,9 +3174,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="str">
-        <f t="shared" ref="A54:A58" si="2">CONCATENATE(D54,".",F54)</f>
+        <f t="shared" ref="A54:A59" si="2">CONCATENATE(D54,".",F54)</f>
         <v>GeneRecordClasses.GeneRecordClass.record_link_outs</v>
       </c>
       <c r="B54" t="s">
@@ -3204,7 +3207,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.sequence_link_outs</v>
@@ -3237,7 +3240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.protein_link_outs</v>
@@ -3270,7 +3273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.clinical_link_outs</v>
@@ -3303,7 +3306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.transcript_link_outs</v>
@@ -3336,12 +3339,36 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>GeneRecordClasses.GeneRecordClass.gws_variants_summary_highchart</v>
+      </c>
+      <c r="B59" t="s">
+        <v>300</v>
+      </c>
+      <c r="C59" t="s">
+        <v>298</v>
+      </c>
+      <c r="D59" t="s">
+        <v>64</v>
+      </c>
+      <c r="E59" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" t="s">
+        <v>480</v>
+      </c>
+      <c r="M59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="str">
         <f>CONCATENATE(D63,".",F63)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vid</v>
@@ -3368,7 +3395,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="str">
         <f>CONCATENATE(D64,".",F64)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vupload</v>
@@ -3395,7 +3422,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="str">
         <f>CONCATENATE(D65,".",F65)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.gwas_stats</v>
@@ -3422,12 +3449,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="str">
         <f>CONCATENATE(D69,".",F69)</f>
         <v>VariantRecordClasses.VariantRecordClass.variant_source</v>
@@ -3457,7 +3484,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="str">
         <f t="shared" ref="A70:A126" si="3">CONCATENATE(D70,".",F70)</f>
         <v>VariantRecordClasses.VariantRecordClass.ref_snp_id</v>
@@ -3487,7 +3514,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="str">
         <f t="shared" ref="A71" si="4">CONCATENATE(D71,".",F71)</f>
         <v>VariantRecordClasses.VariantRecordClass.metaseq_id</v>
@@ -3517,7 +3544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="str">
         <f t="shared" ref="A72" si="5">CONCATENATE(D72,".",F72)</f>
         <v>VariantRecordClasses.VariantRecordClass.is_annotated</v>
@@ -3541,7 +3568,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="str">
         <f t="shared" ref="A73" si="6">CONCATENATE(D73,".",F73)</f>
         <v>VariantRecordClasses.VariantRecordClass.adsp_id</v>
@@ -3571,7 +3598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.ref_allele</v>
@@ -3601,7 +3628,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.alt_allele</v>
@@ -3631,7 +3658,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.chromosome</v>
@@ -3661,7 +3688,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.position</v>
@@ -3691,7 +3718,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.location</v>
@@ -3721,7 +3748,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.full_jbrowse_link</v>
@@ -3745,7 +3772,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.jbrowse_source_url</v>
@@ -3769,7 +3796,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="str">
         <f>CONCATENATE(D81,".",F81)</f>
         <v>VariantRecordClasses.VariantRecordClass.display_allele</v>
@@ -3799,7 +3826,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="str">
         <f>CONCATENATE(D82,".",F82)</f>
         <v>VariantRecordClasses.VariantRecordClass.sequence_allele</v>
@@ -3829,7 +3856,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.upstream_sequence</v>
@@ -3853,7 +3880,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.downstream_sequence</v>
@@ -3877,7 +3904,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_variant</v>
@@ -3907,7 +3934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_wes</v>
@@ -3937,7 +3964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_wgs</v>
@@ -3967,7 +3994,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_multi_allelic</v>
@@ -3997,7 +4024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_reversed</v>
@@ -4024,7 +4051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.variant_class</v>
@@ -4054,7 +4081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.variant_class_abbrev</v>
@@ -4084,7 +4111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.sequence</v>
@@ -4111,7 +4138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.has_merge_history</v>
@@ -4135,7 +4162,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.current_rsid</v>
@@ -4159,7 +4186,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.current_primary_key</v>
@@ -4183,7 +4210,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status</v>
@@ -4210,7 +4237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status</v>
@@ -4237,7 +4264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="str">
         <f t="shared" ref="A98:A99" si="7">CONCATENATE(D98,".",F98)</f>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status_display</v>
@@ -4264,7 +4291,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="str">
         <f t="shared" si="7"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status_display</v>
@@ -4291,7 +4318,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_gene_link</v>
@@ -4318,7 +4345,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_gene</v>
@@ -4345,7 +4372,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.num_colocated_genes</v>
@@ -4375,7 +4402,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_transcripts</v>
@@ -4399,7 +4426,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.cadd_raw_score</v>
@@ -4429,7 +4456,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.cadd_phred_score</v>
@@ -4459,7 +4486,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="str">
         <f t="shared" ref="A106" si="8">CONCATENATE(D106,".",F106)</f>
         <v>VariantRecordClasses.VariantRecordClass.num_colocated_variants</v>
@@ -4483,7 +4510,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="str">
         <f t="shared" ref="A107:A118" si="9">CONCATENATE(D107,".",F107)</f>
         <v>VariantRecordClasses.VariantRecordClass.colocated_variants</v>
@@ -4507,7 +4534,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.num_alternative_variants</v>
@@ -4531,7 +4558,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.alternative_variants</v>
@@ -4555,7 +4582,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.most_severe_consequence</v>
@@ -4585,7 +4612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impact</v>
@@ -4615,7 +4642,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene_link</v>
@@ -4642,7 +4669,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene</v>
@@ -4669,7 +4696,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_symbol</v>
@@ -4696,7 +4723,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_transcript</v>
@@ -4726,7 +4753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_amino_acid_change</v>
@@ -4756,7 +4783,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_codon_change</v>
@@ -4786,7 +4813,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_is_coding</v>
@@ -4816,7 +4843,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="str">
         <f t="shared" ref="A119:A120" si="10">CONCATENATE(D119,".",F119)</f>
         <v>VariantRecordClasses.VariantRecordClass.num_impacted_transcripts</v>
@@ -4840,7 +4867,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="str">
         <f t="shared" si="10"/>
         <v>VariantRecordClasses.VariantRecordClass.num_impacted_genes</v>
@@ -4864,7 +4891,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="str">
         <f t="shared" ref="A121" si="11">CONCATENATE(D121,".",F121)</f>
         <v>VariantRecordClasses.VariantRecordClass.transcript_consequence_summary</v>
@@ -4888,7 +4915,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="str">
         <f t="shared" ref="A122" si="12">CONCATENATE(D122,".",F122)</f>
         <v>VariantRecordClasses.VariantRecordClass.locuszoom_gwas_datasets</v>
@@ -4915,7 +4942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="str">
         <f>CONCATENATE(D123,".",F123)</f>
         <v>VariantRecordClasses.VariantRecordClass.display_metaseq_id</v>
@@ -4939,7 +4966,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="str">
         <f t="shared" ref="A125" si="13">CONCATENATE(D125,".",F125)</f>
         <v>VariantRecordClasses.VariantRecordClass.allele_frequencies</v>
@@ -4969,7 +4996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.transcript_consequences</v>
@@ -4999,7 +5026,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="str">
         <f t="shared" ref="A127:A132" si="14">CONCATENATE(D127,".",F127)</f>
         <v>VariantRecordClasses.VariantRecordClass.intergenic_consequences</v>
@@ -5029,7 +5056,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="str">
         <f t="shared" ref="A128" si="15">CONCATENATE(D128,".",F128)</f>
         <v>VariantRecordClasses.VariantRecordClass.regulatory_consequences</v>
@@ -5059,7 +5086,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_gwas</v>
@@ -5089,7 +5116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.other_associations_from_gwas</v>
@@ -5119,7 +5146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_catalog</v>
@@ -5149,7 +5176,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.other_associations_from_catalog</v>
@@ -5179,7 +5206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="str">
         <f t="shared" ref="A133" si="16">CONCATENATE(D133,".",F133)</f>
         <v>VariantRecordClasses.VariantRecordClass.linkage</v>
@@ -5209,12 +5236,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="str">
         <f>CONCATENATE(D137,".",F137)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.ResourceQuestions.GWAS</v>
@@ -5241,13 +5268,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="str">
         <f t="shared" ref="A141" si="17">CONCATENATE(D141,".",F141)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.name</v>
@@ -5280,7 +5307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="str">
         <f t="shared" ref="A142" si="18">CONCATENATE(D142,".",F142)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.description</v>
@@ -5313,7 +5340,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="str">
         <f t="shared" ref="A143" si="19">CONCATENATE(D143,".",F143)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.attribution</v>
@@ -5346,7 +5373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="str">
         <f t="shared" ref="A144" si="20">CONCATENATE(D144,".",F144)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.version</v>
@@ -5379,7 +5406,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="str">
         <f t="shared" ref="A145" si="21">CONCATENATE(D145,".",F145)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.category</v>
@@ -5412,7 +5439,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="str">
         <f t="shared" ref="A146:A147" si="22">CONCATENATE(D146,".",F146)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.caveats</v>
@@ -5439,7 +5466,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="str">
         <f t="shared" si="22"/>
         <v>DatasetRecordClasses.ResourceRecordClass.is_adsp</v>
@@ -5469,7 +5496,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="str">
         <f t="shared" ref="A148" si="23">CONCATENATE(D148,".",F148)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.accession_link</v>
@@ -5499,7 +5526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="str">
         <f t="shared" ref="A149" si="24">CONCATENATE(D149,".",F149)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.datasets</v>
@@ -5529,12 +5556,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="str">
         <f t="shared" ref="A153:A156" si="25">CONCATENATE(D153,".",F153)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
@@ -5564,7 +5591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
@@ -5594,7 +5621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
@@ -5624,7 +5651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
@@ -5654,7 +5681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="str">
         <f t="shared" ref="A157" si="26">CONCATENATE(D157,".",F157)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
@@ -5684,7 +5711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="str">
         <f t="shared" ref="A158:A163" si="27">CONCATENATE(D158,".",F158)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
@@ -5711,7 +5738,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="str">
         <f>CONCATENATE(D160,".",F160)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
@@ -5738,7 +5765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="str">
         <f t="shared" si="27"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
@@ -5765,7 +5792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="str">
         <f>CONCATENATE(D162,".",F162)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
@@ -5792,7 +5819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="str">
         <f t="shared" si="27"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
@@ -5819,7 +5846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="str">
         <f t="shared" ref="A164:A165" si="28">CONCATENATE(D164,".",F164)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
@@ -5846,7 +5873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="str">
         <f t="shared" si="28"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
@@ -5873,7 +5900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="str">
         <f t="shared" ref="A166" si="29">CONCATENATE(D166,".",F166)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
@@ -5900,7 +5927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="str">
         <f t="shared" ref="A167:A168" si="30">CONCATENATE(D167,".",F167)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
@@ -5927,7 +5954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="str">
         <f t="shared" si="30"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
@@ -5954,7 +5981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="str">
         <f>CONCATENATE(D169,".",F169)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
@@ -5978,7 +6005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="str">
         <f>CONCATENATE(D170,".",F170)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
@@ -6002,7 +6029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="str">
         <f>CONCATENATE(D172,".",F172)</f>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
@@ -6032,7 +6059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="str">
         <f t="shared" ref="A173:A176" si="31">CONCATENATE(D173,".",F173)</f>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
@@ -6062,7 +6089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="str">
         <f t="shared" si="31"/>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
@@ -6092,7 +6119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="str">
         <f t="shared" si="31"/>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
@@ -6122,7 +6149,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="str">
         <f t="shared" si="31"/>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
@@ -6163,16 +6190,16 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.625" customWidth="1"/>
+    <col min="3" max="3" width="45.625" customWidth="1"/>
+    <col min="4" max="4" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>404</v>
       </c>
@@ -6183,7 +6210,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>419</v>
       </c>
@@ -6200,7 +6227,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>420</v>
       </c>
@@ -6217,7 +6244,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -6234,7 +6261,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>224</v>
       </c>
@@ -6251,7 +6278,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>225</v>
       </c>
@@ -6265,7 +6292,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>306</v>
       </c>
@@ -6282,7 +6309,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>307</v>
       </c>
@@ -6299,7 +6326,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>308</v>
       </c>
@@ -6316,7 +6343,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>309</v>
       </c>
@@ -6330,7 +6357,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>310</v>
       </c>
@@ -6347,7 +6374,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>311</v>
       </c>
@@ -6364,7 +6391,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>312</v>
       </c>
@@ -6381,7 +6408,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>313</v>
       </c>
@@ -6398,7 +6425,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>314</v>
       </c>
@@ -6415,7 +6442,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>315</v>
       </c>
@@ -6429,7 +6456,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>316</v>
       </c>
@@ -6443,7 +6470,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>317</v>
       </c>
@@ -6457,7 +6484,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>318</v>
       </c>
@@ -6471,7 +6498,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>319</v>
       </c>
@@ -6485,7 +6512,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>320</v>
       </c>
@@ -6502,7 +6529,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>321</v>
       </c>
@@ -6519,7 +6546,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>322</v>
       </c>
@@ -6536,7 +6563,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>323</v>
       </c>
@@ -6553,7 +6580,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>324</v>
       </c>
@@ -6570,7 +6597,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>325</v>
       </c>
@@ -6587,7 +6614,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>326</v>
       </c>
@@ -6604,7 +6631,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>327</v>
       </c>
@@ -6621,7 +6648,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>328</v>
       </c>
@@ -6638,7 +6665,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>329</v>
       </c>
@@ -6655,7 +6682,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>330</v>
       </c>
@@ -6672,7 +6699,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>331</v>
       </c>
@@ -6686,7 +6713,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>332</v>
       </c>
@@ -6700,7 +6727,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>333</v>
       </c>
@@ -6714,7 +6741,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>334</v>
       </c>
@@ -6728,7 +6755,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>335</v>
       </c>
@@ -6745,7 +6772,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>336</v>
       </c>
@@ -6759,7 +6786,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>337</v>
       </c>
@@ -6776,7 +6803,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>338</v>
       </c>
@@ -6793,7 +6820,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>339</v>
       </c>
@@ -6810,7 +6837,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>340</v>
       </c>
@@ -6827,7 +6854,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>341</v>
       </c>
@@ -6844,7 +6871,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>342</v>
       </c>
@@ -6861,7 +6888,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>343</v>
       </c>
@@ -6875,7 +6902,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>344</v>
       </c>
@@ -6892,7 +6919,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>345</v>
       </c>
@@ -6906,7 +6933,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>346</v>
       </c>
@@ -6920,7 +6947,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>347</v>
       </c>
@@ -6934,7 +6961,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>348</v>
       </c>
@@ -6948,7 +6975,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>349</v>
       </c>
@@ -6962,7 +6989,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>350</v>
       </c>
@@ -6976,7 +7003,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>351</v>
       </c>
@@ -6990,7 +7017,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>352</v>
       </c>
@@ -7004,7 +7031,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>353</v>
       </c>
@@ -7018,7 +7045,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>354</v>
       </c>
@@ -7032,7 +7059,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>355</v>
       </c>
@@ -7046,7 +7073,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>356</v>
       </c>
@@ -7060,7 +7087,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>357</v>
       </c>
@@ -7074,7 +7101,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>358</v>
       </c>
@@ -7091,7 +7118,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>359</v>
       </c>
@@ -7108,7 +7135,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>360</v>
       </c>
@@ -7125,7 +7152,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>361</v>
       </c>
@@ -7139,7 +7166,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>362</v>
       </c>
@@ -7153,7 +7180,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>363</v>
       </c>
@@ -7167,7 +7194,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>364</v>
       </c>
@@ -7181,7 +7208,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>365</v>
       </c>
@@ -7195,7 +7222,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>366</v>
       </c>
@@ -7209,7 +7236,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>367</v>
       </c>
@@ -7223,7 +7250,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>368</v>
       </c>
@@ -7237,7 +7264,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>369</v>
       </c>
@@ -7254,7 +7281,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>370</v>
       </c>
@@ -7271,7 +7298,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>371</v>
       </c>
@@ -7285,7 +7312,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>372</v>
       </c>
@@ -7299,7 +7326,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>373</v>
       </c>
@@ -7313,7 +7340,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>374</v>
       </c>
@@ -7327,7 +7354,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>375</v>
       </c>
@@ -7341,7 +7368,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>376</v>
       </c>
@@ -7355,7 +7382,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>377</v>
       </c>
@@ -7369,7 +7396,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>378</v>
       </c>
@@ -7383,7 +7410,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>379</v>
       </c>
@@ -7397,7 +7424,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>380</v>
       </c>
@@ -7411,7 +7438,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>381</v>
       </c>
@@ -7428,7 +7455,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>382</v>
       </c>
@@ -7445,7 +7472,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>383</v>
       </c>
@@ -7462,7 +7489,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>384</v>
       </c>
@@ -7479,7 +7506,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>385</v>
       </c>
@@ -7496,7 +7523,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>386</v>
       </c>
@@ -7513,7 +7540,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>387</v>
       </c>
@@ -7530,7 +7557,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>388</v>
       </c>
@@ -7547,7 +7574,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>389</v>
       </c>
@@ -7564,7 +7591,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>390</v>
       </c>
@@ -7578,7 +7605,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>391</v>
       </c>
@@ -7592,7 +7619,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>392</v>
       </c>
@@ -7609,7 +7636,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>393</v>
       </c>
@@ -7626,7 +7653,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>394</v>
       </c>
@@ -7640,7 +7667,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>395</v>
       </c>
@@ -7657,7 +7684,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>396</v>
       </c>
@@ -7674,7 +7701,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>397</v>
       </c>
@@ -7691,7 +7718,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>398</v>
       </c>
@@ -7708,7 +7735,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>399</v>
       </c>
@@ -7725,7 +7752,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>400</v>
       </c>
@@ -7742,7 +7769,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>401</v>
       </c>
@@ -7759,7 +7786,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>402</v>
       </c>
@@ -7776,7 +7803,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>403</v>
       </c>
@@ -7793,7 +7820,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>438</v>
       </c>
@@ -7810,7 +7837,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>440</v>
       </c>
@@ -7827,7 +7854,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>441</v>
       </c>
@@ -7844,7 +7871,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>442</v>
       </c>
@@ -7875,15 +7902,15 @@
       <selection activeCell="B61" sqref="B61:C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -7897,7 +7924,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -7911,7 +7938,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -7925,7 +7952,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -7939,7 +7966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -7953,7 +7980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -7967,7 +7994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -7981,7 +8008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -7995,7 +8022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -8009,7 +8036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -8023,7 +8050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -8037,7 +8064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -8051,7 +8078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -8065,7 +8092,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -8079,7 +8106,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -8093,7 +8120,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -8107,7 +8134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -8121,7 +8148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -8135,7 +8162,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -8149,7 +8176,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -8163,7 +8190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -8177,7 +8204,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -8191,7 +8218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -8205,7 +8232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>139</v>
       </c>
@@ -8219,7 +8246,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -8233,7 +8260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -8247,7 +8274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -8261,7 +8288,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -8275,7 +8302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -8289,7 +8316,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>194</v>
       </c>
@@ -8303,7 +8330,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -8317,7 +8344,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -8331,7 +8358,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -8345,7 +8372,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -8359,7 +8386,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -8373,7 +8400,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -8387,7 +8414,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -8401,7 +8428,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -8415,7 +8442,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -8429,7 +8456,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -8443,7 +8470,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -8457,7 +8484,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -8471,7 +8498,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -8485,7 +8512,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -8499,7 +8526,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -8513,7 +8540,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>160</v>
       </c>
@@ -8527,7 +8554,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>162</v>
       </c>
@@ -8541,7 +8568,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -8555,7 +8582,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -8569,7 +8596,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>165</v>
       </c>
@@ -8583,7 +8610,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>167</v>
       </c>
@@ -8597,7 +8624,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -8611,7 +8638,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -8625,7 +8652,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>173</v>
       </c>
@@ -8639,7 +8666,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>175</v>
       </c>
@@ -8653,7 +8680,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>177</v>
       </c>
@@ -8667,7 +8694,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>178</v>
       </c>
@@ -8681,7 +8708,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>180</v>
       </c>
@@ -8695,7 +8722,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -8709,7 +8736,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -8723,7 +8750,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>183</v>
       </c>
@@ -8737,7 +8764,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>185</v>
       </c>
@@ -8751,7 +8778,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>188</v>
       </c>
@@ -8765,7 +8792,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -8779,7 +8806,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
update dataset search in menu/add form to GWAS dataset header
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenem\niagads_genomicsdb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/www/genomics/project_home/GenomicsDBWebsite/Model/lib/wdk/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13465915-4183-4060-8E2F-80836E292D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AF1D47-4AE5-3C41-B33B-5BF8D0A2FBD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="6" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="482">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1510,6 +1510,9 @@
   </si>
   <si>
     <t>gws_variants_summary_highchart</t>
+  </si>
+  <si>
+    <t>niagads_accession</t>
   </si>
 </sst>
 </file>
@@ -1848,32 +1851,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N176"/>
+  <dimension ref="A1:N177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M59" sqref="M59"/>
+      <selection pane="bottomRight" activeCell="N159" sqref="N159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="82.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="82.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="44.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" customWidth="1"/>
-    <col min="6" max="6" width="38.875" customWidth="1"/>
-    <col min="7" max="7" width="68.625" customWidth="1"/>
-    <col min="8" max="8" width="33.625" customWidth="1"/>
-    <col min="9" max="9" width="80.625" customWidth="1"/>
-    <col min="10" max="10" width="32.875" customWidth="1"/>
-    <col min="11" max="11" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="38.83203125" customWidth="1"/>
+    <col min="7" max="7" width="68.6640625" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="9" max="9" width="80.6640625" customWidth="1"/>
+    <col min="10" max="10" width="32.83203125" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -1946,12 +1949,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1979,12 +1982,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
         <f>CONCATENATE(D11,".",F11)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.GeneTextSearch</v>
@@ -2011,7 +2014,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
         <f>CONCATENATE(D12,".",F12)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.Identifier</v>
@@ -2038,7 +2041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str">
         <f>CONCATENATE(D13,".",F13)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.Upload</v>
@@ -2065,7 +2068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str">
         <f>CONCATENATE(D14,".",F14)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneRisk</v>
@@ -2092,12 +2095,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
         <f>CONCATENATE(D18,".",F18)</f>
         <v>GeneRecordClasses.GeneRecordClass.source_id</v>
@@ -2127,7 +2130,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
         <f t="shared" ref="A19:A53" si="0">CONCATENATE(D19,".",F19)</f>
         <v>GeneRecordClasses.GeneRecordClass.chromosome</v>
@@ -2160,7 +2163,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_name</v>
@@ -2193,7 +2196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_type</v>
@@ -2226,7 +2229,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.strand</v>
@@ -2256,7 +2259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.location_start</v>
@@ -2289,7 +2292,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.location_end</v>
@@ -2322,7 +2325,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_symbol</v>
@@ -2355,7 +2358,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.synonyms</v>
@@ -2388,7 +2391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.jbrowse_span</v>
@@ -2415,7 +2418,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.has_ad_evidence</v>
@@ -2445,7 +2448,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_evidence_flag</v>
@@ -2475,7 +2478,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.num_colocated_variants</v>
@@ -2508,7 +2511,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.num_unique_colocated_variants</v>
@@ -2541,7 +2544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.is_reversed</v>
@@ -2565,7 +2568,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.hgnc_id</v>
@@ -2598,7 +2601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.omim_id</v>
@@ -2631,7 +2634,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ucsc_id</v>
@@ -2664,7 +2667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.vega_id</v>
@@ -2697,7 +2700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.entrez_id</v>
@@ -2730,7 +2733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ensembl_id</v>
@@ -2763,7 +2766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.uniprot_id</v>
@@ -2796,7 +2799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.cytogenetic_location</v>
@@ -2829,7 +2832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.full_jbrowse_link</v>
@@ -2856,7 +2859,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="str">
         <f t="shared" ref="A43" si="1">CONCATENATE(D43,".",F43)</f>
         <v>GeneRecordClasses.GeneRecordClass.jbrowse_source_url</v>
@@ -2883,7 +2886,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.dynspan_link</v>
@@ -2910,7 +2913,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.span</v>
@@ -2943,7 +2946,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_skat_adsp</v>
@@ -2976,7 +2979,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_gwas</v>
@@ -3009,7 +3012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.other_variants_from_gwas</v>
@@ -3042,7 +3045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="str">
         <f>CONCATENATE(D50,".",F50)</f>
         <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_catalog</v>
@@ -3075,7 +3078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.other_variants_from_catalog</v>
@@ -3108,7 +3111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.go_terms</v>
@@ -3141,7 +3144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.pathways</v>
@@ -3174,7 +3177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="str">
         <f t="shared" ref="A54:A59" si="2">CONCATENATE(D54,".",F54)</f>
         <v>GeneRecordClasses.GeneRecordClass.record_link_outs</v>
@@ -3207,7 +3210,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.sequence_link_outs</v>
@@ -3240,7 +3243,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.protein_link_outs</v>
@@ -3273,7 +3276,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.clinical_link_outs</v>
@@ -3306,7 +3309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.transcript_link_outs</v>
@@ -3339,7 +3342,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.gws_variants_summary_highchart</v>
@@ -3363,12 +3366,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="str">
         <f>CONCATENATE(D63,".",F63)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vid</v>
@@ -3395,7 +3398,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="str">
         <f>CONCATENATE(D64,".",F64)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vupload</v>
@@ -3422,7 +3425,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="str">
         <f>CONCATENATE(D65,".",F65)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.gwas_stats</v>
@@ -3449,12 +3452,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="str">
         <f>CONCATENATE(D69,".",F69)</f>
         <v>VariantRecordClasses.VariantRecordClass.variant_source</v>
@@ -3484,7 +3487,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="str">
         <f t="shared" ref="A70:A126" si="3">CONCATENATE(D70,".",F70)</f>
         <v>VariantRecordClasses.VariantRecordClass.ref_snp_id</v>
@@ -3514,7 +3517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="str">
         <f t="shared" ref="A71" si="4">CONCATENATE(D71,".",F71)</f>
         <v>VariantRecordClasses.VariantRecordClass.metaseq_id</v>
@@ -3544,7 +3547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="str">
         <f t="shared" ref="A72" si="5">CONCATENATE(D72,".",F72)</f>
         <v>VariantRecordClasses.VariantRecordClass.is_annotated</v>
@@ -3568,7 +3571,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="str">
         <f t="shared" ref="A73" si="6">CONCATENATE(D73,".",F73)</f>
         <v>VariantRecordClasses.VariantRecordClass.adsp_id</v>
@@ -3598,7 +3601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.ref_allele</v>
@@ -3628,7 +3631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.alt_allele</v>
@@ -3658,7 +3661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.chromosome</v>
@@ -3688,7 +3691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.position</v>
@@ -3718,7 +3721,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.location</v>
@@ -3748,7 +3751,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.full_jbrowse_link</v>
@@ -3772,7 +3775,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.jbrowse_source_url</v>
@@ -3796,7 +3799,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="str">
         <f>CONCATENATE(D81,".",F81)</f>
         <v>VariantRecordClasses.VariantRecordClass.display_allele</v>
@@ -3826,7 +3829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="str">
         <f>CONCATENATE(D82,".",F82)</f>
         <v>VariantRecordClasses.VariantRecordClass.sequence_allele</v>
@@ -3856,7 +3859,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.upstream_sequence</v>
@@ -3880,7 +3883,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.downstream_sequence</v>
@@ -3904,7 +3907,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_variant</v>
@@ -3934,7 +3937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_wes</v>
@@ -3964,7 +3967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_wgs</v>
@@ -3994,7 +3997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_multi_allelic</v>
@@ -4024,7 +4027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_reversed</v>
@@ -4051,7 +4054,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.variant_class</v>
@@ -4081,7 +4084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.variant_class_abbrev</v>
@@ -4111,7 +4114,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.sequence</v>
@@ -4138,7 +4141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.has_merge_history</v>
@@ -4162,7 +4165,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.current_rsid</v>
@@ -4186,7 +4189,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.current_primary_key</v>
@@ -4210,7 +4213,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status</v>
@@ -4237,7 +4240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status</v>
@@ -4264,7 +4267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="str">
         <f t="shared" ref="A98:A99" si="7">CONCATENATE(D98,".",F98)</f>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status_display</v>
@@ -4291,7 +4294,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="str">
         <f t="shared" si="7"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status_display</v>
@@ -4318,7 +4321,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_gene_link</v>
@@ -4345,7 +4348,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_gene</v>
@@ -4372,7 +4375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.num_colocated_genes</v>
@@ -4402,7 +4405,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_transcripts</v>
@@ -4426,7 +4429,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.cadd_raw_score</v>
@@ -4456,7 +4459,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.cadd_phred_score</v>
@@ -4486,7 +4489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="str">
         <f t="shared" ref="A106" si="8">CONCATENATE(D106,".",F106)</f>
         <v>VariantRecordClasses.VariantRecordClass.num_colocated_variants</v>
@@ -4510,7 +4513,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="str">
         <f t="shared" ref="A107:A118" si="9">CONCATENATE(D107,".",F107)</f>
         <v>VariantRecordClasses.VariantRecordClass.colocated_variants</v>
@@ -4534,7 +4537,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.num_alternative_variants</v>
@@ -4558,7 +4561,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.alternative_variants</v>
@@ -4582,7 +4585,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.most_severe_consequence</v>
@@ -4612,7 +4615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impact</v>
@@ -4642,7 +4645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene_link</v>
@@ -4669,7 +4672,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene</v>
@@ -4696,7 +4699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_symbol</v>
@@ -4723,7 +4726,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_transcript</v>
@@ -4753,7 +4756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_amino_acid_change</v>
@@ -4783,7 +4786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_codon_change</v>
@@ -4813,7 +4816,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_is_coding</v>
@@ -4843,7 +4846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="str">
         <f t="shared" ref="A119:A120" si="10">CONCATENATE(D119,".",F119)</f>
         <v>VariantRecordClasses.VariantRecordClass.num_impacted_transcripts</v>
@@ -4867,7 +4870,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="str">
         <f t="shared" si="10"/>
         <v>VariantRecordClasses.VariantRecordClass.num_impacted_genes</v>
@@ -4891,7 +4894,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="str">
         <f t="shared" ref="A121" si="11">CONCATENATE(D121,".",F121)</f>
         <v>VariantRecordClasses.VariantRecordClass.transcript_consequence_summary</v>
@@ -4915,7 +4918,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="str">
         <f t="shared" ref="A122" si="12">CONCATENATE(D122,".",F122)</f>
         <v>VariantRecordClasses.VariantRecordClass.locuszoom_gwas_datasets</v>
@@ -4942,7 +4945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="str">
         <f>CONCATENATE(D123,".",F123)</f>
         <v>VariantRecordClasses.VariantRecordClass.display_metaseq_id</v>
@@ -4966,7 +4969,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="str">
         <f t="shared" ref="A125" si="13">CONCATENATE(D125,".",F125)</f>
         <v>VariantRecordClasses.VariantRecordClass.allele_frequencies</v>
@@ -4996,7 +4999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.transcript_consequences</v>
@@ -5026,7 +5029,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="str">
         <f t="shared" ref="A127:A132" si="14">CONCATENATE(D127,".",F127)</f>
         <v>VariantRecordClasses.VariantRecordClass.intergenic_consequences</v>
@@ -5056,7 +5059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="str">
         <f t="shared" ref="A128" si="15">CONCATENATE(D128,".",F128)</f>
         <v>VariantRecordClasses.VariantRecordClass.regulatory_consequences</v>
@@ -5086,7 +5089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_gwas</v>
@@ -5116,7 +5119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.other_associations_from_gwas</v>
@@ -5146,7 +5149,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_catalog</v>
@@ -5176,7 +5179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.other_associations_from_catalog</v>
@@ -5206,7 +5209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="str">
         <f t="shared" ref="A133" si="16">CONCATENATE(D133,".",F133)</f>
         <v>VariantRecordClasses.VariantRecordClass.linkage</v>
@@ -5236,12 +5239,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="str">
         <f>CONCATENATE(D137,".",F137)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.ResourceQuestions.GWAS</v>
@@ -5268,13 +5271,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="str">
         <f t="shared" ref="A141" si="17">CONCATENATE(D141,".",F141)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.name</v>
@@ -5307,7 +5310,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="str">
         <f t="shared" ref="A142" si="18">CONCATENATE(D142,".",F142)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.description</v>
@@ -5340,7 +5343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="str">
         <f t="shared" ref="A143" si="19">CONCATENATE(D143,".",F143)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.attribution</v>
@@ -5373,7 +5376,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="str">
         <f t="shared" ref="A144" si="20">CONCATENATE(D144,".",F144)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.version</v>
@@ -5406,7 +5409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="str">
         <f t="shared" ref="A145" si="21">CONCATENATE(D145,".",F145)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.category</v>
@@ -5439,7 +5442,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="str">
         <f t="shared" ref="A146:A147" si="22">CONCATENATE(D146,".",F146)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.caveats</v>
@@ -5466,7 +5469,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="str">
         <f t="shared" si="22"/>
         <v>DatasetRecordClasses.ResourceRecordClass.is_adsp</v>
@@ -5496,7 +5499,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="str">
         <f t="shared" ref="A148" si="23">CONCATENATE(D148,".",F148)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.accession_link</v>
@@ -5526,7 +5529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="str">
         <f t="shared" ref="A149" si="24">CONCATENATE(D149,".",F149)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.datasets</v>
@@ -5556,14 +5559,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="str">
-        <f t="shared" ref="A153:A156" si="25">CONCATENATE(D153,".",F153)</f>
+        <f t="shared" ref="A153:A157" si="25">CONCATENATE(D153,".",F153)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
       </c>
       <c r="B153" t="s">
@@ -5591,7 +5594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
@@ -5621,7 +5624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
@@ -5651,7 +5654,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
@@ -5681,9 +5684,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="str">
-        <f t="shared" ref="A157" si="26">CONCATENATE(D157,".",F157)</f>
+        <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
       </c>
       <c r="B157" t="s">
@@ -5707,14 +5710,11 @@
       <c r="M157" t="s">
         <v>70</v>
       </c>
-      <c r="N157" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="str">
-        <f t="shared" ref="A158:A163" si="27">CONCATENATE(D158,".",F158)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
+        <f t="shared" ref="A158" si="26">CONCATENATE(D158,".",F158)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.niagads_accession</v>
       </c>
       <c r="B158" t="s">
         <v>31</v>
@@ -5729,74 +5729,74 @@
         <v>24</v>
       </c>
       <c r="F158" t="s">
+        <v>481</v>
+      </c>
+      <c r="M158" t="s">
+        <v>70</v>
+      </c>
+      <c r="N158" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="str">
+        <f t="shared" ref="A159:A164" si="27">CONCATENATE(D159,".",F159)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
+      </c>
+      <c r="B159" t="s">
+        <v>31</v>
+      </c>
+      <c r="C159" t="s">
+        <v>32</v>
+      </c>
+      <c r="D159" t="s">
+        <v>450</v>
+      </c>
+      <c r="E159" t="s">
+        <v>24</v>
+      </c>
+      <c r="F159" t="s">
         <v>451</v>
       </c>
-      <c r="L158" t="s">
+      <c r="L159" t="s">
         <v>27</v>
       </c>
-      <c r="M158" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="str">
-        <f>CONCATENATE(D160,".",F160)</f>
+      <c r="M159" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="str">
+        <f>CONCATENATE(D161,".",F161)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B161" t="s">
         <v>456</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C161" t="s">
         <v>156</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D161" t="s">
         <v>450</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E161" t="s">
         <v>28</v>
       </c>
-      <c r="F160" t="s">
+      <c r="F161" t="s">
         <v>452</v>
       </c>
-      <c r="K160">
+      <c r="K161">
         <v>1</v>
       </c>
-      <c r="M160" t="s">
+      <c r="M161" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="str">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="str">
         <f t="shared" si="27"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
       </c>
-      <c r="B161" t="s">
-        <v>456</v>
-      </c>
-      <c r="C161" t="s">
-        <v>156</v>
-      </c>
-      <c r="D161" t="s">
-        <v>450</v>
-      </c>
-      <c r="E161" t="s">
-        <v>28</v>
-      </c>
-      <c r="F161" t="s">
-        <v>455</v>
-      </c>
-      <c r="K161">
-        <v>2</v>
-      </c>
-      <c r="M161" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="str">
-        <f>CONCATENATE(D162,".",F162)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
-      </c>
       <c r="B162" t="s">
         <v>456</v>
       </c>
@@ -5810,47 +5810,47 @@
         <v>28</v>
       </c>
       <c r="F162" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K162">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M162" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="str">
+        <f>CONCATENATE(D163,".",F163)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
+      </c>
+      <c r="B163" t="s">
+        <v>456</v>
+      </c>
+      <c r="C163" t="s">
+        <v>156</v>
+      </c>
+      <c r="D163" t="s">
+        <v>450</v>
+      </c>
+      <c r="E163" t="s">
+        <v>28</v>
+      </c>
+      <c r="F163" t="s">
+        <v>454</v>
+      </c>
+      <c r="K163">
+        <v>3</v>
+      </c>
+      <c r="M163" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="str">
         <f t="shared" si="27"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
       </c>
-      <c r="B163" t="s">
-        <v>457</v>
-      </c>
-      <c r="C163" t="s">
-        <v>458</v>
-      </c>
-      <c r="D163" t="s">
-        <v>450</v>
-      </c>
-      <c r="E163" t="s">
-        <v>28</v>
-      </c>
-      <c r="F163" t="s">
-        <v>453</v>
-      </c>
-      <c r="K163">
-        <v>1</v>
-      </c>
-      <c r="M163" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A164" s="2" t="str">
-        <f t="shared" ref="A164:A165" si="28">CONCATENATE(D164,".",F164)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
-      </c>
       <c r="B164" t="s">
         <v>457</v>
       </c>
@@ -5864,47 +5864,47 @@
         <v>28</v>
       </c>
       <c r="F164" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="K164">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M164" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="str">
+        <f t="shared" ref="A165:A166" si="28">CONCATENATE(D165,".",F165)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
+      </c>
+      <c r="B165" t="s">
+        <v>457</v>
+      </c>
+      <c r="C165" t="s">
+        <v>458</v>
+      </c>
+      <c r="D165" t="s">
+        <v>450</v>
+      </c>
+      <c r="E165" t="s">
+        <v>28</v>
+      </c>
+      <c r="F165" t="s">
+        <v>461</v>
+      </c>
+      <c r="K165">
+        <v>3</v>
+      </c>
+      <c r="M165" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="str">
         <f t="shared" si="28"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
       </c>
-      <c r="B165" t="s">
-        <v>457</v>
-      </c>
-      <c r="C165" t="s">
-        <v>458</v>
-      </c>
-      <c r="D165" t="s">
-        <v>450</v>
-      </c>
-      <c r="E165" t="s">
-        <v>28</v>
-      </c>
-      <c r="F165" t="s">
-        <v>462</v>
-      </c>
-      <c r="K165">
-        <v>4</v>
-      </c>
-      <c r="M165" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="str">
-        <f t="shared" ref="A166" si="29">CONCATENATE(D166,".",F166)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
-      </c>
       <c r="B166" t="s">
         <v>457</v>
       </c>
@@ -5918,25 +5918,25 @@
         <v>28</v>
       </c>
       <c r="F166" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K166">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M166" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="str">
-        <f t="shared" ref="A167:A168" si="30">CONCATENATE(D167,".",F167)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+        <f t="shared" ref="A167" si="29">CONCATENATE(D167,".",F167)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
       </c>
       <c r="B167" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C167" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D167" t="s">
         <v>450</v>
@@ -5945,7 +5945,7 @@
         <v>28</v>
       </c>
       <c r="F167" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K167">
         <v>2</v>
@@ -5954,43 +5954,43 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="str">
+        <f t="shared" ref="A168:A169" si="30">CONCATENATE(D168,".",F168)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+      </c>
+      <c r="B168" t="s">
+        <v>459</v>
+      </c>
+      <c r="C168" t="s">
+        <v>460</v>
+      </c>
+      <c r="D168" t="s">
+        <v>450</v>
+      </c>
+      <c r="E168" t="s">
+        <v>28</v>
+      </c>
+      <c r="F168" t="s">
+        <v>465</v>
+      </c>
+      <c r="K168">
+        <v>2</v>
+      </c>
+      <c r="M168" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="str">
         <f t="shared" si="30"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B169" t="s">
         <v>459</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C169" t="s">
         <v>460</v>
-      </c>
-      <c r="D168" t="s">
-        <v>450</v>
-      </c>
-      <c r="E168" t="s">
-        <v>28</v>
-      </c>
-      <c r="F168" t="s">
-        <v>466</v>
-      </c>
-      <c r="K168">
-        <v>1</v>
-      </c>
-      <c r="M168" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A169" s="2" t="str">
-        <f>CONCATENATE(D169,".",F169)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
-      </c>
-      <c r="B169" t="s">
-        <v>57</v>
-      </c>
-      <c r="C169" t="s">
-        <v>69</v>
       </c>
       <c r="D169" t="s">
         <v>450</v>
@@ -5999,22 +5999,25 @@
         <v>28</v>
       </c>
       <c r="F169" t="s">
-        <v>464</v>
+        <v>466</v>
+      </c>
+      <c r="K169">
+        <v>1</v>
       </c>
       <c r="M169" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="str">
         <f>CONCATENATE(D170,".",F170)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
       </c>
       <c r="B170" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C170" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D170" t="s">
         <v>450</v>
@@ -6023,46 +6026,40 @@
         <v>28</v>
       </c>
       <c r="F170" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="M170" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="str">
-        <f>CONCATENATE(D172,".",F172)</f>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="str">
+        <f>CONCATENATE(D171,".",F171)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+      </c>
+      <c r="B171" t="s">
+        <v>31</v>
+      </c>
+      <c r="C171" t="s">
+        <v>32</v>
+      </c>
+      <c r="D171" t="s">
+        <v>450</v>
+      </c>
+      <c r="E171" t="s">
+        <v>28</v>
+      </c>
+      <c r="F171" t="s">
+        <v>467</v>
+      </c>
+      <c r="M171" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="str">
+        <f>CONCATENATE(D173,".",F173)</f>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
-      </c>
-      <c r="B172" t="s">
-        <v>31</v>
-      </c>
-      <c r="C172" t="s">
-        <v>32</v>
-      </c>
-      <c r="D172" t="s">
-        <v>468</v>
-      </c>
-      <c r="E172" t="s">
-        <v>24</v>
-      </c>
-      <c r="F172" t="s">
-        <v>3</v>
-      </c>
-      <c r="L172" t="s">
-        <v>470</v>
-      </c>
-      <c r="M172" t="s">
-        <v>70</v>
-      </c>
-      <c r="N172" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="str">
-        <f t="shared" ref="A173:A176" si="31">CONCATENATE(D173,".",F173)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
       </c>
       <c r="B173" t="s">
         <v>31</v>
@@ -6077,7 +6074,7 @@
         <v>24</v>
       </c>
       <c r="F173" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L173" t="s">
         <v>470</v>
@@ -6089,90 +6086,120 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="str">
+        <f t="shared" ref="A174:A177" si="31">CONCATENATE(D174,".",F174)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
+      </c>
+      <c r="B174" t="s">
+        <v>31</v>
+      </c>
+      <c r="C174" t="s">
+        <v>32</v>
+      </c>
+      <c r="D174" t="s">
+        <v>468</v>
+      </c>
+      <c r="E174" t="s">
+        <v>24</v>
+      </c>
+      <c r="F174" t="s">
+        <v>6</v>
+      </c>
+      <c r="L174" t="s">
+        <v>470</v>
+      </c>
+      <c r="M174" t="s">
+        <v>70</v>
+      </c>
+      <c r="N174" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="str">
         <f t="shared" si="31"/>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B175" t="s">
         <v>31</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C175" t="s">
         <v>32</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D175" t="s">
         <v>468</v>
       </c>
-      <c r="E174" t="s">
-        <v>24</v>
-      </c>
-      <c r="F174" t="s">
+      <c r="E175" t="s">
+        <v>24</v>
+      </c>
+      <c r="F175" t="s">
         <v>469</v>
       </c>
-      <c r="L174" t="s">
+      <c r="L175" t="s">
         <v>470</v>
       </c>
-      <c r="M174" t="s">
-        <v>70</v>
-      </c>
-      <c r="N174" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="str">
+      <c r="M175" t="s">
+        <v>70</v>
+      </c>
+      <c r="N175" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="str">
         <f t="shared" si="31"/>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B176" t="s">
         <v>31</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" t="s">
         <v>32</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D176" t="s">
         <v>468</v>
       </c>
-      <c r="E175" t="s">
-        <v>24</v>
-      </c>
-      <c r="F175" t="s">
+      <c r="E176" t="s">
+        <v>24</v>
+      </c>
+      <c r="F176" t="s">
         <v>434</v>
       </c>
-      <c r="L175" t="s">
+      <c r="L176" t="s">
         <v>470</v>
       </c>
-      <c r="M175" t="s">
-        <v>70</v>
-      </c>
-      <c r="N175" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="str">
+      <c r="M176" t="s">
+        <v>70</v>
+      </c>
+      <c r="N176" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="str">
         <f t="shared" si="31"/>
         <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B177" t="s">
         <v>31</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C177" t="s">
         <v>32</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D177" t="s">
         <v>468</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E177" t="s">
         <v>28</v>
       </c>
-      <c r="F176" t="s">
+      <c r="F177" t="s">
         <v>305</v>
       </c>
-      <c r="L176" t="s">
+      <c r="L177" t="s">
         <v>470</v>
       </c>
-      <c r="M176" t="s">
+      <c r="M177" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6190,16 +6217,16 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.625" customWidth="1"/>
-    <col min="3" max="3" width="45.625" customWidth="1"/>
-    <col min="4" max="4" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.6640625" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>404</v>
       </c>
@@ -6210,7 +6237,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>419</v>
       </c>
@@ -6227,7 +6254,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>420</v>
       </c>
@@ -6244,7 +6271,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -6261,7 +6288,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>224</v>
       </c>
@@ -6278,7 +6305,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>225</v>
       </c>
@@ -6292,7 +6319,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>306</v>
       </c>
@@ -6309,7 +6336,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>307</v>
       </c>
@@ -6326,7 +6353,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>308</v>
       </c>
@@ -6343,7 +6370,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>309</v>
       </c>
@@ -6357,7 +6384,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>310</v>
       </c>
@@ -6374,7 +6401,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>311</v>
       </c>
@@ -6391,7 +6418,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>312</v>
       </c>
@@ -6408,7 +6435,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>313</v>
       </c>
@@ -6425,7 +6452,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>314</v>
       </c>
@@ -6442,7 +6469,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>315</v>
       </c>
@@ -6456,7 +6483,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>316</v>
       </c>
@@ -6470,7 +6497,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>317</v>
       </c>
@@ -6484,7 +6511,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>318</v>
       </c>
@@ -6498,7 +6525,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>319</v>
       </c>
@@ -6512,7 +6539,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>320</v>
       </c>
@@ -6529,7 +6556,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>321</v>
       </c>
@@ -6546,7 +6573,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>322</v>
       </c>
@@ -6563,7 +6590,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>323</v>
       </c>
@@ -6580,7 +6607,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>324</v>
       </c>
@@ -6597,7 +6624,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>325</v>
       </c>
@@ -6614,7 +6641,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>326</v>
       </c>
@@ -6631,7 +6658,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>327</v>
       </c>
@@ -6648,7 +6675,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>328</v>
       </c>
@@ -6665,7 +6692,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>329</v>
       </c>
@@ -6682,7 +6709,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>330</v>
       </c>
@@ -6699,7 +6726,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>331</v>
       </c>
@@ -6713,7 +6740,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>332</v>
       </c>
@@ -6727,7 +6754,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>333</v>
       </c>
@@ -6741,7 +6768,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>334</v>
       </c>
@@ -6755,7 +6782,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>335</v>
       </c>
@@ -6772,7 +6799,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>336</v>
       </c>
@@ -6786,7 +6813,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>337</v>
       </c>
@@ -6803,7 +6830,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>338</v>
       </c>
@@ -6820,7 +6847,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>339</v>
       </c>
@@ -6837,7 +6864,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>340</v>
       </c>
@@ -6854,7 +6881,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>341</v>
       </c>
@@ -6871,7 +6898,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>342</v>
       </c>
@@ -6888,7 +6915,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>343</v>
       </c>
@@ -6902,7 +6929,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>344</v>
       </c>
@@ -6919,7 +6946,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>345</v>
       </c>
@@ -6933,7 +6960,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>346</v>
       </c>
@@ -6947,7 +6974,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>347</v>
       </c>
@@ -6961,7 +6988,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>348</v>
       </c>
@@ -6975,7 +7002,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>349</v>
       </c>
@@ -6989,7 +7016,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>350</v>
       </c>
@@ -7003,7 +7030,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>351</v>
       </c>
@@ -7017,7 +7044,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>352</v>
       </c>
@@ -7031,7 +7058,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>353</v>
       </c>
@@ -7045,7 +7072,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>354</v>
       </c>
@@ -7059,7 +7086,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>355</v>
       </c>
@@ -7073,7 +7100,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>356</v>
       </c>
@@ -7087,7 +7114,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>357</v>
       </c>
@@ -7101,7 +7128,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>358</v>
       </c>
@@ -7118,7 +7145,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>359</v>
       </c>
@@ -7135,7 +7162,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>360</v>
       </c>
@@ -7152,7 +7179,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>361</v>
       </c>
@@ -7166,7 +7193,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>362</v>
       </c>
@@ -7180,7 +7207,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>363</v>
       </c>
@@ -7194,7 +7221,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>364</v>
       </c>
@@ -7208,7 +7235,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>365</v>
       </c>
@@ -7222,7 +7249,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>366</v>
       </c>
@@ -7236,7 +7263,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>367</v>
       </c>
@@ -7250,7 +7277,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>368</v>
       </c>
@@ -7264,7 +7291,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>369</v>
       </c>
@@ -7281,7 +7308,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>370</v>
       </c>
@@ -7298,7 +7325,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>371</v>
       </c>
@@ -7312,7 +7339,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>372</v>
       </c>
@@ -7326,7 +7353,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>373</v>
       </c>
@@ -7340,7 +7367,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>374</v>
       </c>
@@ -7354,7 +7381,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>375</v>
       </c>
@@ -7368,7 +7395,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>376</v>
       </c>
@@ -7382,7 +7409,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>377</v>
       </c>
@@ -7396,7 +7423,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>378</v>
       </c>
@@ -7410,7 +7437,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>379</v>
       </c>
@@ -7424,7 +7451,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>380</v>
       </c>
@@ -7438,7 +7465,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>381</v>
       </c>
@@ -7455,7 +7482,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>382</v>
       </c>
@@ -7472,7 +7499,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>383</v>
       </c>
@@ -7489,7 +7516,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>384</v>
       </c>
@@ -7506,7 +7533,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>385</v>
       </c>
@@ -7523,7 +7550,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>386</v>
       </c>
@@ -7540,7 +7567,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>387</v>
       </c>
@@ -7557,7 +7584,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>388</v>
       </c>
@@ -7574,7 +7601,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>389</v>
       </c>
@@ -7591,7 +7618,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>390</v>
       </c>
@@ -7605,7 +7632,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>391</v>
       </c>
@@ -7619,7 +7646,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>392</v>
       </c>
@@ -7636,7 +7663,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>393</v>
       </c>
@@ -7653,7 +7680,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>394</v>
       </c>
@@ -7667,7 +7694,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>395</v>
       </c>
@@ -7684,7 +7711,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>396</v>
       </c>
@@ -7701,7 +7728,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>397</v>
       </c>
@@ -7718,7 +7745,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>398</v>
       </c>
@@ -7735,7 +7762,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>399</v>
       </c>
@@ -7752,7 +7779,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>400</v>
       </c>
@@ -7769,7 +7796,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>401</v>
       </c>
@@ -7786,7 +7813,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>402</v>
       </c>
@@ -7803,7 +7830,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>403</v>
       </c>
@@ -7820,7 +7847,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>438</v>
       </c>
@@ -7837,7 +7864,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>440</v>
       </c>
@@ -7854,7 +7881,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>441</v>
       </c>
@@ -7871,7 +7898,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>442</v>
       </c>
@@ -7902,15 +7929,15 @@
       <selection activeCell="B61" sqref="B61:C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -7924,7 +7951,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -7938,7 +7965,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -7952,7 +7979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -7966,7 +7993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -7980,7 +8007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -7994,7 +8021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -8008,7 +8035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -8022,7 +8049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -8036,7 +8063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -8050,7 +8077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -8064,7 +8091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -8078,7 +8105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -8092,7 +8119,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -8106,7 +8133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -8120,7 +8147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -8134,7 +8161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -8148,7 +8175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -8162,7 +8189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -8176,7 +8203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -8190,7 +8217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -8204,7 +8231,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -8218,7 +8245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -8232,7 +8259,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>139</v>
       </c>
@@ -8246,7 +8273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -8260,7 +8287,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -8274,7 +8301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -8288,7 +8315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -8302,7 +8329,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -8316,7 +8343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>194</v>
       </c>
@@ -8330,7 +8357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -8344,7 +8371,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -8358,7 +8385,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -8372,7 +8399,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -8386,7 +8413,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -8400,7 +8427,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -8414,7 +8441,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -8428,7 +8455,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -8442,7 +8469,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -8456,7 +8483,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -8470,7 +8497,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -8484,7 +8511,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -8498,7 +8525,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -8512,7 +8539,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -8526,7 +8553,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -8540,7 +8567,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>160</v>
       </c>
@@ -8554,7 +8581,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>162</v>
       </c>
@@ -8568,7 +8595,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -8582,7 +8609,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -8596,7 +8623,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>165</v>
       </c>
@@ -8610,7 +8637,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>167</v>
       </c>
@@ -8624,7 +8651,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -8638,7 +8665,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -8652,7 +8679,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>173</v>
       </c>
@@ -8666,7 +8693,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>175</v>
       </c>
@@ -8680,7 +8707,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>177</v>
       </c>
@@ -8694,7 +8721,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>178</v>
       </c>
@@ -8708,7 +8735,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>180</v>
       </c>
@@ -8722,7 +8749,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -8736,7 +8763,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -8750,7 +8777,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>183</v>
       </c>
@@ -8764,7 +8791,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>185</v>
       </c>
@@ -8778,7 +8805,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>188</v>
       </c>
@@ -8792,7 +8819,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -8806,7 +8833,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
first pass charts for variant header; needs revision
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/www/genomics/project_home/GenomicsDBWebsite/Model/lib/wdk/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AF1D47-4AE5-3C41-B33B-5BF8D0A2FBD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A75057-A1DA-364E-A598-E07A38181701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="49000" windowHeight="20900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">entity_data_mapping!$A$1:$A$104</definedName>
-    <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$139</definedName>
+    <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$140</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="483">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1509,10 +1509,13 @@
     <t>transcript_link_outs</t>
   </si>
   <si>
-    <t>gws_variants_summary_highchart</t>
-  </si>
-  <si>
     <t>niagads_accession</t>
+  </si>
+  <si>
+    <t>gws_variants_summary_plot</t>
+  </si>
+  <si>
+    <t>gws_datasets_summary_plot</t>
   </si>
 </sst>
 </file>
@@ -1851,13 +1854,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N177"/>
+  <dimension ref="A1:N178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K147" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N159" sqref="N159"/>
+      <selection pane="bottomRight" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3003,7 +3006,7 @@
         <v>66</v>
       </c>
       <c r="K48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M48" t="s">
         <v>25</v>
@@ -3102,7 +3105,7 @@
         <v>66</v>
       </c>
       <c r="K51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M51" t="s">
         <v>25</v>
@@ -3179,7 +3182,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="str">
-        <f t="shared" ref="A54:A59" si="2">CONCATENATE(D54,".",F54)</f>
+        <f t="shared" ref="A54:A58" si="2">CONCATENATE(D54,".",F54)</f>
         <v>GeneRecordClasses.GeneRecordClass.record_link_outs</v>
       </c>
       <c r="B54" t="s">
@@ -3344,8 +3347,8 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>GeneRecordClasses.GeneRecordClass.gws_variants_summary_highchart</v>
+        <f>CONCATENATE(D59,".",F59)</f>
+        <v>GeneRecordClasses.GeneRecordClass.gws_variants_summary_plot</v>
       </c>
       <c r="B59" t="s">
         <v>300</v>
@@ -3360,7 +3363,7 @@
         <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="M59" t="s">
         <v>70</v>
@@ -3489,7 +3492,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="str">
-        <f t="shared" ref="A70:A126" si="3">CONCATENATE(D70,".",F70)</f>
+        <f t="shared" ref="A70:A127" si="3">CONCATENATE(D70,".",F70)</f>
         <v>VariantRecordClasses.VariantRecordClass.ref_snp_id</v>
       </c>
       <c r="B70" t="s">
@@ -4969,71 +4972,65 @@
         <v>70</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="str">
-        <f t="shared" ref="A125" si="13">CONCATENATE(D125,".",F125)</f>
-        <v>VariantRecordClasses.VariantRecordClass.allele_frequencies</v>
-      </c>
-      <c r="B125" t="s">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="str">
+        <f>CONCATENATE(D124,".",F124)</f>
+        <v>VariantRecordClasses.VariantRecordClass.gws_datasets_summary_plot</v>
+      </c>
+      <c r="B124" t="s">
         <v>57</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C124" t="s">
         <v>69</v>
       </c>
-      <c r="D125" t="s">
-        <v>229</v>
-      </c>
-      <c r="E125" t="s">
-        <v>28</v>
-      </c>
-      <c r="F125" t="s">
-        <v>293</v>
-      </c>
-      <c r="K125">
-        <v>1</v>
-      </c>
-      <c r="M125" t="s">
-        <v>25</v>
-      </c>
-      <c r="N125" t="s">
-        <v>26</v>
+      <c r="D124" t="s">
+        <v>229</v>
+      </c>
+      <c r="E124" t="s">
+        <v>24</v>
+      </c>
+      <c r="F124" t="s">
+        <v>482</v>
+      </c>
+      <c r="M124" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="str">
+        <f t="shared" ref="A126" si="13">CONCATENATE(D126,".",F126)</f>
+        <v>VariantRecordClasses.VariantRecordClass.allele_frequencies</v>
+      </c>
+      <c r="B126" t="s">
+        <v>57</v>
+      </c>
+      <c r="C126" t="s">
+        <v>69</v>
+      </c>
+      <c r="D126" t="s">
+        <v>229</v>
+      </c>
+      <c r="E126" t="s">
+        <v>28</v>
+      </c>
+      <c r="F126" t="s">
+        <v>293</v>
+      </c>
+      <c r="K126">
+        <v>1</v>
+      </c>
+      <c r="M126" t="s">
+        <v>25</v>
+      </c>
+      <c r="N126" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.transcript_consequences</v>
       </c>
-      <c r="B126" t="s">
-        <v>44</v>
-      </c>
-      <c r="C126" t="s">
-        <v>45</v>
-      </c>
-      <c r="D126" t="s">
-        <v>229</v>
-      </c>
-      <c r="E126" t="s">
-        <v>28</v>
-      </c>
-      <c r="F126" t="s">
-        <v>284</v>
-      </c>
-      <c r="K126">
-        <v>1</v>
-      </c>
-      <c r="M126" t="s">
-        <v>25</v>
-      </c>
-      <c r="N126" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="str">
-        <f t="shared" ref="A127:A132" si="14">CONCATENATE(D127,".",F127)</f>
-        <v>VariantRecordClasses.VariantRecordClass.intergenic_consequences</v>
-      </c>
       <c r="B127" t="s">
         <v>44</v>
       </c>
@@ -5047,10 +5044,10 @@
         <v>28</v>
       </c>
       <c r="F127" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K127">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M127" t="s">
         <v>25</v>
@@ -5061,8 +5058,8 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="str">
-        <f t="shared" ref="A128" si="15">CONCATENATE(D128,".",F128)</f>
-        <v>VariantRecordClasses.VariantRecordClass.regulatory_consequences</v>
+        <f t="shared" ref="A128:A133" si="14">CONCATENATE(D128,".",F128)</f>
+        <v>VariantRecordClasses.VariantRecordClass.intergenic_consequences</v>
       </c>
       <c r="B128" t="s">
         <v>44</v>
@@ -5077,10 +5074,10 @@
         <v>28</v>
       </c>
       <c r="F128" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K128">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M128" t="s">
         <v>25</v>
@@ -5091,14 +5088,14 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_gwas</v>
+        <f t="shared" ref="A129" si="15">CONCATENATE(D129,".",F129)</f>
+        <v>VariantRecordClasses.VariantRecordClass.regulatory_consequences</v>
       </c>
       <c r="B129" t="s">
-        <v>300</v>
+        <v>44</v>
       </c>
       <c r="C129" t="s">
-        <v>298</v>
+        <v>45</v>
       </c>
       <c r="D129" t="s">
         <v>229</v>
@@ -5107,7 +5104,7 @@
         <v>28</v>
       </c>
       <c r="F129" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="K129">
         <v>2</v>
@@ -5122,7 +5119,7 @@
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>VariantRecordClasses.VariantRecordClass.other_associations_from_gwas</v>
+        <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_gwas</v>
       </c>
       <c r="B130" t="s">
         <v>300</v>
@@ -5137,10 +5134,10 @@
         <v>28</v>
       </c>
       <c r="F130" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K130">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M130" t="s">
         <v>25</v>
@@ -5152,13 +5149,13 @@
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_catalog</v>
+        <v>VariantRecordClasses.VariantRecordClass.other_associations_from_gwas</v>
       </c>
       <c r="B131" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C131" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D131" t="s">
         <v>229</v>
@@ -5167,10 +5164,10 @@
         <v>28</v>
       </c>
       <c r="F131" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K131">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M131" t="s">
         <v>25</v>
@@ -5182,7 +5179,7 @@
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>VariantRecordClasses.VariantRecordClass.other_associations_from_catalog</v>
+        <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_catalog</v>
       </c>
       <c r="B132" t="s">
         <v>301</v>
@@ -5197,10 +5194,10 @@
         <v>28</v>
       </c>
       <c r="F132" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K132">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M132" t="s">
         <v>25</v>
@@ -5211,14 +5208,14 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="str">
-        <f t="shared" ref="A133" si="16">CONCATENATE(D133,".",F133)</f>
-        <v>VariantRecordClasses.VariantRecordClass.linkage</v>
+        <f t="shared" si="14"/>
+        <v>VariantRecordClasses.VariantRecordClass.other_associations_from_catalog</v>
       </c>
       <c r="B133" t="s">
-        <v>57</v>
+        <v>301</v>
       </c>
       <c r="C133" t="s">
-        <v>69</v>
+        <v>299</v>
       </c>
       <c r="D133" t="s">
         <v>229</v>
@@ -5227,7 +5224,7 @@
         <v>28</v>
       </c>
       <c r="F133" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K133">
         <v>2</v>
@@ -5239,81 +5236,78 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A135" s="2" t="s">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="str">
+        <f t="shared" ref="A134" si="16">CONCATENATE(D134,".",F134)</f>
+        <v>VariantRecordClasses.VariantRecordClass.linkage</v>
+      </c>
+      <c r="B134" t="s">
+        <v>57</v>
+      </c>
+      <c r="C134" t="s">
+        <v>69</v>
+      </c>
+      <c r="D134" t="s">
+        <v>229</v>
+      </c>
+      <c r="E134" t="s">
+        <v>28</v>
+      </c>
+      <c r="F134" t="s">
+        <v>302</v>
+      </c>
+      <c r="K134">
+        <v>2</v>
+      </c>
+      <c r="M134" t="s">
+        <v>25</v>
+      </c>
+      <c r="N134" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="str">
-        <f>CONCATENATE(D137,".",F137)</f>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="str">
+        <f>CONCATENATE(D138,".",F138)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.ResourceQuestions.GWAS</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B138" t="s">
         <v>57</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C138" t="s">
         <v>69</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D138" t="s">
         <v>426</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E138" t="s">
         <v>21</v>
       </c>
-      <c r="F137" t="s">
+      <c r="F138" t="s">
         <v>448</v>
       </c>
-      <c r="L137" t="s">
+      <c r="L138" t="s">
         <v>22</v>
       </c>
-      <c r="M137" t="s">
+      <c r="M138" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A139" s="2" t="s">
+    <row r="139" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
         <v>446</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A141" s="2" t="str">
-        <f t="shared" ref="A141" si="17">CONCATENATE(D141,".",F141)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.name</v>
-      </c>
-      <c r="B141" t="s">
-        <v>31</v>
-      </c>
-      <c r="C141" t="s">
-        <v>32</v>
-      </c>
-      <c r="D141" t="s">
-        <v>426</v>
-      </c>
-      <c r="E141" t="s">
-        <v>24</v>
-      </c>
-      <c r="F141" t="s">
-        <v>3</v>
-      </c>
-      <c r="K141">
-        <v>1</v>
-      </c>
-      <c r="L141" t="s">
-        <v>27</v>
-      </c>
-      <c r="M141" t="s">
-        <v>25</v>
-      </c>
-      <c r="N141" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="str">
-        <f t="shared" ref="A142" si="18">CONCATENATE(D142,".",F142)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.description</v>
+        <f t="shared" ref="A142" si="17">CONCATENATE(D142,".",F142)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.name</v>
       </c>
       <c r="B142" t="s">
         <v>31</v>
@@ -5328,10 +5322,10 @@
         <v>24</v>
       </c>
       <c r="F142" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K142">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L142" t="s">
         <v>27</v>
@@ -5345,8 +5339,8 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="str">
-        <f t="shared" ref="A143" si="19">CONCATENATE(D143,".",F143)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.attribution</v>
+        <f t="shared" ref="A143" si="18">CONCATENATE(D143,".",F143)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.description</v>
       </c>
       <c r="B143" t="s">
         <v>31</v>
@@ -5361,10 +5355,10 @@
         <v>24</v>
       </c>
       <c r="F143" t="s">
-        <v>430</v>
+        <v>6</v>
       </c>
       <c r="K143">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L143" t="s">
         <v>27</v>
@@ -5378,8 +5372,8 @@
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="str">
-        <f t="shared" ref="A144" si="20">CONCATENATE(D144,".",F144)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.version</v>
+        <f t="shared" ref="A144" si="19">CONCATENATE(D144,".",F144)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.attribution</v>
       </c>
       <c r="B144" t="s">
         <v>31</v>
@@ -5394,10 +5388,10 @@
         <v>24</v>
       </c>
       <c r="F144" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K144">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L144" t="s">
         <v>27</v>
@@ -5411,8 +5405,8 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="str">
-        <f t="shared" ref="A145" si="21">CONCATENATE(D145,".",F145)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.category</v>
+        <f t="shared" ref="A145" si="20">CONCATENATE(D145,".",F145)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.version</v>
       </c>
       <c r="B145" t="s">
         <v>31</v>
@@ -5427,10 +5421,10 @@
         <v>24</v>
       </c>
       <c r="F145" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K145">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L145" t="s">
         <v>27</v>
@@ -5444,8 +5438,8 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="str">
-        <f t="shared" ref="A146:A147" si="22">CONCATENATE(D146,".",F146)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.caveats</v>
+        <f t="shared" ref="A146" si="21">CONCATENATE(D146,".",F146)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.category</v>
       </c>
       <c r="B146" t="s">
         <v>31</v>
@@ -5460,50 +5454,53 @@
         <v>24</v>
       </c>
       <c r="F146" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K146">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="L146" t="s">
+        <v>27</v>
       </c>
       <c r="M146" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="N146" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="str">
+        <f t="shared" ref="A147:A148" si="22">CONCATENATE(D147,".",F147)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.caveats</v>
+      </c>
+      <c r="B147" t="s">
+        <v>31</v>
+      </c>
+      <c r="C147" t="s">
+        <v>32</v>
+      </c>
+      <c r="D147" t="s">
+        <v>426</v>
+      </c>
+      <c r="E147" t="s">
+        <v>24</v>
+      </c>
+      <c r="F147" t="s">
+        <v>433</v>
+      </c>
+      <c r="K147">
+        <v>2</v>
+      </c>
+      <c r="M147" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="str">
         <f t="shared" si="22"/>
         <v>DatasetRecordClasses.ResourceRecordClass.is_adsp</v>
       </c>
-      <c r="B147" t="s">
-        <v>31</v>
-      </c>
-      <c r="C147" t="s">
-        <v>32</v>
-      </c>
-      <c r="D147" t="s">
-        <v>426</v>
-      </c>
-      <c r="E147" t="s">
-        <v>24</v>
-      </c>
-      <c r="F147" t="s">
-        <v>434</v>
-      </c>
-      <c r="L147" t="s">
-        <v>27</v>
-      </c>
-      <c r="M147" t="s">
-        <v>25</v>
-      </c>
-      <c r="N147" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A148" s="2" t="str">
-        <f t="shared" ref="A148" si="23">CONCATENATE(D148,".",F148)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.accession_link</v>
-      </c>
       <c r="B148" t="s">
         <v>31</v>
       </c>
@@ -5517,7 +5514,7 @@
         <v>24</v>
       </c>
       <c r="F148" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="L148" t="s">
         <v>27</v>
@@ -5531,8 +5528,8 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="str">
-        <f t="shared" ref="A149" si="24">CONCATENATE(D149,".",F149)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.datasets</v>
+        <f t="shared" ref="A149" si="23">CONCATENATE(D149,".",F149)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.accession_link</v>
       </c>
       <c r="B149" t="s">
         <v>31</v>
@@ -5544,13 +5541,13 @@
         <v>426</v>
       </c>
       <c r="E149" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F149" t="s">
-        <v>305</v>
-      </c>
-      <c r="K149">
-        <v>2</v>
+        <v>429</v>
+      </c>
+      <c r="L149" t="s">
+        <v>27</v>
       </c>
       <c r="M149" t="s">
         <v>25</v>
@@ -5559,45 +5556,45 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A151" s="2" t="s">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="str">
+        <f t="shared" ref="A150" si="24">CONCATENATE(D150,".",F150)</f>
+        <v>DatasetRecordClasses.ResourceRecordClass.datasets</v>
+      </c>
+      <c r="B150" t="s">
+        <v>31</v>
+      </c>
+      <c r="C150" t="s">
+        <v>32</v>
+      </c>
+      <c r="D150" t="s">
+        <v>426</v>
+      </c>
+      <c r="E150" t="s">
+        <v>28</v>
+      </c>
+      <c r="F150" t="s">
+        <v>305</v>
+      </c>
+      <c r="K150">
+        <v>2</v>
+      </c>
+      <c r="M150" t="s">
+        <v>25</v>
+      </c>
+      <c r="N150" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
         <v>449</v>
-      </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A153" s="2" t="str">
-        <f t="shared" ref="A153:A157" si="25">CONCATENATE(D153,".",F153)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
-      </c>
-      <c r="B153" t="s">
-        <v>31</v>
-      </c>
-      <c r="C153" t="s">
-        <v>32</v>
-      </c>
-      <c r="D153" t="s">
-        <v>450</v>
-      </c>
-      <c r="E153" t="s">
-        <v>24</v>
-      </c>
-      <c r="F153" t="s">
-        <v>3</v>
-      </c>
-      <c r="L153" t="s">
-        <v>27</v>
-      </c>
-      <c r="M153" t="s">
-        <v>70</v>
-      </c>
-      <c r="N153" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="str">
-        <f t="shared" si="25"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
+        <f t="shared" ref="A154:A158" si="25">CONCATENATE(D154,".",F154)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
       </c>
       <c r="B154" t="s">
         <v>31</v>
@@ -5612,7 +5609,7 @@
         <v>24</v>
       </c>
       <c r="F154" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L154" t="s">
         <v>27</v>
@@ -5627,7 +5624,7 @@
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="str">
         <f t="shared" si="25"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
       </c>
       <c r="B155" t="s">
         <v>31</v>
@@ -5642,7 +5639,7 @@
         <v>24</v>
       </c>
       <c r="F155" t="s">
-        <v>432</v>
+        <v>6</v>
       </c>
       <c r="L155" t="s">
         <v>27</v>
@@ -5657,7 +5654,7 @@
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="str">
         <f t="shared" si="25"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
       </c>
       <c r="B156" t="s">
         <v>31</v>
@@ -5672,7 +5669,7 @@
         <v>24</v>
       </c>
       <c r="F156" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L156" t="s">
         <v>27</v>
@@ -5687,7 +5684,7 @@
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="str">
         <f t="shared" si="25"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
       </c>
       <c r="B157" t="s">
         <v>31</v>
@@ -5702,7 +5699,7 @@
         <v>24</v>
       </c>
       <c r="F157" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="L157" t="s">
         <v>27</v>
@@ -5710,11 +5707,14 @@
       <c r="M157" t="s">
         <v>70</v>
       </c>
+      <c r="N157" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="str">
-        <f t="shared" ref="A158" si="26">CONCATENATE(D158,".",F158)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.niagads_accession</v>
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
       </c>
       <c r="B158" t="s">
         <v>31</v>
@@ -5729,19 +5729,19 @@
         <v>24</v>
       </c>
       <c r="F158" t="s">
-        <v>481</v>
+        <v>429</v>
+      </c>
+      <c r="L158" t="s">
+        <v>27</v>
       </c>
       <c r="M158" t="s">
         <v>70</v>
-      </c>
-      <c r="N158" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="str">
-        <f t="shared" ref="A159:A164" si="27">CONCATENATE(D159,".",F159)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
+        <f t="shared" ref="A159" si="26">CONCATENATE(D159,".",F159)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.niagads_accession</v>
       </c>
       <c r="B159" t="s">
         <v>31</v>
@@ -5756,74 +5756,74 @@
         <v>24</v>
       </c>
       <c r="F159" t="s">
+        <v>480</v>
+      </c>
+      <c r="M159" t="s">
+        <v>70</v>
+      </c>
+      <c r="N159" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="str">
+        <f t="shared" ref="A160:A165" si="27">CONCATENATE(D160,".",F160)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
+      </c>
+      <c r="B160" t="s">
+        <v>31</v>
+      </c>
+      <c r="C160" t="s">
+        <v>32</v>
+      </c>
+      <c r="D160" t="s">
+        <v>450</v>
+      </c>
+      <c r="E160" t="s">
+        <v>24</v>
+      </c>
+      <c r="F160" t="s">
         <v>451</v>
       </c>
-      <c r="L159" t="s">
+      <c r="L160" t="s">
         <v>27</v>
       </c>
-      <c r="M159" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A161" s="2" t="str">
-        <f>CONCATENATE(D161,".",F161)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
-      </c>
-      <c r="B161" t="s">
-        <v>456</v>
-      </c>
-      <c r="C161" t="s">
-        <v>156</v>
-      </c>
-      <c r="D161" t="s">
-        <v>450</v>
-      </c>
-      <c r="E161" t="s">
-        <v>28</v>
-      </c>
-      <c r="F161" t="s">
-        <v>452</v>
-      </c>
-      <c r="K161">
-        <v>1</v>
-      </c>
-      <c r="M161" t="s">
-        <v>25</v>
+      <c r="M160" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="str">
+        <f>CONCATENATE(D162,".",F162)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
+      </c>
+      <c r="B162" t="s">
+        <v>456</v>
+      </c>
+      <c r="C162" t="s">
+        <v>156</v>
+      </c>
+      <c r="D162" t="s">
+        <v>450</v>
+      </c>
+      <c r="E162" t="s">
+        <v>28</v>
+      </c>
+      <c r="F162" t="s">
+        <v>452</v>
+      </c>
+      <c r="K162">
+        <v>1</v>
+      </c>
+      <c r="M162" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="str">
         <f t="shared" si="27"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
       </c>
-      <c r="B162" t="s">
-        <v>456</v>
-      </c>
-      <c r="C162" t="s">
-        <v>156</v>
-      </c>
-      <c r="D162" t="s">
-        <v>450</v>
-      </c>
-      <c r="E162" t="s">
-        <v>28</v>
-      </c>
-      <c r="F162" t="s">
-        <v>455</v>
-      </c>
-      <c r="K162">
-        <v>2</v>
-      </c>
-      <c r="M162" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A163" s="2" t="str">
-        <f>CONCATENATE(D163,".",F163)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
-      </c>
       <c r="B163" t="s">
         <v>456</v>
       </c>
@@ -5837,10 +5837,10 @@
         <v>28</v>
       </c>
       <c r="F163" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K163">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M163" t="s">
         <v>25</v>
@@ -5848,36 +5848,36 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="str">
+        <f>CONCATENATE(D164,".",F164)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
+      </c>
+      <c r="B164" t="s">
+        <v>456</v>
+      </c>
+      <c r="C164" t="s">
+        <v>156</v>
+      </c>
+      <c r="D164" t="s">
+        <v>450</v>
+      </c>
+      <c r="E164" t="s">
+        <v>28</v>
+      </c>
+      <c r="F164" t="s">
+        <v>454</v>
+      </c>
+      <c r="K164">
+        <v>3</v>
+      </c>
+      <c r="M164" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="str">
         <f t="shared" si="27"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
       </c>
-      <c r="B164" t="s">
-        <v>457</v>
-      </c>
-      <c r="C164" t="s">
-        <v>458</v>
-      </c>
-      <c r="D164" t="s">
-        <v>450</v>
-      </c>
-      <c r="E164" t="s">
-        <v>28</v>
-      </c>
-      <c r="F164" t="s">
-        <v>453</v>
-      </c>
-      <c r="K164">
-        <v>1</v>
-      </c>
-      <c r="M164" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="str">
-        <f t="shared" ref="A165:A166" si="28">CONCATENATE(D165,".",F165)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
-      </c>
       <c r="B165" t="s">
         <v>457</v>
       </c>
@@ -5891,10 +5891,10 @@
         <v>28</v>
       </c>
       <c r="F165" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="K165">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M165" t="s">
         <v>25</v>
@@ -5902,36 +5902,36 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="str">
+        <f t="shared" ref="A166:A167" si="28">CONCATENATE(D166,".",F166)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
+      </c>
+      <c r="B166" t="s">
+        <v>457</v>
+      </c>
+      <c r="C166" t="s">
+        <v>458</v>
+      </c>
+      <c r="D166" t="s">
+        <v>450</v>
+      </c>
+      <c r="E166" t="s">
+        <v>28</v>
+      </c>
+      <c r="F166" t="s">
+        <v>461</v>
+      </c>
+      <c r="K166">
+        <v>3</v>
+      </c>
+      <c r="M166" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="str">
         <f t="shared" si="28"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
       </c>
-      <c r="B166" t="s">
-        <v>457</v>
-      </c>
-      <c r="C166" t="s">
-        <v>458</v>
-      </c>
-      <c r="D166" t="s">
-        <v>450</v>
-      </c>
-      <c r="E166" t="s">
-        <v>28</v>
-      </c>
-      <c r="F166" t="s">
-        <v>462</v>
-      </c>
-      <c r="K166">
-        <v>4</v>
-      </c>
-      <c r="M166" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A167" s="2" t="str">
-        <f t="shared" ref="A167" si="29">CONCATENATE(D167,".",F167)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
-      </c>
       <c r="B167" t="s">
         <v>457</v>
       </c>
@@ -5945,10 +5945,10 @@
         <v>28</v>
       </c>
       <c r="F167" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K167">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M167" t="s">
         <v>25</v>
@@ -5956,14 +5956,14 @@
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="str">
-        <f t="shared" ref="A168:A169" si="30">CONCATENATE(D168,".",F168)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+        <f t="shared" ref="A168" si="29">CONCATENATE(D168,".",F168)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
       </c>
       <c r="B168" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C168" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D168" t="s">
         <v>450</v>
@@ -5972,7 +5972,7 @@
         <v>28</v>
       </c>
       <c r="F168" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K168">
         <v>2</v>
@@ -5983,41 +5983,41 @@
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="str">
+        <f t="shared" ref="A169:A170" si="30">CONCATENATE(D169,".",F169)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+      </c>
+      <c r="B169" t="s">
+        <v>459</v>
+      </c>
+      <c r="C169" t="s">
+        <v>460</v>
+      </c>
+      <c r="D169" t="s">
+        <v>450</v>
+      </c>
+      <c r="E169" t="s">
+        <v>28</v>
+      </c>
+      <c r="F169" t="s">
+        <v>465</v>
+      </c>
+      <c r="K169">
+        <v>2</v>
+      </c>
+      <c r="M169" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="str">
         <f t="shared" si="30"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B170" t="s">
         <v>459</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C170" t="s">
         <v>460</v>
-      </c>
-      <c r="D169" t="s">
-        <v>450</v>
-      </c>
-      <c r="E169" t="s">
-        <v>28</v>
-      </c>
-      <c r="F169" t="s">
-        <v>466</v>
-      </c>
-      <c r="K169">
-        <v>1</v>
-      </c>
-      <c r="M169" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="str">
-        <f>CONCATENATE(D170,".",F170)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
-      </c>
-      <c r="B170" t="s">
-        <v>57</v>
-      </c>
-      <c r="C170" t="s">
-        <v>69</v>
       </c>
       <c r="D170" t="s">
         <v>450</v>
@@ -6026,7 +6026,10 @@
         <v>28</v>
       </c>
       <c r="F170" t="s">
-        <v>464</v>
+        <v>466</v>
+      </c>
+      <c r="K170">
+        <v>1</v>
       </c>
       <c r="M170" t="s">
         <v>25</v>
@@ -6035,13 +6038,13 @@
     <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="str">
         <f>CONCATENATE(D171,".",F171)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
       </c>
       <c r="B171" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C171" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D171" t="s">
         <v>450</v>
@@ -6050,46 +6053,40 @@
         <v>28</v>
       </c>
       <c r="F171" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="M171" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A173" s="2" t="str">
-        <f>CONCATENATE(D173,".",F173)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
-      </c>
-      <c r="B173" t="s">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="str">
+        <f>CONCATENATE(D172,".",F172)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+      </c>
+      <c r="B172" t="s">
         <v>31</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C172" t="s">
         <v>32</v>
       </c>
-      <c r="D173" t="s">
-        <v>468</v>
-      </c>
-      <c r="E173" t="s">
-        <v>24</v>
-      </c>
-      <c r="F173" t="s">
-        <v>3</v>
-      </c>
-      <c r="L173" t="s">
-        <v>470</v>
-      </c>
-      <c r="M173" t="s">
-        <v>70</v>
-      </c>
-      <c r="N173" t="s">
-        <v>26</v>
+      <c r="D172" t="s">
+        <v>450</v>
+      </c>
+      <c r="E172" t="s">
+        <v>28</v>
+      </c>
+      <c r="F172" t="s">
+        <v>467</v>
+      </c>
+      <c r="M172" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="str">
-        <f t="shared" ref="A174:A177" si="31">CONCATENATE(D174,".",F174)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
+        <f>CONCATENATE(D174,".",F174)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
       </c>
       <c r="B174" t="s">
         <v>31</v>
@@ -6104,7 +6101,7 @@
         <v>24</v>
       </c>
       <c r="F174" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L174" t="s">
         <v>470</v>
@@ -6118,8 +6115,8 @@
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="str">
-        <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
+        <f t="shared" ref="A175:A178" si="31">CONCATENATE(D175,".",F175)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
       </c>
       <c r="B175" t="s">
         <v>31</v>
@@ -6134,7 +6131,7 @@
         <v>24</v>
       </c>
       <c r="F175" t="s">
-        <v>469</v>
+        <v>6</v>
       </c>
       <c r="L175" t="s">
         <v>470</v>
@@ -6149,7 +6146,7 @@
     <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="str">
         <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
       </c>
       <c r="B176" t="s">
         <v>31</v>
@@ -6164,7 +6161,7 @@
         <v>24</v>
       </c>
       <c r="F176" t="s">
-        <v>434</v>
+        <v>469</v>
       </c>
       <c r="L176" t="s">
         <v>470</v>
@@ -6176,10 +6173,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="str">
         <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
       </c>
       <c r="B177" t="s">
         <v>31</v>
@@ -6191,15 +6188,45 @@
         <v>468</v>
       </c>
       <c r="E177" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F177" t="s">
-        <v>305</v>
+        <v>434</v>
       </c>
       <c r="L177" t="s">
         <v>470</v>
       </c>
       <c r="M177" t="s">
+        <v>70</v>
+      </c>
+      <c r="N177" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+      </c>
+      <c r="B178" t="s">
+        <v>31</v>
+      </c>
+      <c r="C178" t="s">
+        <v>32</v>
+      </c>
+      <c r="D178" t="s">
+        <v>468</v>
+      </c>
+      <c r="E178" t="s">
+        <v>28</v>
+      </c>
+      <c r="F178" t="s">
+        <v>305</v>
+      </c>
+      <c r="L178" t="s">
+        <v>470</v>
+      </c>
+      <c r="M178" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update dataset summary attributes
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/www/genomics/project_home/GenomicsDBWebsite/Model/lib/wdk/ontology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenem\niagads_genomicsdb\GenomicsDBWebsite\Model\lib\wdk\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A75057-A1DA-364E-A598-E07A38181701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4596D352-B27E-4809-BE7C-81286471063B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="49000" windowHeight="20900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="6" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="484">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1516,6 +1516,9 @@
   </si>
   <si>
     <t>gws_datasets_summary_plot</t>
+  </si>
+  <si>
+    <t>interactive_manhattan_plot</t>
   </si>
 </sst>
 </file>
@@ -1854,32 +1857,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N178"/>
+  <dimension ref="A1:N180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D158" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K52" sqref="K52"/>
+      <selection pane="bottomRight" activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="82.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="38.83203125" customWidth="1"/>
-    <col min="7" max="7" width="68.6640625" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
-    <col min="9" max="9" width="80.6640625" customWidth="1"/>
-    <col min="10" max="10" width="32.83203125" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" customWidth="1"/>
+    <col min="6" max="6" width="38.875" customWidth="1"/>
+    <col min="7" max="7" width="68.625" customWidth="1"/>
+    <col min="8" max="8" width="33.625" customWidth="1"/>
+    <col min="9" max="9" width="80.625" customWidth="1"/>
+    <col min="10" max="10" width="32.875" customWidth="1"/>
+    <col min="11" max="11" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -1952,12 +1955,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1985,12 +1988,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
         <f>CONCATENATE(D11,".",F11)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.GeneTextSearch</v>
@@ -2017,7 +2020,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
         <f>CONCATENATE(D12,".",F12)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.Identifier</v>
@@ -2044,7 +2047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
         <f>CONCATENATE(D13,".",F13)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneQuestions.Upload</v>
@@ -2071,7 +2074,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f>CONCATENATE(D14,".",F14)</f>
         <v>GeneRecordClasses.GeneRecordClass.GeneRisk</v>
@@ -2098,12 +2101,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f>CONCATENATE(D18,".",F18)</f>
         <v>GeneRecordClasses.GeneRecordClass.source_id</v>
@@ -2133,7 +2136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f t="shared" ref="A19:A53" si="0">CONCATENATE(D19,".",F19)</f>
         <v>GeneRecordClasses.GeneRecordClass.chromosome</v>
@@ -2166,7 +2169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_name</v>
@@ -2199,7 +2202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_type</v>
@@ -2232,7 +2235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.strand</v>
@@ -2262,7 +2265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.location_start</v>
@@ -2295,7 +2298,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.location_end</v>
@@ -2328,7 +2331,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.gene_symbol</v>
@@ -2361,7 +2364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.synonyms</v>
@@ -2394,7 +2397,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.jbrowse_span</v>
@@ -2421,7 +2424,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.has_ad_evidence</v>
@@ -2451,7 +2454,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_evidence_flag</v>
@@ -2481,7 +2484,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.num_colocated_variants</v>
@@ -2514,7 +2517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.num_unique_colocated_variants</v>
@@ -2547,7 +2550,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.is_reversed</v>
@@ -2571,7 +2574,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.hgnc_id</v>
@@ -2604,7 +2607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.omim_id</v>
@@ -2637,7 +2640,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ucsc_id</v>
@@ -2670,7 +2673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.vega_id</v>
@@ -2703,7 +2706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.entrez_id</v>
@@ -2736,7 +2739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ensembl_id</v>
@@ -2769,7 +2772,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.uniprot_id</v>
@@ -2802,7 +2805,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.cytogenetic_location</v>
@@ -2835,7 +2838,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.full_jbrowse_link</v>
@@ -2862,7 +2865,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="str">
         <f t="shared" ref="A43" si="1">CONCATENATE(D43,".",F43)</f>
         <v>GeneRecordClasses.GeneRecordClass.jbrowse_source_url</v>
@@ -2889,7 +2892,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.dynspan_link</v>
@@ -2916,7 +2919,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.span</v>
@@ -2949,7 +2952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_skat_adsp</v>
@@ -2982,7 +2985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_gwas</v>
@@ -3015,7 +3018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.other_variants_from_gwas</v>
@@ -3048,7 +3051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="str">
         <f>CONCATENATE(D50,".",F50)</f>
         <v>GeneRecordClasses.GeneRecordClass.ad_variants_from_catalog</v>
@@ -3081,7 +3084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.other_variants_from_catalog</v>
@@ -3114,7 +3117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.go_terms</v>
@@ -3147,7 +3150,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GeneRecordClasses.GeneRecordClass.pathways</v>
@@ -3180,7 +3183,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="str">
         <f t="shared" ref="A54:A58" si="2">CONCATENATE(D54,".",F54)</f>
         <v>GeneRecordClasses.GeneRecordClass.record_link_outs</v>
@@ -3213,7 +3216,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.sequence_link_outs</v>
@@ -3246,7 +3249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.protein_link_outs</v>
@@ -3279,7 +3282,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.clinical_link_outs</v>
@@ -3312,7 +3315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="str">
         <f t="shared" si="2"/>
         <v>GeneRecordClasses.GeneRecordClass.transcript_link_outs</v>
@@ -3345,7 +3348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="str">
         <f>CONCATENATE(D59,".",F59)</f>
         <v>GeneRecordClasses.GeneRecordClass.gws_variants_summary_plot</v>
@@ -3369,12 +3372,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="str">
         <f>CONCATENATE(D63,".",F63)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vid</v>
@@ -3401,7 +3404,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="str">
         <f>CONCATENATE(D64,".",F64)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.vupload</v>
@@ -3428,7 +3431,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="str">
         <f>CONCATENATE(D65,".",F65)</f>
         <v>VariantRecordClasses.VariantRecordClass.VariantQuestions.gwas_stats</v>
@@ -3455,12 +3458,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="str">
         <f>CONCATENATE(D69,".",F69)</f>
         <v>VariantRecordClasses.VariantRecordClass.variant_source</v>
@@ -3490,7 +3493,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="str">
         <f t="shared" ref="A70:A127" si="3">CONCATENATE(D70,".",F70)</f>
         <v>VariantRecordClasses.VariantRecordClass.ref_snp_id</v>
@@ -3520,7 +3523,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="str">
         <f t="shared" ref="A71" si="4">CONCATENATE(D71,".",F71)</f>
         <v>VariantRecordClasses.VariantRecordClass.metaseq_id</v>
@@ -3550,7 +3553,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="str">
         <f t="shared" ref="A72" si="5">CONCATENATE(D72,".",F72)</f>
         <v>VariantRecordClasses.VariantRecordClass.is_annotated</v>
@@ -3574,7 +3577,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="str">
         <f t="shared" ref="A73" si="6">CONCATENATE(D73,".",F73)</f>
         <v>VariantRecordClasses.VariantRecordClass.adsp_id</v>
@@ -3604,7 +3607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.ref_allele</v>
@@ -3634,7 +3637,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.alt_allele</v>
@@ -3664,7 +3667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.chromosome</v>
@@ -3694,7 +3697,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.position</v>
@@ -3724,7 +3727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.location</v>
@@ -3754,7 +3757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.full_jbrowse_link</v>
@@ -3778,7 +3781,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.jbrowse_source_url</v>
@@ -3802,7 +3805,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="str">
         <f>CONCATENATE(D81,".",F81)</f>
         <v>VariantRecordClasses.VariantRecordClass.display_allele</v>
@@ -3832,7 +3835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="str">
         <f>CONCATENATE(D82,".",F82)</f>
         <v>VariantRecordClasses.VariantRecordClass.sequence_allele</v>
@@ -3862,7 +3865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.upstream_sequence</v>
@@ -3886,7 +3889,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.downstream_sequence</v>
@@ -3910,7 +3913,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_variant</v>
@@ -3940,7 +3943,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_wes</v>
@@ -3970,7 +3973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_adsp_wgs</v>
@@ -4000,7 +4003,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_multi_allelic</v>
@@ -4030,7 +4033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.is_reversed</v>
@@ -4057,7 +4060,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.variant_class</v>
@@ -4087,7 +4090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.variant_class_abbrev</v>
@@ -4117,7 +4120,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.sequence</v>
@@ -4144,7 +4147,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.has_merge_history</v>
@@ -4168,7 +4171,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.current_rsid</v>
@@ -4192,7 +4195,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.current_primary_key</v>
@@ -4216,7 +4219,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status</v>
@@ -4243,7 +4246,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status</v>
@@ -4270,7 +4273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="str">
         <f t="shared" ref="A98:A99" si="7">CONCATENATE(D98,".",F98)</f>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wes_qc_filter_status_display</v>
@@ -4297,7 +4300,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="str">
         <f t="shared" si="7"/>
         <v>VariantRecordClasses.VariantRecordClass.adsp_wgs_qc_filter_status_display</v>
@@ -4324,7 +4327,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_gene_link</v>
@@ -4351,7 +4354,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_gene</v>
@@ -4378,7 +4381,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.num_colocated_genes</v>
@@ -4408,7 +4411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.colocated_transcripts</v>
@@ -4432,7 +4435,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.cadd_raw_score</v>
@@ -4462,7 +4465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.cadd_phred_score</v>
@@ -4492,7 +4495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="str">
         <f t="shared" ref="A106" si="8">CONCATENATE(D106,".",F106)</f>
         <v>VariantRecordClasses.VariantRecordClass.num_colocated_variants</v>
@@ -4516,7 +4519,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="str">
         <f t="shared" ref="A107:A118" si="9">CONCATENATE(D107,".",F107)</f>
         <v>VariantRecordClasses.VariantRecordClass.colocated_variants</v>
@@ -4540,7 +4543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.num_alternative_variants</v>
@@ -4564,7 +4567,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.alternative_variants</v>
@@ -4588,7 +4591,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.most_severe_consequence</v>
@@ -4618,7 +4621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impact</v>
@@ -4648,7 +4651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene_link</v>
@@ -4675,7 +4678,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_gene</v>
@@ -4702,7 +4705,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_symbol</v>
@@ -4729,7 +4732,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_impacted_transcript</v>
@@ -4759,7 +4762,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_amino_acid_change</v>
@@ -4789,7 +4792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_codon_change</v>
@@ -4819,7 +4822,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="str">
         <f t="shared" si="9"/>
         <v>VariantRecordClasses.VariantRecordClass.msc_is_coding</v>
@@ -4849,7 +4852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="str">
         <f t="shared" ref="A119:A120" si="10">CONCATENATE(D119,".",F119)</f>
         <v>VariantRecordClasses.VariantRecordClass.num_impacted_transcripts</v>
@@ -4873,7 +4876,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="str">
         <f t="shared" si="10"/>
         <v>VariantRecordClasses.VariantRecordClass.num_impacted_genes</v>
@@ -4897,7 +4900,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="str">
         <f t="shared" ref="A121" si="11">CONCATENATE(D121,".",F121)</f>
         <v>VariantRecordClasses.VariantRecordClass.transcript_consequence_summary</v>
@@ -4921,7 +4924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="str">
         <f t="shared" ref="A122" si="12">CONCATENATE(D122,".",F122)</f>
         <v>VariantRecordClasses.VariantRecordClass.locuszoom_gwas_datasets</v>
@@ -4948,7 +4951,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="str">
         <f>CONCATENATE(D123,".",F123)</f>
         <v>VariantRecordClasses.VariantRecordClass.display_metaseq_id</v>
@@ -4972,7 +4975,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="str">
         <f>CONCATENATE(D124,".",F124)</f>
         <v>VariantRecordClasses.VariantRecordClass.gws_datasets_summary_plot</v>
@@ -4996,7 +4999,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="str">
         <f t="shared" ref="A126" si="13">CONCATENATE(D126,".",F126)</f>
         <v>VariantRecordClasses.VariantRecordClass.allele_frequencies</v>
@@ -5026,7 +5029,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="str">
         <f t="shared" si="3"/>
         <v>VariantRecordClasses.VariantRecordClass.transcript_consequences</v>
@@ -5056,7 +5059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="str">
         <f t="shared" ref="A128:A133" si="14">CONCATENATE(D128,".",F128)</f>
         <v>VariantRecordClasses.VariantRecordClass.intergenic_consequences</v>
@@ -5086,7 +5089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="str">
         <f t="shared" ref="A129" si="15">CONCATENATE(D129,".",F129)</f>
         <v>VariantRecordClasses.VariantRecordClass.regulatory_consequences</v>
@@ -5116,7 +5119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_gwas</v>
@@ -5146,7 +5149,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.other_associations_from_gwas</v>
@@ -5176,7 +5179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.ad_associations_from_catalog</v>
@@ -5206,7 +5209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="str">
         <f t="shared" si="14"/>
         <v>VariantRecordClasses.VariantRecordClass.other_associations_from_catalog</v>
@@ -5236,7 +5239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="str">
         <f t="shared" ref="A134" si="16">CONCATENATE(D134,".",F134)</f>
         <v>VariantRecordClasses.VariantRecordClass.linkage</v>
@@ -5266,12 +5269,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="str">
         <f>CONCATENATE(D138,".",F138)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.ResourceQuestions.GWAS</v>
@@ -5298,13 +5301,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="str">
         <f t="shared" ref="A142" si="17">CONCATENATE(D142,".",F142)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.name</v>
@@ -5337,7 +5340,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="str">
         <f t="shared" ref="A143" si="18">CONCATENATE(D143,".",F143)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.description</v>
@@ -5370,7 +5373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="str">
         <f t="shared" ref="A144" si="19">CONCATENATE(D144,".",F144)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.attribution</v>
@@ -5403,7 +5406,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="str">
         <f t="shared" ref="A145" si="20">CONCATENATE(D145,".",F145)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.version</v>
@@ -5436,7 +5439,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="str">
         <f t="shared" ref="A146" si="21">CONCATENATE(D146,".",F146)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.category</v>
@@ -5469,7 +5472,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="str">
         <f t="shared" ref="A147:A148" si="22">CONCATENATE(D147,".",F147)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.caveats</v>
@@ -5496,7 +5499,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="str">
         <f t="shared" si="22"/>
         <v>DatasetRecordClasses.ResourceRecordClass.is_adsp</v>
@@ -5526,7 +5529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="str">
         <f t="shared" ref="A149" si="23">CONCATENATE(D149,".",F149)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.accession_link</v>
@@ -5556,7 +5559,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="str">
         <f t="shared" ref="A150" si="24">CONCATENATE(D150,".",F150)</f>
         <v>DatasetRecordClasses.ResourceRecordClass.datasets</v>
@@ -5586,12 +5589,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="str">
         <f t="shared" ref="A154:A158" si="25">CONCATENATE(D154,".",F154)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
@@ -5611,9 +5614,6 @@
       <c r="F154" t="s">
         <v>3</v>
       </c>
-      <c r="L154" t="s">
-        <v>27</v>
-      </c>
       <c r="M154" t="s">
         <v>70</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
@@ -5651,7 +5651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
@@ -5671,17 +5671,11 @@
       <c r="F156" t="s">
         <v>432</v>
       </c>
-      <c r="L156" t="s">
-        <v>27</v>
-      </c>
       <c r="M156" t="s">
         <v>70</v>
       </c>
-      <c r="N156" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
@@ -5711,7 +5705,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="str">
         <f t="shared" si="25"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
@@ -5738,7 +5732,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="str">
         <f t="shared" ref="A159" si="26">CONCATENATE(D159,".",F159)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.niagads_accession</v>
@@ -5765,9 +5759,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="str">
-        <f t="shared" ref="A160:A165" si="27">CONCATENATE(D160,".",F160)</f>
+        <f t="shared" ref="A160:A167" si="27">CONCATENATE(D160,".",F160)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
       </c>
       <c r="B160" t="s">
@@ -5792,16 +5786,46 @@
         <v>70</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="str">
+        <f t="shared" ref="A161" si="28">CONCATENATE(D161,".",F161)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.attribution</v>
+      </c>
+      <c r="B161" t="s">
+        <v>31</v>
+      </c>
+      <c r="C161" t="s">
+        <v>32</v>
+      </c>
+      <c r="D161" t="s">
+        <v>450</v>
+      </c>
+      <c r="E161" t="s">
+        <v>24</v>
+      </c>
+      <c r="F161" t="s">
+        <v>430</v>
+      </c>
+      <c r="L161" t="s">
+        <v>27</v>
+      </c>
+      <c r="M161" t="s">
+        <v>70</v>
+      </c>
+      <c r="N161" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="str">
         <f>CONCATENATE(D162,".",F162)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.interactive_manhattan_plot</v>
       </c>
       <c r="B162" t="s">
-        <v>456</v>
+        <v>57</v>
       </c>
       <c r="C162" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="D162" t="s">
         <v>450</v>
@@ -5810,7 +5834,7 @@
         <v>28</v>
       </c>
       <c r="F162" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="K162">
         <v>1</v>
@@ -5819,119 +5843,92 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A163" s="2" t="str">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="str">
+        <f>CONCATENATE(D164,".",F164)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
+      </c>
+      <c r="B164" t="s">
+        <v>456</v>
+      </c>
+      <c r="C164" t="s">
+        <v>156</v>
+      </c>
+      <c r="D164" t="s">
+        <v>450</v>
+      </c>
+      <c r="E164" t="s">
+        <v>28</v>
+      </c>
+      <c r="F164" t="s">
+        <v>452</v>
+      </c>
+      <c r="K164">
+        <v>1</v>
+      </c>
+      <c r="M164" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="str">
         <f t="shared" si="27"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>456</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C165" t="s">
         <v>156</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D165" t="s">
         <v>450</v>
       </c>
-      <c r="E163" t="s">
+      <c r="E165" t="s">
         <v>28</v>
       </c>
-      <c r="F163" t="s">
+      <c r="F165" t="s">
         <v>455</v>
       </c>
-      <c r="K163">
+      <c r="K165">
         <v>2</v>
       </c>
-      <c r="M163" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="str">
-        <f>CONCATENATE(D164,".",F164)</f>
+      <c r="M165" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="str">
+        <f>CONCATENATE(D166,".",F166)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>456</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C166" t="s">
         <v>156</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D166" t="s">
         <v>450</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E166" t="s">
         <v>28</v>
       </c>
-      <c r="F164" t="s">
+      <c r="F166" t="s">
         <v>454</v>
       </c>
-      <c r="K164">
+      <c r="K166">
         <v>3</v>
       </c>
-      <c r="M164" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="str">
+      <c r="M166" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="str">
         <f t="shared" si="27"/>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
       </c>
-      <c r="B165" t="s">
-        <v>457</v>
-      </c>
-      <c r="C165" t="s">
-        <v>458</v>
-      </c>
-      <c r="D165" t="s">
-        <v>450</v>
-      </c>
-      <c r="E165" t="s">
-        <v>28</v>
-      </c>
-      <c r="F165" t="s">
-        <v>453</v>
-      </c>
-      <c r="K165">
-        <v>1</v>
-      </c>
-      <c r="M165" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="str">
-        <f t="shared" ref="A166:A167" si="28">CONCATENATE(D166,".",F166)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
-      </c>
-      <c r="B166" t="s">
-        <v>457</v>
-      </c>
-      <c r="C166" t="s">
-        <v>458</v>
-      </c>
-      <c r="D166" t="s">
-        <v>450</v>
-      </c>
-      <c r="E166" t="s">
-        <v>28</v>
-      </c>
-      <c r="F166" t="s">
-        <v>461</v>
-      </c>
-      <c r="K166">
-        <v>3</v>
-      </c>
-      <c r="M166" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A167" s="2" t="str">
-        <f t="shared" si="28"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
-      </c>
       <c r="B167" t="s">
         <v>457</v>
       </c>
@@ -5945,19 +5942,19 @@
         <v>28</v>
       </c>
       <c r="F167" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="K167">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M167" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="str">
-        <f t="shared" ref="A168" si="29">CONCATENATE(D168,".",F168)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
+        <f t="shared" ref="A168:A169" si="29">CONCATENATE(D168,".",F168)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
       </c>
       <c r="B168" t="s">
         <v>457</v>
@@ -5972,25 +5969,25 @@
         <v>28</v>
       </c>
       <c r="F168" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K168">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M168" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="str">
-        <f t="shared" ref="A169:A170" si="30">CONCATENATE(D169,".",F169)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+        <f t="shared" si="29"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
       </c>
       <c r="B169" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C169" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D169" t="s">
         <v>450</v>
@@ -5999,25 +5996,25 @@
         <v>28</v>
       </c>
       <c r="F169" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="K169">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M169" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
+        <f t="shared" ref="A170" si="30">CONCATENATE(D170,".",F170)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
       </c>
       <c r="B170" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C170" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D170" t="s">
         <v>450</v>
@@ -6026,25 +6023,25 @@
         <v>28</v>
       </c>
       <c r="F170" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="K170">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M170" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="str">
-        <f>CONCATENATE(D171,".",F171)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
+        <f t="shared" ref="A171:A172" si="31">CONCATENATE(D171,".",F171)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
       </c>
       <c r="B171" t="s">
-        <v>57</v>
+        <v>459</v>
       </c>
       <c r="C171" t="s">
-        <v>69</v>
+        <v>460</v>
       </c>
       <c r="D171" t="s">
         <v>450</v>
@@ -6053,22 +6050,25 @@
         <v>28</v>
       </c>
       <c r="F171" t="s">
-        <v>464</v>
+        <v>465</v>
+      </c>
+      <c r="K171">
+        <v>2</v>
       </c>
       <c r="M171" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="str">
-        <f>CONCATENATE(D172,".",F172)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
       </c>
       <c r="B172" t="s">
-        <v>31</v>
+        <v>459</v>
       </c>
       <c r="C172" t="s">
-        <v>32</v>
+        <v>460</v>
       </c>
       <c r="D172" t="s">
         <v>450</v>
@@ -6077,16 +6077,46 @@
         <v>28</v>
       </c>
       <c r="F172" t="s">
-        <v>467</v>
+        <v>466</v>
+      </c>
+      <c r="K172">
+        <v>1</v>
       </c>
       <c r="M172" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="str">
+        <f>CONCATENATE(D173,".",F173)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
+      </c>
+      <c r="B173" t="s">
+        <v>57</v>
+      </c>
+      <c r="C173" t="s">
+        <v>69</v>
+      </c>
+      <c r="D173" t="s">
+        <v>450</v>
+      </c>
+      <c r="E173" t="s">
+        <v>28</v>
+      </c>
+      <c r="F173" t="s">
+        <v>464</v>
+      </c>
+      <c r="K173">
+        <v>2</v>
+      </c>
+      <c r="M173" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="str">
         <f>CONCATENATE(D174,".",F174)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
       </c>
       <c r="B174" t="s">
         <v>31</v>
@@ -6095,58 +6125,22 @@
         <v>32</v>
       </c>
       <c r="D174" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="E174" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F174" t="s">
-        <v>3</v>
-      </c>
-      <c r="L174" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="M174" t="s">
-        <v>70</v>
-      </c>
-      <c r="N174" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A175" s="2" t="str">
-        <f t="shared" ref="A175:A178" si="31">CONCATENATE(D175,".",F175)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
-      </c>
-      <c r="B175" t="s">
-        <v>31</v>
-      </c>
-      <c r="C175" t="s">
-        <v>32</v>
-      </c>
-      <c r="D175" t="s">
-        <v>468</v>
-      </c>
-      <c r="E175" t="s">
-        <v>24</v>
-      </c>
-      <c r="F175" t="s">
-        <v>6</v>
-      </c>
-      <c r="L175" t="s">
-        <v>470</v>
-      </c>
-      <c r="M175" t="s">
-        <v>70</v>
-      </c>
-      <c r="N175" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="str">
-        <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
+        <f>CONCATENATE(D176,".",F176)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
       </c>
       <c r="B176" t="s">
         <v>31</v>
@@ -6161,7 +6155,7 @@
         <v>24</v>
       </c>
       <c r="F176" t="s">
-        <v>469</v>
+        <v>3</v>
       </c>
       <c r="L176" t="s">
         <v>470</v>
@@ -6173,10 +6167,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="str">
-        <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+        <f t="shared" ref="A177:A180" si="32">CONCATENATE(D177,".",F177)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
       </c>
       <c r="B177" t="s">
         <v>31</v>
@@ -6191,7 +6185,7 @@
         <v>24</v>
       </c>
       <c r="F177" t="s">
-        <v>434</v>
+        <v>6</v>
       </c>
       <c r="L177" t="s">
         <v>470</v>
@@ -6203,10 +6197,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="str">
-        <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+        <f t="shared" si="32"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
       </c>
       <c r="B178" t="s">
         <v>31</v>
@@ -6218,15 +6212,75 @@
         <v>468</v>
       </c>
       <c r="E178" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F178" t="s">
-        <v>305</v>
+        <v>469</v>
       </c>
       <c r="L178" t="s">
         <v>470</v>
       </c>
       <c r="M178" t="s">
+        <v>70</v>
+      </c>
+      <c r="N178" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+      </c>
+      <c r="B179" t="s">
+        <v>31</v>
+      </c>
+      <c r="C179" t="s">
+        <v>32</v>
+      </c>
+      <c r="D179" t="s">
+        <v>468</v>
+      </c>
+      <c r="E179" t="s">
+        <v>24</v>
+      </c>
+      <c r="F179" t="s">
+        <v>434</v>
+      </c>
+      <c r="L179" t="s">
+        <v>470</v>
+      </c>
+      <c r="M179" t="s">
+        <v>70</v>
+      </c>
+      <c r="N179" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+      </c>
+      <c r="B180" t="s">
+        <v>31</v>
+      </c>
+      <c r="C180" t="s">
+        <v>32</v>
+      </c>
+      <c r="D180" t="s">
+        <v>468</v>
+      </c>
+      <c r="E180" t="s">
+        <v>28</v>
+      </c>
+      <c r="F180" t="s">
+        <v>305</v>
+      </c>
+      <c r="L180" t="s">
+        <v>470</v>
+      </c>
+      <c r="M180" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6244,16 +6298,16 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.625" customWidth="1"/>
+    <col min="3" max="3" width="45.625" customWidth="1"/>
+    <col min="4" max="4" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>404</v>
       </c>
@@ -6264,7 +6318,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>419</v>
       </c>
@@ -6281,7 +6335,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>420</v>
       </c>
@@ -6298,7 +6352,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -6315,7 +6369,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>224</v>
       </c>
@@ -6332,7 +6386,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>225</v>
       </c>
@@ -6346,7 +6400,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>306</v>
       </c>
@@ -6363,7 +6417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>307</v>
       </c>
@@ -6380,7 +6434,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>308</v>
       </c>
@@ -6397,7 +6451,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>309</v>
       </c>
@@ -6411,7 +6465,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>310</v>
       </c>
@@ -6428,7 +6482,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>311</v>
       </c>
@@ -6445,7 +6499,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>312</v>
       </c>
@@ -6462,7 +6516,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>313</v>
       </c>
@@ -6479,7 +6533,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>314</v>
       </c>
@@ -6496,7 +6550,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>315</v>
       </c>
@@ -6510,7 +6564,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>316</v>
       </c>
@@ -6524,7 +6578,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>317</v>
       </c>
@@ -6538,7 +6592,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>318</v>
       </c>
@@ -6552,7 +6606,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>319</v>
       </c>
@@ -6566,7 +6620,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>320</v>
       </c>
@@ -6583,7 +6637,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>321</v>
       </c>
@@ -6600,7 +6654,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>322</v>
       </c>
@@ -6617,7 +6671,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>323</v>
       </c>
@@ -6634,7 +6688,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>324</v>
       </c>
@@ -6651,7 +6705,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>325</v>
       </c>
@@ -6668,7 +6722,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>326</v>
       </c>
@@ -6685,7 +6739,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>327</v>
       </c>
@@ -6702,7 +6756,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>328</v>
       </c>
@@ -6719,7 +6773,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>329</v>
       </c>
@@ -6736,7 +6790,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>330</v>
       </c>
@@ -6753,7 +6807,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>331</v>
       </c>
@@ -6767,7 +6821,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>332</v>
       </c>
@@ -6781,7 +6835,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>333</v>
       </c>
@@ -6795,7 +6849,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>334</v>
       </c>
@@ -6809,7 +6863,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>335</v>
       </c>
@@ -6826,7 +6880,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>336</v>
       </c>
@@ -6840,7 +6894,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>337</v>
       </c>
@@ -6857,7 +6911,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>338</v>
       </c>
@@ -6874,7 +6928,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>339</v>
       </c>
@@ -6891,7 +6945,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>340</v>
       </c>
@@ -6908,7 +6962,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>341</v>
       </c>
@@ -6925,7 +6979,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>342</v>
       </c>
@@ -6942,7 +6996,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>343</v>
       </c>
@@ -6956,7 +7010,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>344</v>
       </c>
@@ -6973,7 +7027,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>345</v>
       </c>
@@ -6987,7 +7041,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>346</v>
       </c>
@@ -7001,7 +7055,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>347</v>
       </c>
@@ -7015,7 +7069,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>348</v>
       </c>
@@ -7029,7 +7083,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>349</v>
       </c>
@@ -7043,7 +7097,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>350</v>
       </c>
@@ -7057,7 +7111,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>351</v>
       </c>
@@ -7071,7 +7125,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>352</v>
       </c>
@@ -7085,7 +7139,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>353</v>
       </c>
@@ -7099,7 +7153,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>354</v>
       </c>
@@ -7113,7 +7167,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>355</v>
       </c>
@@ -7127,7 +7181,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>356</v>
       </c>
@@ -7141,7 +7195,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>357</v>
       </c>
@@ -7155,7 +7209,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>358</v>
       </c>
@@ -7172,7 +7226,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>359</v>
       </c>
@@ -7189,7 +7243,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>360</v>
       </c>
@@ -7206,7 +7260,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>361</v>
       </c>
@@ -7220,7 +7274,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>362</v>
       </c>
@@ -7234,7 +7288,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>363</v>
       </c>
@@ -7248,7 +7302,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>364</v>
       </c>
@@ -7262,7 +7316,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>365</v>
       </c>
@@ -7276,7 +7330,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>366</v>
       </c>
@@ -7290,7 +7344,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>367</v>
       </c>
@@ -7304,7 +7358,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>368</v>
       </c>
@@ -7318,7 +7372,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>369</v>
       </c>
@@ -7335,7 +7389,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>370</v>
       </c>
@@ -7352,7 +7406,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>371</v>
       </c>
@@ -7366,7 +7420,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>372</v>
       </c>
@@ -7380,7 +7434,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>373</v>
       </c>
@@ -7394,7 +7448,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>374</v>
       </c>
@@ -7408,7 +7462,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>375</v>
       </c>
@@ -7422,7 +7476,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>376</v>
       </c>
@@ -7436,7 +7490,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>377</v>
       </c>
@@ -7450,7 +7504,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>378</v>
       </c>
@@ -7464,7 +7518,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>379</v>
       </c>
@@ -7478,7 +7532,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>380</v>
       </c>
@@ -7492,7 +7546,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>381</v>
       </c>
@@ -7509,7 +7563,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>382</v>
       </c>
@@ -7526,7 +7580,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>383</v>
       </c>
@@ -7543,7 +7597,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>384</v>
       </c>
@@ -7560,7 +7614,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>385</v>
       </c>
@@ -7577,7 +7631,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>386</v>
       </c>
@@ -7594,7 +7648,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>387</v>
       </c>
@@ -7611,7 +7665,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>388</v>
       </c>
@@ -7628,7 +7682,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>389</v>
       </c>
@@ -7645,7 +7699,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>390</v>
       </c>
@@ -7659,7 +7713,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>391</v>
       </c>
@@ -7673,7 +7727,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>392</v>
       </c>
@@ -7690,7 +7744,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>393</v>
       </c>
@@ -7707,7 +7761,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>394</v>
       </c>
@@ -7721,7 +7775,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>395</v>
       </c>
@@ -7738,7 +7792,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>396</v>
       </c>
@@ -7755,7 +7809,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>397</v>
       </c>
@@ -7772,7 +7826,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>398</v>
       </c>
@@ -7789,7 +7843,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>399</v>
       </c>
@@ -7806,7 +7860,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>400</v>
       </c>
@@ -7823,7 +7877,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>401</v>
       </c>
@@ -7840,7 +7894,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>402</v>
       </c>
@@ -7857,7 +7911,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>403</v>
       </c>
@@ -7874,7 +7928,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>438</v>
       </c>
@@ -7891,7 +7945,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>440</v>
       </c>
@@ -7908,7 +7962,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>441</v>
       </c>
@@ -7925,7 +7979,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>442</v>
       </c>
@@ -7956,15 +8010,15 @@
       <selection activeCell="B61" sqref="B61:C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -7978,7 +8032,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -7992,7 +8046,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -8006,7 +8060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -8020,7 +8074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -8034,7 +8088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -8048,7 +8102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -8062,7 +8116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -8076,7 +8130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -8090,7 +8144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -8104,7 +8158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -8118,7 +8172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -8132,7 +8186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -8146,7 +8200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -8160,7 +8214,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -8174,7 +8228,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -8188,7 +8242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -8202,7 +8256,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -8216,7 +8270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -8230,7 +8284,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -8244,7 +8298,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -8258,7 +8312,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -8272,7 +8326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -8286,7 +8340,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>139</v>
       </c>
@@ -8300,7 +8354,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -8314,7 +8368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -8328,7 +8382,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -8342,7 +8396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -8356,7 +8410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -8370,7 +8424,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>194</v>
       </c>
@@ -8384,7 +8438,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -8398,7 +8452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -8412,7 +8466,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -8426,7 +8480,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -8440,7 +8494,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -8454,7 +8508,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -8468,7 +8522,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -8482,7 +8536,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -8496,7 +8550,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -8510,7 +8564,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -8524,7 +8578,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -8538,7 +8592,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -8552,7 +8606,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -8566,7 +8620,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -8580,7 +8634,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -8594,7 +8648,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>160</v>
       </c>
@@ -8608,7 +8662,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>162</v>
       </c>
@@ -8622,7 +8676,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -8636,7 +8690,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -8650,7 +8704,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>165</v>
       </c>
@@ -8664,7 +8718,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>167</v>
       </c>
@@ -8678,7 +8732,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -8692,7 +8746,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -8706,7 +8760,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>173</v>
       </c>
@@ -8720,7 +8774,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>175</v>
       </c>
@@ -8734,7 +8788,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>177</v>
       </c>
@@ -8748,7 +8802,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>178</v>
       </c>
@@ -8762,7 +8816,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>180</v>
       </c>
@@ -8776,7 +8830,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -8790,7 +8844,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -8804,7 +8858,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>183</v>
       </c>
@@ -8818,7 +8872,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>185</v>
       </c>
@@ -8832,7 +8886,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>188</v>
       </c>
@@ -8846,7 +8900,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -8860,7 +8914,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
clean up dataset attributes
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\GenomicsDBWebsite\Model\lib\wdk\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0C0E5F-7C62-4F93-BDF7-DBFA2D401434}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E7C220-A1AD-4C74-BC81-0CC0D53981C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">entity_data_mapping!$A$1:$A$104</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">individuals!$A$1:$N$170</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">individuals!$A$1:$N$174</definedName>
     <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$130</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="491">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1535,6 +1535,12 @@
   </si>
   <si>
     <t>functional_genomics_enhancers</t>
+  </si>
+  <si>
+    <t>phenotype_list</t>
+  </si>
+  <si>
+    <t>covariate_list</t>
   </si>
 </sst>
 </file>
@@ -1873,13 +1879,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N170"/>
+  <dimension ref="A1:N174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O60" sqref="O60"/>
+      <selection pane="bottomRight" activeCell="N154" sqref="N154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5399,7 +5405,7 @@
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="str">
-        <f t="shared" ref="A150:A157" si="25">CONCATENATE(D150,".",F150)</f>
+        <f t="shared" ref="A150:A159" si="25">CONCATENATE(D150,".",F150)</f>
         <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
       </c>
       <c r="B150" t="s">
@@ -5481,64 +5487,70 @@
         <v>70</v>
       </c>
     </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="str">
+        <f t="shared" ref="A153:A154" si="27">CONCATENATE(D153,".",F153)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotype_list</v>
+      </c>
+      <c r="B153" t="s">
+        <v>31</v>
+      </c>
+      <c r="C153" t="s">
+        <v>32</v>
+      </c>
+      <c r="D153" t="s">
+        <v>450</v>
+      </c>
+      <c r="E153" t="s">
+        <v>24</v>
+      </c>
+      <c r="F153" t="s">
+        <v>489</v>
+      </c>
+      <c r="L153" t="s">
+        <v>27</v>
+      </c>
+      <c r="M153" t="s">
+        <v>70</v>
+      </c>
+      <c r="N153" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="str">
-        <f>CONCATENATE(D154,".",F154)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
+        <f t="shared" si="27"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.covariate_list</v>
       </c>
       <c r="B154" t="s">
-        <v>456</v>
+        <v>31</v>
       </c>
       <c r="C154" t="s">
-        <v>156</v>
+        <v>32</v>
       </c>
       <c r="D154" t="s">
         <v>450</v>
       </c>
       <c r="E154" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F154" t="s">
-        <v>452</v>
-      </c>
-      <c r="K154">
-        <v>1</v>
+        <v>490</v>
+      </c>
+      <c r="L154" t="s">
+        <v>27</v>
       </c>
       <c r="M154" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="str">
-        <f t="shared" si="25"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
-      </c>
-      <c r="B155" t="s">
-        <v>456</v>
-      </c>
-      <c r="C155" t="s">
-        <v>156</v>
-      </c>
-      <c r="D155" t="s">
-        <v>450</v>
-      </c>
-      <c r="E155" t="s">
-        <v>28</v>
-      </c>
-      <c r="F155" t="s">
-        <v>455</v>
-      </c>
-      <c r="K155">
-        <v>2</v>
-      </c>
-      <c r="M155" t="s">
-        <v>70</v>
+      <c r="N154" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="str">
         <f>CONCATENATE(D156,".",F156)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
       </c>
       <c r="B156" t="s">
         <v>456</v>
@@ -5553,10 +5565,10 @@
         <v>28</v>
       </c>
       <c r="F156" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="K156">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M156" t="s">
         <v>70</v>
@@ -5565,13 +5577,13 @@
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="str">
         <f t="shared" si="25"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
       </c>
       <c r="B157" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C157" t="s">
-        <v>458</v>
+        <v>156</v>
       </c>
       <c r="D157" t="s">
         <v>450</v>
@@ -5580,10 +5592,10 @@
         <v>28</v>
       </c>
       <c r="F157" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="K157">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M157" t="s">
         <v>70</v>
@@ -5591,14 +5603,14 @@
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="str">
-        <f t="shared" ref="A158:A159" si="27">CONCATENATE(D158,".",F158)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
+        <f>CONCATENATE(D158,".",F158)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
       </c>
       <c r="B158" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C158" t="s">
-        <v>458</v>
+        <v>156</v>
       </c>
       <c r="D158" t="s">
         <v>450</v>
@@ -5607,7 +5619,7 @@
         <v>28</v>
       </c>
       <c r="F158" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="K158">
         <v>3</v>
@@ -5618,8 +5630,8 @@
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="str">
-        <f t="shared" si="27"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
       </c>
       <c r="B159" t="s">
         <v>457</v>
@@ -5634,10 +5646,10 @@
         <v>28</v>
       </c>
       <c r="F159" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="K159">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M159" t="s">
         <v>70</v>
@@ -5645,8 +5657,8 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="str">
-        <f t="shared" ref="A160" si="28">CONCATENATE(D160,".",F160)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
+        <f t="shared" ref="A160:A161" si="28">CONCATENATE(D160,".",F160)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
       </c>
       <c r="B160" t="s">
         <v>457</v>
@@ -5661,10 +5673,10 @@
         <v>28</v>
       </c>
       <c r="F160" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K160">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M160" t="s">
         <v>70</v>
@@ -5672,14 +5684,14 @@
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="str">
-        <f t="shared" ref="A161:A162" si="29">CONCATENATE(D161,".",F161)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+        <f t="shared" si="28"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
       </c>
       <c r="B161" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C161" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D161" t="s">
         <v>450</v>
@@ -5688,10 +5700,10 @@
         <v>28</v>
       </c>
       <c r="F161" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="K161">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M161" t="s">
         <v>70</v>
@@ -5699,14 +5711,14 @@
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="str">
-        <f t="shared" si="29"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
+        <f t="shared" ref="A162" si="29">CONCATENATE(D162,".",F162)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
       </c>
       <c r="B162" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C162" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D162" t="s">
         <v>450</v>
@@ -5715,10 +5727,10 @@
         <v>28</v>
       </c>
       <c r="F162" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="K162">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M162" t="s">
         <v>70</v>
@@ -5726,14 +5738,14 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="str">
-        <f>CONCATENATE(D163,".",F163)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
+        <f t="shared" ref="A163:A164" si="30">CONCATENATE(D163,".",F163)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
       </c>
       <c r="B163" t="s">
-        <v>57</v>
+        <v>459</v>
       </c>
       <c r="C163" t="s">
-        <v>69</v>
+        <v>460</v>
       </c>
       <c r="D163" t="s">
         <v>450</v>
@@ -5742,25 +5754,25 @@
         <v>28</v>
       </c>
       <c r="F163" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="K163">
         <v>2</v>
       </c>
       <c r="M163" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="str">
-        <f>CONCATENATE(D164,".",F164)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+        <f t="shared" si="30"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
       </c>
       <c r="B164" t="s">
-        <v>31</v>
+        <v>459</v>
       </c>
       <c r="C164" t="s">
-        <v>32</v>
+        <v>460</v>
       </c>
       <c r="D164" t="s">
         <v>450</v>
@@ -5769,16 +5781,46 @@
         <v>28</v>
       </c>
       <c r="F164" t="s">
-        <v>467</v>
+        <v>466</v>
+      </c>
+      <c r="K164">
+        <v>1</v>
       </c>
       <c r="M164" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="str">
+        <f>CONCATENATE(D165,".",F165)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
+      </c>
+      <c r="B165" t="s">
+        <v>57</v>
+      </c>
+      <c r="C165" t="s">
+        <v>69</v>
+      </c>
+      <c r="D165" t="s">
+        <v>450</v>
+      </c>
+      <c r="E165" t="s">
+        <v>28</v>
+      </c>
+      <c r="F165" t="s">
+        <v>464</v>
+      </c>
+      <c r="K165">
+        <v>2</v>
+      </c>
+      <c r="M165" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="str">
         <f>CONCATENATE(D166,".",F166)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
       </c>
       <c r="B166" t="s">
         <v>31</v>
@@ -5787,118 +5829,22 @@
         <v>32</v>
       </c>
       <c r="D166" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="E166" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F166" t="s">
-        <v>3</v>
-      </c>
-      <c r="L166" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="M166" t="s">
-        <v>70</v>
-      </c>
-      <c r="N166" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="str">
-        <f t="shared" ref="A167:A170" si="30">CONCATENATE(D167,".",F167)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
-      </c>
-      <c r="B167" t="s">
-        <v>31</v>
-      </c>
-      <c r="C167" t="s">
-        <v>32</v>
-      </c>
-      <c r="D167" t="s">
-        <v>468</v>
-      </c>
-      <c r="E167" t="s">
-        <v>24</v>
-      </c>
-      <c r="F167" t="s">
-        <v>6</v>
-      </c>
-      <c r="L167" t="s">
-        <v>470</v>
-      </c>
-      <c r="M167" t="s">
-        <v>70</v>
-      </c>
-      <c r="N167" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A168" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
-      </c>
-      <c r="B168" t="s">
-        <v>31</v>
-      </c>
-      <c r="C168" t="s">
-        <v>32</v>
-      </c>
-      <c r="D168" t="s">
-        <v>468</v>
-      </c>
-      <c r="E168" t="s">
-        <v>24</v>
-      </c>
-      <c r="F168" t="s">
-        <v>469</v>
-      </c>
-      <c r="L168" t="s">
-        <v>470</v>
-      </c>
-      <c r="M168" t="s">
-        <v>70</v>
-      </c>
-      <c r="N168" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A169" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
-      </c>
-      <c r="B169" t="s">
-        <v>31</v>
-      </c>
-      <c r="C169" t="s">
-        <v>32</v>
-      </c>
-      <c r="D169" t="s">
-        <v>468</v>
-      </c>
-      <c r="E169" t="s">
-        <v>24</v>
-      </c>
-      <c r="F169" t="s">
-        <v>434</v>
-      </c>
-      <c r="L169" t="s">
-        <v>470</v>
-      </c>
-      <c r="M169" t="s">
-        <v>70</v>
-      </c>
-      <c r="N169" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+        <f>CONCATENATE(D170,".",F170)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
       </c>
       <c r="B170" t="s">
         <v>31</v>
@@ -5910,15 +5856,135 @@
         <v>468</v>
       </c>
       <c r="E170" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F170" t="s">
-        <v>305</v>
+        <v>3</v>
       </c>
       <c r="L170" t="s">
         <v>470</v>
       </c>
       <c r="M170" t="s">
+        <v>70</v>
+      </c>
+      <c r="N170" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="str">
+        <f t="shared" ref="A171:A174" si="31">CONCATENATE(D171,".",F171)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
+      </c>
+      <c r="B171" t="s">
+        <v>31</v>
+      </c>
+      <c r="C171" t="s">
+        <v>32</v>
+      </c>
+      <c r="D171" t="s">
+        <v>468</v>
+      </c>
+      <c r="E171" t="s">
+        <v>24</v>
+      </c>
+      <c r="F171" t="s">
+        <v>6</v>
+      </c>
+      <c r="L171" t="s">
+        <v>470</v>
+      </c>
+      <c r="M171" t="s">
+        <v>70</v>
+      </c>
+      <c r="N171" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
+      </c>
+      <c r="B172" t="s">
+        <v>31</v>
+      </c>
+      <c r="C172" t="s">
+        <v>32</v>
+      </c>
+      <c r="D172" t="s">
+        <v>468</v>
+      </c>
+      <c r="E172" t="s">
+        <v>24</v>
+      </c>
+      <c r="F172" t="s">
+        <v>469</v>
+      </c>
+      <c r="L172" t="s">
+        <v>470</v>
+      </c>
+      <c r="M172" t="s">
+        <v>70</v>
+      </c>
+      <c r="N172" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+      </c>
+      <c r="B173" t="s">
+        <v>31</v>
+      </c>
+      <c r="C173" t="s">
+        <v>32</v>
+      </c>
+      <c r="D173" t="s">
+        <v>468</v>
+      </c>
+      <c r="E173" t="s">
+        <v>24</v>
+      </c>
+      <c r="F173" t="s">
+        <v>434</v>
+      </c>
+      <c r="L173" t="s">
+        <v>470</v>
+      </c>
+      <c r="M173" t="s">
+        <v>70</v>
+      </c>
+      <c r="N173" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+      </c>
+      <c r="B174" t="s">
+        <v>31</v>
+      </c>
+      <c r="C174" t="s">
+        <v>32</v>
+      </c>
+      <c r="D174" t="s">
+        <v>468</v>
+      </c>
+      <c r="E174" t="s">
+        <v>28</v>
+      </c>
+      <c r="F174" t="s">
+        <v>305</v>
+      </c>
+      <c r="L174" t="s">
+        <v>470</v>
+      </c>
+      <c r="M174" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished tables / updates to dataset record
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\GenomicsDBWebsite\Model\lib\wdk\ontology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenem\wsl-share\GenomicsDBWebsite\Model\lib\wdk\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E7C220-A1AD-4C74-BC81-0CC0D53981C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DEBF3F-F99B-4C75-92EA-205A7BB161F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="6" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">entity_data_mapping!$A$1:$A$104</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">individuals!$A$1:$N$174</definedName>
-    <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">individuals!$A$1:$N$176</definedName>
+    <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{F48A47E3-6C12-0846-9751-7C223C6867EC}" name="individuals" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{F48A47E3-6C12-0846-9751-7C223C6867EC}" name="individuals" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
     <textPr sourceFile="/www/genomics/project_home/NiagadsSite/Model/lib/wdk/ontology/individuals.txt">
       <textFields count="14">
         <textField/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="495">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1348,9 +1348,6 @@
     <t>VariantQuestions.GWAS</t>
   </si>
   <si>
-    <t>DatasetRecordClasses.ResourceRecordClass</t>
-  </si>
-  <si>
     <t>DatasetRecordClasses.DatasetRecordClass</t>
   </si>
   <si>
@@ -1363,15 +1360,9 @@
     <t>attribution</t>
   </si>
   <si>
-    <t>version</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
-    <t>caveats</t>
-  </si>
-  <si>
     <t>is_adsp</t>
   </si>
   <si>
@@ -1408,15 +1399,6 @@
     <t>question</t>
   </si>
   <si>
-    <t>## Resource Attributes ##</t>
-  </si>
-  <si>
-    <t>## Resource Questions  ##</t>
-  </si>
-  <si>
-    <t>ResourceQuestions.GWAS</t>
-  </si>
-  <si>
     <t>## GWAS Dataset Attributes ##</t>
   </si>
   <si>
@@ -1541,6 +1523,36 @@
   </si>
   <si>
     <t>covariate_list</t>
+  </si>
+  <si>
+    <t>## Dataset Questions  ##</t>
+  </si>
+  <si>
+    <t>## Dataset Attributes ##</t>
+  </si>
+  <si>
+    <t>gwas</t>
+  </si>
+  <si>
+    <t>rare_variants</t>
+  </si>
+  <si>
+    <t>gene_risk</t>
+  </si>
+  <si>
+    <t>ontology</t>
+  </si>
+  <si>
+    <t>gene_annotation</t>
+  </si>
+  <si>
+    <t>sequence_annotation</t>
+  </si>
+  <si>
+    <t>variant_annotation</t>
+  </si>
+  <si>
+    <t>gene_function</t>
   </si>
 </sst>
 </file>
@@ -1879,13 +1891,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N174"/>
+  <dimension ref="A1:N176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N154" sqref="N154"/>
+      <selection pane="bottomRight" activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2437,7 +2449,7 @@
         <v>24</v>
       </c>
       <c r="F27" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="J27" t="s">
         <v>66</v>
@@ -2467,7 +2479,7 @@
         <v>24</v>
       </c>
       <c r="F28" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="J28" t="s">
         <v>66</v>
@@ -3217,7 +3229,7 @@
         <v>33</v>
       </c>
       <c r="C54" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D54" t="s">
         <v>64</v>
@@ -3250,7 +3262,7 @@
         <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D55" t="s">
         <v>64</v>
@@ -3259,7 +3271,7 @@
         <v>28</v>
       </c>
       <c r="F55" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="J55" t="s">
         <v>66</v>
@@ -3283,7 +3295,7 @@
         <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D56" t="s">
         <v>64</v>
@@ -3292,7 +3304,7 @@
         <v>28</v>
       </c>
       <c r="F56" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="J56" t="s">
         <v>66</v>
@@ -3316,7 +3328,7 @@
         <v>33</v>
       </c>
       <c r="C57" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D57" t="s">
         <v>64</v>
@@ -3325,7 +3337,7 @@
         <v>28</v>
       </c>
       <c r="F57" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="J57" t="s">
         <v>66</v>
@@ -3349,7 +3361,7 @@
         <v>33</v>
       </c>
       <c r="C58" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D58" t="s">
         <v>64</v>
@@ -3358,7 +3370,7 @@
         <v>28</v>
       </c>
       <c r="F58" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="J58" t="s">
         <v>66</v>
@@ -3391,7 +3403,7 @@
         <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="J59" t="s">
         <v>66</v>
@@ -3418,7 +3430,7 @@
         <v>28</v>
       </c>
       <c r="F60" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="J60" t="s">
         <v>66</v>
@@ -3453,7 +3465,7 @@
         <v>21</v>
       </c>
       <c r="F64" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="L64" t="s">
         <v>22</v>
@@ -3480,7 +3492,7 @@
         <v>21</v>
       </c>
       <c r="F65" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="L65" t="s">
         <v>22</v>
@@ -3507,7 +3519,7 @@
         <v>21</v>
       </c>
       <c r="F66" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="L66" t="s">
         <v>22</v>
@@ -3827,7 +3839,7 @@
         <v>24</v>
       </c>
       <c r="F80" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="M80" t="s">
         <v>70</v>
@@ -3914,7 +3926,7 @@
         <v>24</v>
       </c>
       <c r="F83" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="L83" t="s">
         <v>27</v>
@@ -4391,7 +4403,7 @@
         <v>24</v>
       </c>
       <c r="F102" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="M102" t="s">
         <v>70</v>
@@ -4751,7 +4763,7 @@
         <v>28</v>
       </c>
       <c r="F119" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="K119">
         <v>3</v>
@@ -4915,46 +4927,49 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="str">
-        <f>CONCATENATE(D128,".",F128)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.ResourceQuestions.GWAS</v>
-      </c>
-      <c r="B128" t="s">
-        <v>57</v>
-      </c>
-      <c r="C128" t="s">
-        <v>69</v>
-      </c>
-      <c r="D128" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="str">
+        <f t="shared" ref="A131" si="15">CONCATENATE(D131,".",F131)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.name</v>
+      </c>
+      <c r="B131" t="s">
+        <v>31</v>
+      </c>
+      <c r="C131" t="s">
+        <v>32</v>
+      </c>
+      <c r="D131" t="s">
         <v>426</v>
       </c>
-      <c r="E128" t="s">
-        <v>21</v>
-      </c>
-      <c r="F128" t="s">
-        <v>448</v>
-      </c>
-      <c r="L128" t="s">
-        <v>22</v>
-      </c>
-      <c r="M128" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="129" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>446</v>
+      <c r="E131" t="s">
+        <v>24</v>
+      </c>
+      <c r="F131" t="s">
+        <v>3</v>
+      </c>
+      <c r="K131">
+        <v>1</v>
+      </c>
+      <c r="M131" t="s">
+        <v>25</v>
+      </c>
+      <c r="N131" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="str">
-        <f t="shared" ref="A132" si="15">CONCATENATE(D132,".",F132)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.name</v>
+        <f t="shared" ref="A132" si="16">CONCATENATE(D132,".",F132)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.description</v>
       </c>
       <c r="B132" t="s">
         <v>31</v>
@@ -4969,13 +4984,10 @@
         <v>24</v>
       </c>
       <c r="F132" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K132">
-        <v>1</v>
-      </c>
-      <c r="L132" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="M132" t="s">
         <v>25</v>
@@ -4986,8 +4998,8 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="str">
-        <f t="shared" ref="A133" si="16">CONCATENATE(D133,".",F133)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.description</v>
+        <f t="shared" ref="A133" si="17">CONCATENATE(D133,".",F133)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.attribution</v>
       </c>
       <c r="B133" t="s">
         <v>31</v>
@@ -5002,13 +5014,10 @@
         <v>24</v>
       </c>
       <c r="F133" t="s">
-        <v>6</v>
+        <v>429</v>
       </c>
       <c r="K133">
-        <v>4</v>
-      </c>
-      <c r="L133" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="M133" t="s">
         <v>25</v>
@@ -5019,29 +5028,26 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="str">
-        <f t="shared" ref="A134" si="17">CONCATENATE(D134,".",F134)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.attribution</v>
+        <f t="shared" ref="A134" si="18">CONCATENATE(D134,".",F134)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.gwas</v>
       </c>
       <c r="B134" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C134" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D134" t="s">
         <v>426</v>
       </c>
       <c r="E134" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F134" t="s">
-        <v>430</v>
+        <v>487</v>
       </c>
       <c r="K134">
-        <v>3</v>
-      </c>
-      <c r="L134" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="M134" t="s">
         <v>25</v>
@@ -5052,29 +5058,26 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="str">
-        <f t="shared" ref="A135" si="18">CONCATENATE(D135,".",F135)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.version</v>
+        <f t="shared" ref="A135" si="19">CONCATENATE(D135,".",F135)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.rare_variants</v>
       </c>
       <c r="B135" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C135" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D135" t="s">
         <v>426</v>
       </c>
       <c r="E135" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F135" t="s">
-        <v>431</v>
+        <v>488</v>
       </c>
       <c r="K135">
-        <v>5</v>
-      </c>
-      <c r="L135" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="M135" t="s">
         <v>25</v>
@@ -5085,29 +5088,26 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="str">
-        <f t="shared" ref="A136" si="19">CONCATENATE(D136,".",F136)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.category</v>
+        <f t="shared" ref="A136" si="20">CONCATENATE(D136,".",F136)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.gene_risk</v>
       </c>
       <c r="B136" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C136" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D136" t="s">
         <v>426</v>
       </c>
       <c r="E136" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F136" t="s">
-        <v>432</v>
+        <v>489</v>
       </c>
       <c r="K136">
-        <v>6</v>
-      </c>
-      <c r="L136" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="M136" t="s">
         <v>25</v>
@@ -5118,8 +5118,8 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="str">
-        <f t="shared" ref="A137:A138" si="20">CONCATENATE(D137,".",F137)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.caveats</v>
+        <f t="shared" ref="A137" si="21">CONCATENATE(D137,".",F137)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.ontology</v>
       </c>
       <c r="B137" t="s">
         <v>31</v>
@@ -5131,22 +5131,25 @@
         <v>426</v>
       </c>
       <c r="E137" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F137" t="s">
-        <v>433</v>
+        <v>490</v>
       </c>
       <c r="K137">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M137" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="N137" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>DatasetRecordClasses.ResourceRecordClass.is_adsp</v>
+        <f t="shared" ref="A138" si="22">CONCATENATE(D138,".",F138)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.gene_annotation</v>
       </c>
       <c r="B138" t="s">
         <v>31</v>
@@ -5158,13 +5161,13 @@
         <v>426</v>
       </c>
       <c r="E138" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F138" t="s">
-        <v>434</v>
-      </c>
-      <c r="L138" t="s">
-        <v>27</v>
+        <v>491</v>
+      </c>
+      <c r="K138">
+        <v>3</v>
       </c>
       <c r="M138" t="s">
         <v>25</v>
@@ -5175,8 +5178,8 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="str">
-        <f t="shared" ref="A139" si="21">CONCATENATE(D139,".",F139)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.accession_link</v>
+        <f t="shared" ref="A139" si="23">CONCATENATE(D139,".",F139)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.sequence_annotation</v>
       </c>
       <c r="B139" t="s">
         <v>31</v>
@@ -5188,13 +5191,13 @@
         <v>426</v>
       </c>
       <c r="E139" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F139" t="s">
-        <v>429</v>
-      </c>
-      <c r="L139" t="s">
-        <v>27</v>
+        <v>492</v>
+      </c>
+      <c r="K139">
+        <v>3</v>
       </c>
       <c r="M139" t="s">
         <v>25</v>
@@ -5205,14 +5208,14 @@
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="str">
-        <f t="shared" ref="A140" si="22">CONCATENATE(D140,".",F140)</f>
-        <v>DatasetRecordClasses.ResourceRecordClass.datasets</v>
+        <f t="shared" ref="A140" si="24">CONCATENATE(D140,".",F140)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.variant_annotation</v>
       </c>
       <c r="B140" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C140" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D140" t="s">
         <v>426</v>
@@ -5221,10 +5224,10 @@
         <v>28</v>
       </c>
       <c r="F140" t="s">
-        <v>305</v>
+        <v>493</v>
       </c>
       <c r="K140">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M140" t="s">
         <v>25</v>
@@ -5233,72 +5236,45 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>449</v>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="str">
+        <f t="shared" ref="A141" si="25">CONCATENATE(D141,".",F141)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.gene_function</v>
+      </c>
+      <c r="B141" t="s">
+        <v>44</v>
+      </c>
+      <c r="C141" t="s">
+        <v>45</v>
+      </c>
+      <c r="D141" t="s">
+        <v>426</v>
+      </c>
+      <c r="E141" t="s">
+        <v>28</v>
+      </c>
+      <c r="F141" t="s">
+        <v>494</v>
+      </c>
+      <c r="K141">
+        <v>3</v>
+      </c>
+      <c r="M141" t="s">
+        <v>25</v>
+      </c>
+      <c r="N141" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="str">
-        <f t="shared" ref="A144:A148" si="23">CONCATENATE(D144,".",F144)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
-      </c>
-      <c r="B144" t="s">
-        <v>31</v>
-      </c>
-      <c r="C144" t="s">
-        <v>32</v>
-      </c>
-      <c r="D144" t="s">
-        <v>450</v>
-      </c>
-      <c r="E144" t="s">
-        <v>24</v>
-      </c>
-      <c r="F144" t="s">
-        <v>3</v>
-      </c>
-      <c r="M144" t="s">
-        <v>70</v>
-      </c>
-      <c r="N144" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="str">
-        <f t="shared" si="23"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
-      </c>
-      <c r="B145" t="s">
-        <v>31</v>
-      </c>
-      <c r="C145" t="s">
-        <v>32</v>
-      </c>
-      <c r="D145" t="s">
-        <v>450</v>
-      </c>
-      <c r="E145" t="s">
-        <v>24</v>
-      </c>
-      <c r="F145" t="s">
-        <v>6</v>
-      </c>
-      <c r="L145" t="s">
-        <v>27</v>
-      </c>
-      <c r="M145" t="s">
-        <v>70</v>
-      </c>
-      <c r="N145" t="s">
-        <v>26</v>
+      <c r="A144" s="2" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="str">
-        <f t="shared" si="23"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
+        <f t="shared" ref="A146:A150" si="26">CONCATENATE(D146,".",F146)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
       </c>
       <c r="B146" t="s">
         <v>31</v>
@@ -5307,22 +5283,25 @@
         <v>32</v>
       </c>
       <c r="D146" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E146" t="s">
         <v>24</v>
       </c>
       <c r="F146" t="s">
-        <v>432</v>
+        <v>3</v>
       </c>
       <c r="M146" t="s">
         <v>70</v>
+      </c>
+      <c r="N146" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="str">
-        <f t="shared" si="23"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
+        <f t="shared" si="26"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
       </c>
       <c r="B147" t="s">
         <v>31</v>
@@ -5331,13 +5310,13 @@
         <v>32</v>
       </c>
       <c r="D147" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E147" t="s">
         <v>24</v>
       </c>
       <c r="F147" t="s">
-        <v>434</v>
+        <v>6</v>
       </c>
       <c r="L147" t="s">
         <v>27</v>
@@ -5351,8 +5330,8 @@
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="str">
-        <f t="shared" si="23"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
+        <f t="shared" si="26"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
       </c>
       <c r="B148" t="s">
         <v>31</v>
@@ -5361,16 +5340,13 @@
         <v>32</v>
       </c>
       <c r="D148" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E148" t="s">
         <v>24</v>
       </c>
       <c r="F148" t="s">
-        <v>429</v>
-      </c>
-      <c r="L148" t="s">
-        <v>27</v>
+        <v>430</v>
       </c>
       <c r="M148" t="s">
         <v>70</v>
@@ -5378,8 +5354,8 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="str">
-        <f t="shared" ref="A149" si="24">CONCATENATE(D149,".",F149)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.niagads_accession</v>
+        <f t="shared" si="26"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
       </c>
       <c r="B149" t="s">
         <v>31</v>
@@ -5388,13 +5364,16 @@
         <v>32</v>
       </c>
       <c r="D149" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E149" t="s">
         <v>24</v>
       </c>
       <c r="F149" t="s">
-        <v>479</v>
+        <v>431</v>
+      </c>
+      <c r="L149" t="s">
+        <v>27</v>
       </c>
       <c r="M149" t="s">
         <v>70</v>
@@ -5405,8 +5384,8 @@
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="str">
-        <f t="shared" ref="A150:A159" si="25">CONCATENATE(D150,".",F150)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
+        <f t="shared" si="26"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
       </c>
       <c r="B150" t="s">
         <v>31</v>
@@ -5415,13 +5394,13 @@
         <v>32</v>
       </c>
       <c r="D150" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E150" t="s">
         <v>24</v>
       </c>
       <c r="F150" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="L150" t="s">
         <v>27</v>
@@ -5432,8 +5411,8 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="str">
-        <f t="shared" ref="A151" si="26">CONCATENATE(D151,".",F151)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.attribution</v>
+        <f t="shared" ref="A151" si="27">CONCATENATE(D151,".",F151)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.niagads_accession</v>
       </c>
       <c r="B151" t="s">
         <v>31</v>
@@ -5442,16 +5421,13 @@
         <v>32</v>
       </c>
       <c r="D151" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
       </c>
       <c r="F151" t="s">
-        <v>430</v>
-      </c>
-      <c r="L151" t="s">
-        <v>27</v>
+        <v>473</v>
       </c>
       <c r="M151" t="s">
         <v>70</v>
@@ -5462,26 +5438,26 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="str">
-        <f>CONCATENATE(D152,".",F152)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.has_manhattan_plot</v>
+        <f t="shared" ref="A152:A161" si="28">CONCATENATE(D152,".",F152)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
       </c>
       <c r="B152" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C152" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D152" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E152" t="s">
         <v>24</v>
       </c>
       <c r="F152" t="s">
-        <v>482</v>
-      </c>
-      <c r="K152">
-        <v>1</v>
+        <v>445</v>
+      </c>
+      <c r="L152" t="s">
+        <v>27</v>
       </c>
       <c r="M152" t="s">
         <v>70</v>
@@ -5489,8 +5465,8 @@
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="str">
-        <f t="shared" ref="A153:A154" si="27">CONCATENATE(D153,".",F153)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotype_list</v>
+        <f t="shared" ref="A153" si="29">CONCATENATE(D153,".",F153)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.attribution</v>
       </c>
       <c r="B153" t="s">
         <v>31</v>
@@ -5499,13 +5475,13 @@
         <v>32</v>
       </c>
       <c r="D153" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E153" t="s">
         <v>24</v>
       </c>
       <c r="F153" t="s">
-        <v>489</v>
+        <v>429</v>
       </c>
       <c r="L153" t="s">
         <v>27</v>
@@ -5519,110 +5495,113 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="str">
-        <f t="shared" si="27"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.covariate_list</v>
+        <f>CONCATENATE(D154,".",F154)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.has_manhattan_plot</v>
       </c>
       <c r="B154" t="s">
+        <v>57</v>
+      </c>
+      <c r="C154" t="s">
+        <v>69</v>
+      </c>
+      <c r="D154" t="s">
+        <v>444</v>
+      </c>
+      <c r="E154" t="s">
+        <v>24</v>
+      </c>
+      <c r="F154" t="s">
+        <v>476</v>
+      </c>
+      <c r="K154">
+        <v>1</v>
+      </c>
+      <c r="M154" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="str">
+        <f t="shared" ref="A155:A156" si="30">CONCATENATE(D155,".",F155)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotype_list</v>
+      </c>
+      <c r="B155" t="s">
         <v>31</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C155" t="s">
         <v>32</v>
       </c>
-      <c r="D154" t="s">
-        <v>450</v>
-      </c>
-      <c r="E154" t="s">
-        <v>24</v>
-      </c>
-      <c r="F154" t="s">
-        <v>490</v>
-      </c>
-      <c r="L154" t="s">
+      <c r="D155" t="s">
+        <v>444</v>
+      </c>
+      <c r="E155" t="s">
+        <v>24</v>
+      </c>
+      <c r="F155" t="s">
+        <v>483</v>
+      </c>
+      <c r="L155" t="s">
         <v>27</v>
       </c>
-      <c r="M154" t="s">
-        <v>70</v>
-      </c>
-      <c r="N154" t="s">
+      <c r="M155" t="s">
+        <v>70</v>
+      </c>
+      <c r="N155" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="str">
-        <f>CONCATENATE(D156,".",F156)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
+        <f t="shared" si="30"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.covariate_list</v>
       </c>
       <c r="B156" t="s">
-        <v>456</v>
+        <v>31</v>
       </c>
       <c r="C156" t="s">
-        <v>156</v>
+        <v>32</v>
       </c>
       <c r="D156" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E156" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F156" t="s">
-        <v>452</v>
-      </c>
-      <c r="K156">
-        <v>1</v>
+        <v>484</v>
+      </c>
+      <c r="L156" t="s">
+        <v>27</v>
       </c>
       <c r="M156" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="str">
-        <f t="shared" si="25"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
-      </c>
-      <c r="B157" t="s">
-        <v>456</v>
-      </c>
-      <c r="C157" t="s">
-        <v>156</v>
-      </c>
-      <c r="D157" t="s">
-        <v>450</v>
-      </c>
-      <c r="E157" t="s">
-        <v>28</v>
-      </c>
-      <c r="F157" t="s">
-        <v>455</v>
-      </c>
-      <c r="K157">
-        <v>2</v>
-      </c>
-      <c r="M157" t="s">
-        <v>70</v>
+      <c r="N156" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="str">
         <f>CONCATENATE(D158,".",F158)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
       </c>
       <c r="B158" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C158" t="s">
         <v>156</v>
       </c>
       <c r="D158" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E158" t="s">
         <v>28</v>
       </c>
       <c r="F158" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="K158">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M158" t="s">
         <v>70</v>
@@ -5630,26 +5609,26 @@
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="str">
-        <f t="shared" si="25"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
+        <f t="shared" si="28"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
       </c>
       <c r="B159" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C159" t="s">
-        <v>458</v>
+        <v>156</v>
       </c>
       <c r="D159" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E159" t="s">
         <v>28</v>
       </c>
       <c r="F159" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="K159">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M159" t="s">
         <v>70</v>
@@ -5657,23 +5636,23 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="str">
-        <f t="shared" ref="A160:A161" si="28">CONCATENATE(D160,".",F160)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
+        <f>CONCATENATE(D160,".",F160)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
       </c>
       <c r="B160" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C160" t="s">
-        <v>458</v>
+        <v>156</v>
       </c>
       <c r="D160" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E160" t="s">
         <v>28</v>
       </c>
       <c r="F160" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="K160">
         <v>3</v>
@@ -5685,25 +5664,25 @@
     <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="str">
         <f t="shared" si="28"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
       </c>
       <c r="B161" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="C161" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D161" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E161" t="s">
         <v>28</v>
       </c>
       <c r="F161" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="K161">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M161" t="s">
         <v>70</v>
@@ -5711,26 +5690,26 @@
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="str">
-        <f t="shared" ref="A162" si="29">CONCATENATE(D162,".",F162)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
+        <f t="shared" ref="A162:A163" si="31">CONCATENATE(D162,".",F162)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
       </c>
       <c r="B162" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="C162" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D162" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E162" t="s">
         <v>28</v>
       </c>
       <c r="F162" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="K162">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M162" t="s">
         <v>70</v>
@@ -5738,26 +5717,26 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="str">
-        <f t="shared" ref="A163:A164" si="30">CONCATENATE(D163,".",F163)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+        <f t="shared" si="31"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
       </c>
       <c r="B163" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C163" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="D163" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E163" t="s">
         <v>28</v>
       </c>
       <c r="F163" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="K163">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M163" t="s">
         <v>70</v>
@@ -5765,26 +5744,26 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
+        <f t="shared" ref="A164" si="32">CONCATENATE(D164,".",F164)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
       </c>
       <c r="B164" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C164" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="D164" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E164" t="s">
         <v>28</v>
       </c>
       <c r="F164" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="K164">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M164" t="s">
         <v>70</v>
@@ -5792,119 +5771,113 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="str">
-        <f>CONCATENATE(D165,".",F165)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
+        <f t="shared" ref="A165:A166" si="33">CONCATENATE(D165,".",F165)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
       </c>
       <c r="B165" t="s">
-        <v>57</v>
+        <v>453</v>
       </c>
       <c r="C165" t="s">
-        <v>69</v>
+        <v>454</v>
       </c>
       <c r="D165" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E165" t="s">
         <v>28</v>
       </c>
       <c r="F165" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="K165">
         <v>2</v>
       </c>
       <c r="M165" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="str">
-        <f>CONCATENATE(D166,".",F166)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+        <f t="shared" si="33"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
       </c>
       <c r="B166" t="s">
-        <v>31</v>
+        <v>453</v>
       </c>
       <c r="C166" t="s">
-        <v>32</v>
+        <v>454</v>
       </c>
       <c r="D166" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E166" t="s">
         <v>28</v>
       </c>
       <c r="F166" t="s">
-        <v>467</v>
+        <v>460</v>
+      </c>
+      <c r="K166">
+        <v>1</v>
       </c>
       <c r="M166" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="str">
+        <f>CONCATENATE(D167,".",F167)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
+      </c>
+      <c r="B167" t="s">
+        <v>57</v>
+      </c>
+      <c r="C167" t="s">
+        <v>69</v>
+      </c>
+      <c r="D167" t="s">
+        <v>444</v>
+      </c>
+      <c r="E167" t="s">
+        <v>28</v>
+      </c>
+      <c r="F167" t="s">
+        <v>458</v>
+      </c>
+      <c r="K167">
+        <v>2</v>
+      </c>
+      <c r="M167" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="str">
-        <f>CONCATENATE(D170,".",F170)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
-      </c>
-      <c r="B170" t="s">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="str">
+        <f>CONCATENATE(D168,".",F168)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
+      </c>
+      <c r="B168" t="s">
         <v>31</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C168" t="s">
         <v>32</v>
       </c>
-      <c r="D170" t="s">
-        <v>468</v>
-      </c>
-      <c r="E170" t="s">
-        <v>24</v>
-      </c>
-      <c r="F170" t="s">
-        <v>3</v>
-      </c>
-      <c r="L170" t="s">
-        <v>470</v>
-      </c>
-      <c r="M170" t="s">
-        <v>70</v>
-      </c>
-      <c r="N170" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="str">
-        <f t="shared" ref="A171:A174" si="31">CONCATENATE(D171,".",F171)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
-      </c>
-      <c r="B171" t="s">
-        <v>31</v>
-      </c>
-      <c r="C171" t="s">
-        <v>32</v>
-      </c>
-      <c r="D171" t="s">
-        <v>468</v>
-      </c>
-      <c r="E171" t="s">
-        <v>24</v>
-      </c>
-      <c r="F171" t="s">
-        <v>6</v>
-      </c>
-      <c r="L171" t="s">
-        <v>470</v>
-      </c>
-      <c r="M171" t="s">
-        <v>70</v>
-      </c>
-      <c r="N171" t="s">
-        <v>26</v>
+      <c r="D168" t="s">
+        <v>444</v>
+      </c>
+      <c r="E168" t="s">
+        <v>28</v>
+      </c>
+      <c r="F168" t="s">
+        <v>461</v>
+      </c>
+      <c r="M168" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="str">
-        <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
+        <f>CONCATENATE(D172,".",F172)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
       </c>
       <c r="B172" t="s">
         <v>31</v>
@@ -5913,16 +5886,16 @@
         <v>32</v>
       </c>
       <c r="D172" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="E172" t="s">
         <v>24</v>
       </c>
       <c r="F172" t="s">
-        <v>469</v>
+        <v>3</v>
       </c>
       <c r="L172" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="M172" t="s">
         <v>70</v>
@@ -5933,8 +5906,8 @@
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="str">
-        <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+        <f t="shared" ref="A173:A176" si="34">CONCATENATE(D173,".",F173)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
       </c>
       <c r="B173" t="s">
         <v>31</v>
@@ -5943,16 +5916,16 @@
         <v>32</v>
       </c>
       <c r="D173" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="E173" t="s">
         <v>24</v>
       </c>
       <c r="F173" t="s">
-        <v>434</v>
+        <v>6</v>
       </c>
       <c r="L173" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="M173" t="s">
         <v>70</v>
@@ -5963,8 +5936,8 @@
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="str">
-        <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+        <f t="shared" si="34"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
       </c>
       <c r="B174" t="s">
         <v>31</v>
@@ -5973,18 +5946,78 @@
         <v>32</v>
       </c>
       <c r="D174" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="E174" t="s">
+        <v>24</v>
+      </c>
+      <c r="F174" t="s">
+        <v>463</v>
+      </c>
+      <c r="L174" t="s">
+        <v>464</v>
+      </c>
+      <c r="M174" t="s">
+        <v>70</v>
+      </c>
+      <c r="N174" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+      </c>
+      <c r="B175" t="s">
+        <v>31</v>
+      </c>
+      <c r="C175" t="s">
+        <v>32</v>
+      </c>
+      <c r="D175" t="s">
+        <v>462</v>
+      </c>
+      <c r="E175" t="s">
+        <v>24</v>
+      </c>
+      <c r="F175" t="s">
+        <v>431</v>
+      </c>
+      <c r="L175" t="s">
+        <v>464</v>
+      </c>
+      <c r="M175" t="s">
+        <v>70</v>
+      </c>
+      <c r="N175" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+      </c>
+      <c r="B176" t="s">
+        <v>31</v>
+      </c>
+      <c r="C176" t="s">
+        <v>32</v>
+      </c>
+      <c r="D176" t="s">
+        <v>462</v>
+      </c>
+      <c r="E176" t="s">
         <v>28</v>
       </c>
-      <c r="F174" t="s">
+      <c r="F176" t="s">
         <v>305</v>
       </c>
-      <c r="L174" t="s">
-        <v>470</v>
-      </c>
-      <c r="M174" t="s">
+      <c r="L176" t="s">
+        <v>464</v>
+      </c>
+      <c r="M176" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6016,7 +6049,7 @@
         <v>404</v>
       </c>
       <c r="B1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C1" t="s">
         <v>305</v>
@@ -6027,7 +6060,7 @@
         <v>419</v>
       </c>
       <c r="B2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C2" t="s">
         <v>405</v>
@@ -6044,7 +6077,7 @@
         <v>420</v>
       </c>
       <c r="B3" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C3" t="s">
         <v>405</v>
@@ -6061,7 +6094,7 @@
         <v>223</v>
       </c>
       <c r="B4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C4" t="s">
         <v>406</v>
@@ -6070,7 +6103,7 @@
         <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -6078,7 +6111,7 @@
         <v>224</v>
       </c>
       <c r="B5" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C5" t="s">
         <v>407</v>
@@ -6087,7 +6120,7 @@
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -6095,7 +6128,7 @@
         <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D6" t="s">
         <v>64</v>
@@ -7589,7 +7622,7 @@
         <v>28</v>
       </c>
       <c r="C102" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D102" t="s">
         <v>229</v>
@@ -7606,7 +7639,7 @@
         <v>28</v>
       </c>
       <c r="C103" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D103" t="s">
         <v>229</v>
@@ -7634,30 +7667,30 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B105" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C105" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D105" t="s">
+        <v>426</v>
+      </c>
+      <c r="E105" t="s">
         <v>427</v>
-      </c>
-      <c r="E105" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>437</v>
+      </c>
+      <c r="B106" t="s">
+        <v>442</v>
+      </c>
+      <c r="C106" t="s">
         <v>440</v>
-      </c>
-      <c r="B106" t="s">
-        <v>445</v>
-      </c>
-      <c r="C106" t="s">
-        <v>443</v>
       </c>
       <c r="D106" t="s">
         <v>229</v>
@@ -7668,13 +7701,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B107" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C107" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D107" t="s">
         <v>229</v>
@@ -7685,13 +7718,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>439</v>
+      </c>
+      <c r="B108" t="s">
         <v>442</v>
       </c>
-      <c r="B108" t="s">
-        <v>445</v>
-      </c>
       <c r="C108" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D108" t="s">
         <v>229</v>

</xml_diff>

<commit_message>
wrapping up dataset/accession record
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenem\wsl-share\GenomicsDBWebsite\Model\lib\wdk\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DEBF3F-F99B-4C75-92EA-205A7BB161F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5545A4B3-6DBC-4715-BAC8-00B2DC51C192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">entity_data_mapping!$A$1:$A$104</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">individuals!$A$1:$N$176</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">individuals!$A$1:$N$175</definedName>
     <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="495">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1891,13 +1891,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N176"/>
+  <dimension ref="A1:N175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C132" sqref="C132"/>
+      <selection pane="bottomRight" activeCell="A133" sqref="A133:XFD133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4960,7 +4960,7 @@
         <v>1</v>
       </c>
       <c r="M131" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="N131" t="s">
         <v>26</v>
@@ -4990,7 +4990,7 @@
         <v>4</v>
       </c>
       <c r="M132" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="N132" t="s">
         <v>26</v>
@@ -4999,25 +4999,25 @@
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="str">
         <f t="shared" ref="A133" si="17">CONCATENATE(D133,".",F133)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.attribution</v>
+        <v>DatasetRecordClasses.DatasetRecordClass.gwas</v>
       </c>
       <c r="B133" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C133" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D133" t="s">
         <v>426</v>
       </c>
       <c r="E133" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F133" t="s">
-        <v>429</v>
+        <v>487</v>
       </c>
       <c r="K133">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M133" t="s">
         <v>25</v>
@@ -5029,7 +5029,7 @@
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="str">
         <f t="shared" ref="A134" si="18">CONCATENATE(D134,".",F134)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.gwas</v>
+        <v>DatasetRecordClasses.DatasetRecordClass.rare_variants</v>
       </c>
       <c r="B134" t="s">
         <v>57</v>
@@ -5044,10 +5044,10 @@
         <v>28</v>
       </c>
       <c r="F134" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="K134">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M134" t="s">
         <v>25</v>
@@ -5059,7 +5059,7 @@
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="str">
         <f t="shared" ref="A135" si="19">CONCATENATE(D135,".",F135)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.rare_variants</v>
+        <v>DatasetRecordClasses.DatasetRecordClass.gene_risk</v>
       </c>
       <c r="B135" t="s">
         <v>57</v>
@@ -5074,10 +5074,10 @@
         <v>28</v>
       </c>
       <c r="F135" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="K135">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M135" t="s">
         <v>25</v>
@@ -5089,13 +5089,13 @@
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="str">
         <f t="shared" ref="A136" si="20">CONCATENATE(D136,".",F136)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.gene_risk</v>
+        <v>DatasetRecordClasses.DatasetRecordClass.ontology</v>
       </c>
       <c r="B136" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D136" t="s">
         <v>426</v>
@@ -5104,7 +5104,7 @@
         <v>28</v>
       </c>
       <c r="F136" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="K136">
         <v>3</v>
@@ -5119,7 +5119,7 @@
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="str">
         <f t="shared" ref="A137" si="21">CONCATENATE(D137,".",F137)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.ontology</v>
+        <v>DatasetRecordClasses.DatasetRecordClass.gene_annotation</v>
       </c>
       <c r="B137" t="s">
         <v>31</v>
@@ -5134,7 +5134,7 @@
         <v>28</v>
       </c>
       <c r="F137" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="K137">
         <v>3</v>
@@ -5149,7 +5149,7 @@
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="str">
         <f t="shared" ref="A138" si="22">CONCATENATE(D138,".",F138)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.gene_annotation</v>
+        <v>DatasetRecordClasses.DatasetRecordClass.sequence_annotation</v>
       </c>
       <c r="B138" t="s">
         <v>31</v>
@@ -5164,7 +5164,7 @@
         <v>28</v>
       </c>
       <c r="F138" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K138">
         <v>3</v>
@@ -5179,13 +5179,13 @@
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="str">
         <f t="shared" ref="A139" si="23">CONCATENATE(D139,".",F139)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.sequence_annotation</v>
+        <v>DatasetRecordClasses.DatasetRecordClass.variant_annotation</v>
       </c>
       <c r="B139" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C139" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D139" t="s">
         <v>426</v>
@@ -5194,7 +5194,7 @@
         <v>28</v>
       </c>
       <c r="F139" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="K139">
         <v>3</v>
@@ -5209,13 +5209,13 @@
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="str">
         <f t="shared" ref="A140" si="24">CONCATENATE(D140,".",F140)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.variant_annotation</v>
+        <v>DatasetRecordClasses.DatasetRecordClass.gene_function</v>
       </c>
       <c r="B140" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C140" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D140" t="s">
         <v>426</v>
@@ -5224,7 +5224,7 @@
         <v>28</v>
       </c>
       <c r="F140" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="K140">
         <v>3</v>
@@ -5236,45 +5236,42 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="str">
-        <f t="shared" ref="A141" si="25">CONCATENATE(D141,".",F141)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.gene_function</v>
-      </c>
-      <c r="B141" t="s">
-        <v>44</v>
-      </c>
-      <c r="C141" t="s">
-        <v>45</v>
-      </c>
-      <c r="D141" t="s">
-        <v>426</v>
-      </c>
-      <c r="E141" t="s">
-        <v>28</v>
-      </c>
-      <c r="F141" t="s">
-        <v>494</v>
-      </c>
-      <c r="K141">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="str">
+        <f t="shared" ref="A145:A149" si="25">CONCATENATE(D145,".",F145)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
+      </c>
+      <c r="B145" t="s">
+        <v>31</v>
+      </c>
+      <c r="C145" t="s">
+        <v>32</v>
+      </c>
+      <c r="D145" t="s">
+        <v>444</v>
+      </c>
+      <c r="E145" t="s">
+        <v>24</v>
+      </c>
+      <c r="F145" t="s">
         <v>3</v>
       </c>
-      <c r="M141" t="s">
-        <v>25</v>
-      </c>
-      <c r="N141" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>443</v>
+      <c r="M145" t="s">
+        <v>70</v>
+      </c>
+      <c r="N145" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="str">
-        <f t="shared" ref="A146:A150" si="26">CONCATENATE(D146,".",F146)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.name</v>
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
       </c>
       <c r="B146" t="s">
         <v>31</v>
@@ -5289,7 +5286,10 @@
         <v>24</v>
       </c>
       <c r="F146" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="L146" t="s">
+        <v>27</v>
       </c>
       <c r="M146" t="s">
         <v>70</v>
@@ -5300,8 +5300,8 @@
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="str">
-        <f t="shared" si="26"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.description</v>
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
       </c>
       <c r="B147" t="s">
         <v>31</v>
@@ -5316,22 +5316,16 @@
         <v>24</v>
       </c>
       <c r="F147" t="s">
-        <v>6</v>
-      </c>
-      <c r="L147" t="s">
-        <v>27</v>
+        <v>430</v>
       </c>
       <c r="M147" t="s">
         <v>70</v>
-      </c>
-      <c r="N147" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="str">
-        <f t="shared" si="26"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.category</v>
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
       </c>
       <c r="B148" t="s">
         <v>31</v>
@@ -5346,16 +5340,22 @@
         <v>24</v>
       </c>
       <c r="F148" t="s">
-        <v>430</v>
+        <v>431</v>
+      </c>
+      <c r="L148" t="s">
+        <v>27</v>
       </c>
       <c r="M148" t="s">
         <v>70</v>
+      </c>
+      <c r="N148" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="str">
-        <f t="shared" si="26"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.is_adsp</v>
+        <f t="shared" si="25"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
       </c>
       <c r="B149" t="s">
         <v>31</v>
@@ -5370,7 +5370,7 @@
         <v>24</v>
       </c>
       <c r="F149" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="L149" t="s">
         <v>27</v>
@@ -5378,14 +5378,11 @@
       <c r="M149" t="s">
         <v>70</v>
       </c>
-      <c r="N149" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="str">
-        <f t="shared" si="26"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.accession_link</v>
+        <f t="shared" ref="A150" si="26">CONCATENATE(D150,".",F150)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.niagads_accession</v>
       </c>
       <c r="B150" t="s">
         <v>31</v>
@@ -5400,19 +5397,19 @@
         <v>24</v>
       </c>
       <c r="F150" t="s">
-        <v>428</v>
-      </c>
-      <c r="L150" t="s">
-        <v>27</v>
+        <v>473</v>
       </c>
       <c r="M150" t="s">
         <v>70</v>
+      </c>
+      <c r="N150" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="str">
-        <f t="shared" ref="A151" si="27">CONCATENATE(D151,".",F151)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.niagads_accession</v>
+        <f t="shared" ref="A151:A160" si="27">CONCATENATE(D151,".",F151)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
       </c>
       <c r="B151" t="s">
         <v>31</v>
@@ -5427,19 +5424,19 @@
         <v>24</v>
       </c>
       <c r="F151" t="s">
-        <v>473</v>
+        <v>445</v>
+      </c>
+      <c r="L151" t="s">
+        <v>27</v>
       </c>
       <c r="M151" t="s">
         <v>70</v>
-      </c>
-      <c r="N151" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="str">
-        <f t="shared" ref="A152:A161" si="28">CONCATENATE(D152,".",F152)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.search_link</v>
+        <f t="shared" ref="A152" si="28">CONCATENATE(D152,".",F152)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.attribution</v>
       </c>
       <c r="B152" t="s">
         <v>31</v>
@@ -5454,7 +5451,7 @@
         <v>24</v>
       </c>
       <c r="F152" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="L152" t="s">
         <v>27</v>
@@ -5462,17 +5459,20 @@
       <c r="M152" t="s">
         <v>70</v>
       </c>
+      <c r="N152" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="str">
-        <f t="shared" ref="A153" si="29">CONCATENATE(D153,".",F153)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.attribution</v>
+        <f>CONCATENATE(D153,".",F153)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.has_manhattan_plot</v>
       </c>
       <c r="B153" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C153" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D153" t="s">
         <v>444</v>
@@ -5481,28 +5481,25 @@
         <v>24</v>
       </c>
       <c r="F153" t="s">
-        <v>429</v>
-      </c>
-      <c r="L153" t="s">
-        <v>27</v>
+        <v>476</v>
+      </c>
+      <c r="K153">
+        <v>1</v>
       </c>
       <c r="M153" t="s">
         <v>70</v>
-      </c>
-      <c r="N153" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="str">
-        <f>CONCATENATE(D154,".",F154)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.has_manhattan_plot</v>
+        <f t="shared" ref="A154:A155" si="29">CONCATENATE(D154,".",F154)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotype_list</v>
       </c>
       <c r="B154" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C154" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D154" t="s">
         <v>444</v>
@@ -5511,19 +5508,22 @@
         <v>24</v>
       </c>
       <c r="F154" t="s">
-        <v>476</v>
-      </c>
-      <c r="K154">
-        <v>1</v>
+        <v>483</v>
+      </c>
+      <c r="L154" t="s">
+        <v>27</v>
       </c>
       <c r="M154" t="s">
         <v>70</v>
+      </c>
+      <c r="N154" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="str">
-        <f t="shared" ref="A155:A156" si="30">CONCATENATE(D155,".",F155)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotype_list</v>
+        <f t="shared" si="29"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.covariate_list</v>
       </c>
       <c r="B155" t="s">
         <v>31</v>
@@ -5538,7 +5538,7 @@
         <v>24</v>
       </c>
       <c r="F155" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="L155" t="s">
         <v>27</v>
@@ -5550,40 +5550,37 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="str">
-        <f t="shared" si="30"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.covariate_list</v>
-      </c>
-      <c r="B156" t="s">
-        <v>31</v>
-      </c>
-      <c r="C156" t="s">
-        <v>32</v>
-      </c>
-      <c r="D156" t="s">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="str">
+        <f>CONCATENATE(D157,".",F157)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
+      </c>
+      <c r="B157" t="s">
+        <v>450</v>
+      </c>
+      <c r="C157" t="s">
+        <v>156</v>
+      </c>
+      <c r="D157" t="s">
         <v>444</v>
       </c>
-      <c r="E156" t="s">
-        <v>24</v>
-      </c>
-      <c r="F156" t="s">
-        <v>484</v>
-      </c>
-      <c r="L156" t="s">
-        <v>27</v>
-      </c>
-      <c r="M156" t="s">
-        <v>70</v>
-      </c>
-      <c r="N156" t="s">
-        <v>26</v>
+      <c r="E157" t="s">
+        <v>28</v>
+      </c>
+      <c r="F157" t="s">
+        <v>446</v>
+      </c>
+      <c r="K157">
+        <v>1</v>
+      </c>
+      <c r="M157" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="str">
-        <f>CONCATENATE(D158,".",F158)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_expanded_snps</v>
+        <f t="shared" si="27"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
       </c>
       <c r="B158" t="s">
         <v>450</v>
@@ -5598,10 +5595,10 @@
         <v>28</v>
       </c>
       <c r="F158" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K158">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M158" t="s">
         <v>70</v>
@@ -5609,8 +5606,8 @@
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="str">
-        <f t="shared" si="28"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tag_ideogram</v>
+        <f>CONCATENATE(D159,".",F159)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
       </c>
       <c r="B159" t="s">
         <v>450</v>
@@ -5625,10 +5622,10 @@
         <v>28</v>
       </c>
       <c r="F159" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K159">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M159" t="s">
         <v>70</v>
@@ -5636,14 +5633,14 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="str">
-        <f>CONCATENATE(D160,".",F160)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_tags</v>
+        <f t="shared" si="27"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
       </c>
       <c r="B160" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C160" t="s">
-        <v>156</v>
+        <v>452</v>
       </c>
       <c r="D160" t="s">
         <v>444</v>
@@ -5652,10 +5649,10 @@
         <v>28</v>
       </c>
       <c r="F160" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K160">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M160" t="s">
         <v>70</v>
@@ -5663,8 +5660,8 @@
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="str">
-        <f t="shared" si="28"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_genomic_partitions</v>
+        <f t="shared" ref="A161:A162" si="30">CONCATENATE(D161,".",F161)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
       </c>
       <c r="B161" t="s">
         <v>451</v>
@@ -5679,10 +5676,10 @@
         <v>28</v>
       </c>
       <c r="F161" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="K161">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M161" t="s">
         <v>70</v>
@@ -5690,8 +5687,8 @@
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="str">
-        <f t="shared" ref="A162:A163" si="31">CONCATENATE(D162,".",F162)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_gene_mapping</v>
+        <f t="shared" si="30"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
       </c>
       <c r="B162" t="s">
         <v>451</v>
@@ -5706,10 +5703,10 @@
         <v>28</v>
       </c>
       <c r="F162" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K162">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M162" t="s">
         <v>70</v>
@@ -5717,8 +5714,8 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="str">
-        <f t="shared" si="31"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_lncRNA_mapping</v>
+        <f t="shared" ref="A163" si="31">CONCATENATE(D163,".",F163)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
       </c>
       <c r="B163" t="s">
         <v>451</v>
@@ -5733,10 +5730,10 @@
         <v>28</v>
       </c>
       <c r="F163" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="K163">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M163" t="s">
         <v>70</v>
@@ -5744,14 +5741,14 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="str">
-        <f t="shared" ref="A164" si="32">CONCATENATE(D164,".",F164)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_list_mRNA_mapping</v>
+        <f t="shared" ref="A164:A165" si="32">CONCATENATE(D164,".",F164)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
       </c>
       <c r="B164" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C164" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D164" t="s">
         <v>444</v>
@@ -5760,7 +5757,7 @@
         <v>28</v>
       </c>
       <c r="F164" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="K164">
         <v>2</v>
@@ -5771,8 +5768,8 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="str">
-        <f t="shared" ref="A165:A166" si="33">CONCATENATE(D165,".",F165)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+        <f t="shared" si="32"/>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
       </c>
       <c r="B165" t="s">
         <v>453</v>
@@ -5787,10 +5784,10 @@
         <v>28</v>
       </c>
       <c r="F165" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="K165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M165" t="s">
         <v>70</v>
@@ -5798,14 +5795,14 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="str">
-        <f t="shared" si="33"/>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
+        <f>CONCATENATE(D166,".",F166)</f>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
       </c>
       <c r="B166" t="s">
-        <v>453</v>
+        <v>57</v>
       </c>
       <c r="C166" t="s">
-        <v>454</v>
+        <v>69</v>
       </c>
       <c r="D166" t="s">
         <v>444</v>
@@ -5814,25 +5811,25 @@
         <v>28</v>
       </c>
       <c r="F166" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K166">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M166" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="str">
         <f>CONCATENATE(D167,".",F167)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.top_variants</v>
+        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
       </c>
       <c r="B167" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C167" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D167" t="s">
         <v>444</v>
@@ -5841,43 +5838,46 @@
         <v>28</v>
       </c>
       <c r="F167" t="s">
-        <v>458</v>
-      </c>
-      <c r="K167">
-        <v>2</v>
+        <v>461</v>
       </c>
       <c r="M167" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A168" s="2" t="str">
-        <f>CONCATENATE(D168,".",F168)</f>
-        <v>DatasetRecordClasses.GWASDatasetRecordClass.phenotypes</v>
-      </c>
-      <c r="B168" t="s">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="str">
+        <f>CONCATENATE(D171,".",F171)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
+      </c>
+      <c r="B171" t="s">
         <v>31</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C171" t="s">
         <v>32</v>
       </c>
-      <c r="D168" t="s">
-        <v>444</v>
-      </c>
-      <c r="E168" t="s">
-        <v>28</v>
-      </c>
-      <c r="F168" t="s">
-        <v>461</v>
-      </c>
-      <c r="M168" t="s">
-        <v>25</v>
+      <c r="D171" t="s">
+        <v>462</v>
+      </c>
+      <c r="E171" t="s">
+        <v>24</v>
+      </c>
+      <c r="F171" t="s">
+        <v>3</v>
+      </c>
+      <c r="L171" t="s">
+        <v>464</v>
+      </c>
+      <c r="M171" t="s">
+        <v>70</v>
+      </c>
+      <c r="N171" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="str">
-        <f>CONCATENATE(D172,".",F172)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
+        <f t="shared" ref="A172:A175" si="33">CONCATENATE(D172,".",F172)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
       </c>
       <c r="B172" t="s">
         <v>31</v>
@@ -5892,7 +5892,7 @@
         <v>24</v>
       </c>
       <c r="F172" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L172" t="s">
         <v>464</v>
@@ -5906,8 +5906,8 @@
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="str">
-        <f t="shared" ref="A173:A176" si="34">CONCATENATE(D173,".",F173)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
+        <f t="shared" si="33"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
       </c>
       <c r="B173" t="s">
         <v>31</v>
@@ -5922,7 +5922,7 @@
         <v>24</v>
       </c>
       <c r="F173" t="s">
-        <v>6</v>
+        <v>463</v>
       </c>
       <c r="L173" t="s">
         <v>464</v>
@@ -5936,8 +5936,8 @@
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="str">
-        <f t="shared" si="34"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
+        <f t="shared" si="33"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
       </c>
       <c r="B174" t="s">
         <v>31</v>
@@ -5952,7 +5952,7 @@
         <v>24</v>
       </c>
       <c r="F174" t="s">
-        <v>463</v>
+        <v>431</v>
       </c>
       <c r="L174" t="s">
         <v>464</v>
@@ -5966,8 +5966,8 @@
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="str">
-        <f t="shared" si="34"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+        <f t="shared" si="33"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
       </c>
       <c r="B175" t="s">
         <v>31</v>
@@ -5979,45 +5979,15 @@
         <v>462</v>
       </c>
       <c r="E175" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F175" t="s">
-        <v>431</v>
+        <v>305</v>
       </c>
       <c r="L175" t="s">
         <v>464</v>
       </c>
       <c r="M175" t="s">
-        <v>70</v>
-      </c>
-      <c r="N175" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="str">
-        <f t="shared" si="34"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
-      </c>
-      <c r="B176" t="s">
-        <v>31</v>
-      </c>
-      <c r="C176" t="s">
-        <v>32</v>
-      </c>
-      <c r="D176" t="s">
-        <v>462</v>
-      </c>
-      <c r="E176" t="s">
-        <v>28</v>
-      </c>
-      <c r="F176" t="s">
-        <v>305</v>
-      </c>
-      <c r="L176" t="s">
-        <v>464</v>
-      </c>
-      <c r="M176" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
genome browser in progress
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\GenomicsDBWebsite\Model\lib\wdk\ontology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenem\DOCUME~1\MobaXterm\slash\RemoteFiles\394476_4_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C00EE4-854C-4945-B565-A00C07C56393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8C6199-188B-4406-8D0E-2AD422D175DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">entity_data_mapping!$A$1:$A$104</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">individuals!$A$1:$N$175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">individuals!$A$1:$N$176</definedName>
     <definedName name="individuals_1" localSheetId="0">individuals!$A$1:$N$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="498">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1559,6 +1559,9 @@
   </si>
   <si>
     <t>terms</t>
+  </si>
+  <si>
+    <t>related_tracks</t>
   </si>
 </sst>
 </file>
@@ -1897,13 +1900,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N180"/>
+  <dimension ref="A1:N181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D161" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K152" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F180" sqref="F180"/>
+      <selection pane="bottomRight" activeCell="N157" sqref="N157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5414,7 +5417,7 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="str">
-        <f t="shared" ref="A151:A160" si="27">CONCATENATE(D151,".",F151)</f>
+        <f t="shared" ref="A151:A161" si="27">CONCATENATE(D151,".",F151)</f>
         <v>TrackRecordClasses.TrackRecordClass.search_link</v>
       </c>
       <c r="B151" t="s">
@@ -5498,7 +5501,7 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="str">
-        <f t="shared" ref="A154:A155" si="29">CONCATENATE(D154,".",F154)</f>
+        <f t="shared" ref="A154:A156" si="29">CONCATENATE(D154,".",F154)</f>
         <v>TrackRecordClasses.TrackRecordClass.phenotype_list</v>
       </c>
       <c r="B154" t="s">
@@ -5556,65 +5559,65 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="str">
-        <f>CONCATENATE(D157,".",F157)</f>
-        <v>TrackRecordClasses.TrackRecordClass.inferno_expanded_snps</v>
-      </c>
-      <c r="B157" t="s">
-        <v>449</v>
-      </c>
-      <c r="C157" t="s">
-        <v>156</v>
-      </c>
-      <c r="D157" t="s">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>TrackRecordClasses.TrackRecordClass.related_tracks</v>
+      </c>
+      <c r="B156" t="s">
+        <v>31</v>
+      </c>
+      <c r="C156" t="s">
+        <v>32</v>
+      </c>
+      <c r="D156" t="s">
         <v>494</v>
       </c>
-      <c r="E157" t="s">
-        <v>28</v>
-      </c>
-      <c r="F157" t="s">
-        <v>445</v>
-      </c>
-      <c r="K157">
-        <v>1</v>
-      </c>
-      <c r="M157" t="s">
-        <v>70</v>
+      <c r="E156" t="s">
+        <v>24</v>
+      </c>
+      <c r="F156" t="s">
+        <v>497</v>
+      </c>
+      <c r="M156" t="s">
+        <v>70</v>
+      </c>
+      <c r="N156" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="str">
+        <f>CONCATENATE(D158,".",F158)</f>
+        <v>TrackRecordClasses.TrackRecordClass.inferno_expanded_snps</v>
+      </c>
+      <c r="B158" t="s">
+        <v>449</v>
+      </c>
+      <c r="C158" t="s">
+        <v>156</v>
+      </c>
+      <c r="D158" t="s">
+        <v>494</v>
+      </c>
+      <c r="E158" t="s">
+        <v>28</v>
+      </c>
+      <c r="F158" t="s">
+        <v>445</v>
+      </c>
+      <c r="K158">
+        <v>1</v>
+      </c>
+      <c r="M158" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="str">
         <f t="shared" si="27"/>
         <v>TrackRecordClasses.TrackRecordClass.inferno_tag_ideogram</v>
       </c>
-      <c r="B158" t="s">
-        <v>449</v>
-      </c>
-      <c r="C158" t="s">
-        <v>156</v>
-      </c>
-      <c r="D158" t="s">
-        <v>494</v>
-      </c>
-      <c r="E158" t="s">
-        <v>28</v>
-      </c>
-      <c r="F158" t="s">
-        <v>448</v>
-      </c>
-      <c r="K158">
-        <v>2</v>
-      </c>
-      <c r="M158" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="str">
-        <f>CONCATENATE(D159,".",F159)</f>
-        <v>TrackRecordClasses.TrackRecordClass.inferno_tags</v>
-      </c>
       <c r="B159" t="s">
         <v>449</v>
       </c>
@@ -5628,10 +5631,10 @@
         <v>28</v>
       </c>
       <c r="F159" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="K159">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M159" t="s">
         <v>70</v>
@@ -5639,36 +5642,36 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="str">
+        <f>CONCATENATE(D160,".",F160)</f>
+        <v>TrackRecordClasses.TrackRecordClass.inferno_tags</v>
+      </c>
+      <c r="B160" t="s">
+        <v>449</v>
+      </c>
+      <c r="C160" t="s">
+        <v>156</v>
+      </c>
+      <c r="D160" t="s">
+        <v>494</v>
+      </c>
+      <c r="E160" t="s">
+        <v>28</v>
+      </c>
+      <c r="F160" t="s">
+        <v>447</v>
+      </c>
+      <c r="K160">
+        <v>3</v>
+      </c>
+      <c r="M160" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="str">
         <f t="shared" si="27"/>
         <v>TrackRecordClasses.TrackRecordClass.inferno_genomic_partitions</v>
       </c>
-      <c r="B160" t="s">
-        <v>450</v>
-      </c>
-      <c r="C160" t="s">
-        <v>451</v>
-      </c>
-      <c r="D160" t="s">
-        <v>494</v>
-      </c>
-      <c r="E160" t="s">
-        <v>28</v>
-      </c>
-      <c r="F160" t="s">
-        <v>446</v>
-      </c>
-      <c r="K160">
-        <v>1</v>
-      </c>
-      <c r="M160" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="str">
-        <f t="shared" ref="A161:A162" si="30">CONCATENATE(D161,".",F161)</f>
-        <v>TrackRecordClasses.TrackRecordClass.inferno_highchart_gene_mapping</v>
-      </c>
       <c r="B161" t="s">
         <v>450</v>
       </c>
@@ -5682,10 +5685,10 @@
         <v>28</v>
       </c>
       <c r="F161" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="K161">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M161" t="s">
         <v>70</v>
@@ -5693,36 +5696,36 @@
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="str">
+        <f t="shared" ref="A162:A163" si="30">CONCATENATE(D162,".",F162)</f>
+        <v>TrackRecordClasses.TrackRecordClass.inferno_highchart_gene_mapping</v>
+      </c>
+      <c r="B162" t="s">
+        <v>450</v>
+      </c>
+      <c r="C162" t="s">
+        <v>451</v>
+      </c>
+      <c r="D162" t="s">
+        <v>494</v>
+      </c>
+      <c r="E162" t="s">
+        <v>28</v>
+      </c>
+      <c r="F162" t="s">
+        <v>454</v>
+      </c>
+      <c r="K162">
+        <v>3</v>
+      </c>
+      <c r="M162" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="str">
         <f t="shared" si="30"/>
         <v>TrackRecordClasses.TrackRecordClass.inferno_highchart_list_lncRNA_mapping</v>
       </c>
-      <c r="B162" t="s">
-        <v>450</v>
-      </c>
-      <c r="C162" t="s">
-        <v>451</v>
-      </c>
-      <c r="D162" t="s">
-        <v>494</v>
-      </c>
-      <c r="E162" t="s">
-        <v>28</v>
-      </c>
-      <c r="F162" t="s">
-        <v>455</v>
-      </c>
-      <c r="K162">
-        <v>4</v>
-      </c>
-      <c r="M162" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="str">
-        <f t="shared" ref="A163" si="31">CONCATENATE(D163,".",F163)</f>
-        <v>TrackRecordClasses.TrackRecordClass.inferno_highchart_list_mRNA_mapping</v>
-      </c>
       <c r="B163" t="s">
         <v>450</v>
       </c>
@@ -5736,10 +5739,10 @@
         <v>28</v>
       </c>
       <c r="F163" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K163">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M163" t="s">
         <v>70</v>
@@ -5747,14 +5750,14 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="str">
-        <f t="shared" ref="A164:A165" si="32">CONCATENATE(D164,".",F164)</f>
-        <v>TrackRecordClasses.TrackRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+        <f t="shared" ref="A164" si="31">CONCATENATE(D164,".",F164)</f>
+        <v>TrackRecordClasses.TrackRecordClass.inferno_highchart_list_mRNA_mapping</v>
       </c>
       <c r="B164" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C164" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D164" t="s">
         <v>494</v>
@@ -5763,7 +5766,7 @@
         <v>28</v>
       </c>
       <c r="F164" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K164">
         <v>2</v>
@@ -5774,41 +5777,41 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="str">
+        <f t="shared" ref="A165:A166" si="32">CONCATENATE(D165,".",F165)</f>
+        <v>TrackRecordClasses.TrackRecordClass.inferno_highchart_enhancer_overlap_roadmap</v>
+      </c>
+      <c r="B165" t="s">
+        <v>452</v>
+      </c>
+      <c r="C165" t="s">
+        <v>453</v>
+      </c>
+      <c r="D165" t="s">
+        <v>494</v>
+      </c>
+      <c r="E165" t="s">
+        <v>28</v>
+      </c>
+      <c r="F165" t="s">
+        <v>458</v>
+      </c>
+      <c r="K165">
+        <v>2</v>
+      </c>
+      <c r="M165" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="str">
         <f t="shared" si="32"/>
         <v>TrackRecordClasses.TrackRecordClass.inferno_highchart_enhancer_overlap_fantom5</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B166" t="s">
         <v>452</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C166" t="s">
         <v>453</v>
-      </c>
-      <c r="D165" t="s">
-        <v>494</v>
-      </c>
-      <c r="E165" t="s">
-        <v>28</v>
-      </c>
-      <c r="F165" t="s">
-        <v>459</v>
-      </c>
-      <c r="K165">
-        <v>1</v>
-      </c>
-      <c r="M165" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="str">
-        <f>CONCATENATE(D166,".",F166)</f>
-        <v>TrackRecordClasses.TrackRecordClass.top_variants</v>
-      </c>
-      <c r="B166" t="s">
-        <v>57</v>
-      </c>
-      <c r="C166" t="s">
-        <v>69</v>
       </c>
       <c r="D166" t="s">
         <v>494</v>
@@ -5817,25 +5820,25 @@
         <v>28</v>
       </c>
       <c r="F166" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="K166">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M166" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="str">
         <f>CONCATENATE(D167,".",F167)</f>
-        <v>TrackRecordClasses.TrackRecordClass.phenotypes</v>
+        <v>TrackRecordClasses.TrackRecordClass.top_variants</v>
       </c>
       <c r="B167" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C167" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D167" t="s">
         <v>494</v>
@@ -5844,46 +5847,43 @@
         <v>28</v>
       </c>
       <c r="F167" t="s">
-        <v>460</v>
+        <v>457</v>
+      </c>
+      <c r="K167">
+        <v>2</v>
       </c>
       <c r="M167" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="str">
-        <f>CONCATENATE(D171,".",F171)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
-      </c>
-      <c r="B171" t="s">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="str">
+        <f>CONCATENATE(D168,".",F168)</f>
+        <v>TrackRecordClasses.TrackRecordClass.phenotypes</v>
+      </c>
+      <c r="B168" t="s">
         <v>31</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C168" t="s">
         <v>32</v>
       </c>
-      <c r="D171" t="s">
-        <v>461</v>
-      </c>
-      <c r="E171" t="s">
-        <v>24</v>
-      </c>
-      <c r="F171" t="s">
-        <v>3</v>
-      </c>
-      <c r="L171" t="s">
-        <v>463</v>
-      </c>
-      <c r="M171" t="s">
-        <v>70</v>
-      </c>
-      <c r="N171" t="s">
-        <v>26</v>
+      <c r="D168" t="s">
+        <v>494</v>
+      </c>
+      <c r="E168" t="s">
+        <v>28</v>
+      </c>
+      <c r="F168" t="s">
+        <v>460</v>
+      </c>
+      <c r="M168" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="str">
-        <f t="shared" ref="A172:A180" si="33">CONCATENATE(D172,".",F172)</f>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
+        <f>CONCATENATE(D172,".",F172)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.name</v>
       </c>
       <c r="B172" t="s">
         <v>31</v>
@@ -5898,7 +5898,7 @@
         <v>24</v>
       </c>
       <c r="F172" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L172" t="s">
         <v>463</v>
@@ -5912,8 +5912,8 @@
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="str">
-        <f t="shared" si="33"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
+        <f t="shared" ref="A173:A181" si="33">CONCATENATE(D173,".",F173)</f>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.description</v>
       </c>
       <c r="B173" t="s">
         <v>31</v>
@@ -5928,7 +5928,7 @@
         <v>24</v>
       </c>
       <c r="F173" t="s">
-        <v>462</v>
+        <v>6</v>
       </c>
       <c r="L173" t="s">
         <v>463</v>
@@ -5943,7 +5943,7 @@
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="str">
         <f t="shared" si="33"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.external_link</v>
       </c>
       <c r="B174" t="s">
         <v>31</v>
@@ -5958,7 +5958,7 @@
         <v>24</v>
       </c>
       <c r="F174" t="s">
-        <v>431</v>
+        <v>462</v>
       </c>
       <c r="L174" t="s">
         <v>463</v>
@@ -5973,7 +5973,7 @@
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="str">
         <f t="shared" si="33"/>
-        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.is_adsp</v>
       </c>
       <c r="B175" t="s">
         <v>31</v>
@@ -5985,49 +5985,52 @@
         <v>461</v>
       </c>
       <c r="E175" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F175" t="s">
-        <v>305</v>
+        <v>431</v>
       </c>
       <c r="L175" t="s">
         <v>463</v>
       </c>
       <c r="M175" t="s">
+        <v>70</v>
+      </c>
+      <c r="N175" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="str">
+        <f t="shared" si="33"/>
+        <v>DatasetRecordClasses.NIAGADSDatasetRecordClass.datasets</v>
+      </c>
+      <c r="B176" t="s">
+        <v>31</v>
+      </c>
+      <c r="C176" t="s">
+        <v>32</v>
+      </c>
+      <c r="D176" t="s">
+        <v>461</v>
+      </c>
+      <c r="E176" t="s">
+        <v>28</v>
+      </c>
+      <c r="F176" t="s">
+        <v>305</v>
+      </c>
+      <c r="L176" t="s">
+        <v>463</v>
+      </c>
+      <c r="M176" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="str">
-        <f t="shared" si="33"/>
-        <v>OntologyRecordClasses.OntologyRecordClass.name</v>
-      </c>
-      <c r="B177" t="s">
-        <v>31</v>
-      </c>
-      <c r="C177" t="s">
-        <v>32</v>
-      </c>
-      <c r="D177" t="s">
-        <v>495</v>
-      </c>
-      <c r="E177" t="s">
-        <v>24</v>
-      </c>
-      <c r="F177" t="s">
-        <v>3</v>
-      </c>
-      <c r="M177" t="s">
-        <v>70</v>
-      </c>
-      <c r="N177" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="str">
         <f t="shared" si="33"/>
-        <v>OntologyRecordClasses.OntologyRecordClass.description</v>
+        <v>OntologyRecordClasses.OntologyRecordClass.name</v>
       </c>
       <c r="B178" t="s">
         <v>31</v>
@@ -6042,7 +6045,7 @@
         <v>24</v>
       </c>
       <c r="F178" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M178" t="s">
         <v>70</v>
@@ -6054,7 +6057,7 @@
     <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="str">
         <f t="shared" si="33"/>
-        <v>OntologyRecordClasses.OntologyRecordClass.ontology</v>
+        <v>OntologyRecordClasses.OntologyRecordClass.description</v>
       </c>
       <c r="B179" t="s">
         <v>31</v>
@@ -6069,7 +6072,7 @@
         <v>24</v>
       </c>
       <c r="F179" t="s">
-        <v>489</v>
+        <v>6</v>
       </c>
       <c r="M179" t="s">
         <v>70</v>
@@ -6081,7 +6084,7 @@
     <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="str">
         <f t="shared" si="33"/>
-        <v>OntologyRecordClasses.OntologyRecordClass.terms</v>
+        <v>OntologyRecordClasses.OntologyRecordClass.ontology</v>
       </c>
       <c r="B180" t="s">
         <v>31</v>
@@ -6093,15 +6096,42 @@
         <v>495</v>
       </c>
       <c r="E180" t="s">
+        <v>24</v>
+      </c>
+      <c r="F180" t="s">
+        <v>489</v>
+      </c>
+      <c r="M180" t="s">
+        <v>70</v>
+      </c>
+      <c r="N180" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="str">
+        <f t="shared" si="33"/>
+        <v>OntologyRecordClasses.OntologyRecordClass.terms</v>
+      </c>
+      <c r="B181" t="s">
+        <v>31</v>
+      </c>
+      <c r="C181" t="s">
+        <v>32</v>
+      </c>
+      <c r="D181" t="s">
+        <v>495</v>
+      </c>
+      <c r="E181" t="s">
         <v>28</v>
       </c>
-      <c r="F180" t="s">
+      <c r="F181" t="s">
         <v>496</v>
       </c>
-      <c r="M180" t="s">
+      <c r="M181" t="s">
         <v>25</v>
       </c>
-      <c r="N180" t="s">
+      <c r="N181" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
top variants to download
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\GenomicsDBWebsite\Model\lib\wdk\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA6A54D-F730-4AC2-8F88-8CC5B046D87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB2CC782-1EF8-4A38-96F6-9C5392A3D99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-195" yWindow="-195" windowWidth="29190" windowHeight="17670" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals-old" sheetId="6" r:id="rId1"/>
@@ -6357,10 +6357,10 @@
   <dimension ref="A1:N180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="N165" sqref="N165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13676,7 +13676,7 @@
         <v>25</v>
       </c>
       <c r="N166" t="s">
-        <v>121</v>
+        <v>26</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>